<commit_message>
Fix Content Security Policy Error - VSF Project
</commit_message>
<xml_diff>
--- a/me/13.Year-2021-Updates.xlsx
+++ b/me/13.Year-2021-Updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\LightningWebComponent\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52D1C00-356E-4CDB-B417-769DB3088929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E8152A-4A90-4A4E-BE15-404A1A4B25D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets in Javascript" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="316">
   <si>
     <t>構成</t>
   </si>
@@ -1047,6 +1047,21 @@
   </si>
   <si>
     <t xml:space="preserve">This is an error that we are most likely to get when we are going to make call out from our javascript code </t>
+  </si>
+  <si>
+    <t>Resolve error</t>
+  </si>
+  <si>
+    <t>3.VSF-Project</t>
+  </si>
+  <si>
+    <t>cowin-api-sample-response</t>
+  </si>
+  <si>
+    <t>db.json</t>
+  </si>
+  <si>
+    <t>backup</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1188,8 +1203,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1411,13 +1424,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>207</xdr:row>
+      <xdr:row>210</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>209</xdr:row>
+      <xdr:row>212</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1464,13 +1477,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>221</xdr:row>
+      <xdr:row>224</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>228</xdr:row>
+      <xdr:row>231</xdr:row>
       <xdr:rowOff>102961</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1508,6 +1521,241 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85164</xdr:colOff>
+      <xdr:row>235</xdr:row>
+      <xdr:rowOff>125506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>268941</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>45555</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D59383C2-4AF3-B2E1-47A2-58B06C0DDC4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="690282" y="44131006"/>
+          <a:ext cx="11075894" cy="4492049"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>290</xdr:row>
+      <xdr:rowOff>51649</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81D8F2EC-A775-395A-A0C5-195283C81198}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="694765" y="49081765"/>
+          <a:ext cx="11172264" cy="5643384"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>291</xdr:row>
+      <xdr:rowOff>100854</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>448236</xdr:colOff>
+      <xdr:row>320</xdr:row>
+      <xdr:rowOff>113668</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6092E73F-8A34-54E4-6787-B71B41CB3430}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="739588" y="54964854"/>
+          <a:ext cx="11205883" cy="5537314"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>156882</xdr:colOff>
+      <xdr:row>321</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>336177</xdr:colOff>
+      <xdr:row>351</xdr:row>
+      <xdr:rowOff>53634</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09CF0D35-1379-D7DE-F7F8-65140431E458}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="60747088"/>
+          <a:ext cx="11071412" cy="5600546"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>168088</xdr:colOff>
+      <xdr:row>227</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>246529</xdr:colOff>
+      <xdr:row>234</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C4C7899-C329-A154-B39C-FFD5FE71F266}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="168088" y="42772853"/>
+          <a:ext cx="683559" cy="1255059"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6707,10 +6955,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67357BF7-6643-493F-B16E-6641B4CEB2D9}">
-  <dimension ref="A2:N221"/>
+  <dimension ref="A2:N235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
-      <selection activeCell="Q213" sqref="Q213"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P189" sqref="P189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7799,16 +8047,14 @@
     </row>
     <row r="158" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B158" s="5"/>
-      <c r="G158" s="12" t="s">
+      <c r="G158" t="s">
         <v>230</v>
       </c>
-      <c r="H158" s="12"/>
       <c r="L158" s="6"/>
     </row>
     <row r="159" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B159" s="5"/>
-      <c r="G159" s="12"/>
-      <c r="H159" s="12" t="s">
+      <c r="H159" t="s">
         <v>231</v>
       </c>
       <c r="L159" s="6"/>
@@ -7828,7 +8074,7 @@
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B161" s="5"/>
-      <c r="H161" s="12" t="s">
+      <c r="H161" t="s">
         <v>233</v>
       </c>
       <c r="L161" s="6"/>
@@ -8050,334 +8296,214 @@
       </c>
       <c r="L192" s="6"/>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B193" s="8"/>
-      <c r="C193" s="9"/>
-      <c r="D193" s="9"/>
-      <c r="E193" s="9"/>
-      <c r="F193" s="9"/>
-      <c r="G193" s="9"/>
-      <c r="H193" s="9"/>
-      <c r="I193" s="9"/>
-      <c r="J193" s="9"/>
-      <c r="K193" s="9"/>
-      <c r="L193" s="10"/>
-    </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B193" s="5"/>
+      <c r="D193" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="L193" s="6"/>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B194" s="5"/>
+      <c r="E194" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="L194" s="6"/>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B195" s="5"/>
+      <c r="F195" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="L195" s="6"/>
+      <c r="M195" t="s">
+        <v>181</v>
+      </c>
+      <c r="N195" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B196" s="8"/>
+      <c r="C196" s="9"/>
+      <c r="D196" s="9"/>
+      <c r="E196" s="9"/>
+      <c r="F196" s="9"/>
+      <c r="G196" s="9"/>
+      <c r="H196" s="9"/>
+      <c r="I196" s="9"/>
+      <c r="J196" s="9"/>
+      <c r="K196" s="9"/>
+      <c r="L196" s="10"/>
+    </row>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B197" s="2" t="s">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B200" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C197" s="3"/>
-      <c r="D197" s="3"/>
-      <c r="E197" s="3"/>
-      <c r="F197" s="3"/>
-      <c r="G197" s="3"/>
-      <c r="H197" s="3"/>
-      <c r="I197" s="3"/>
-      <c r="J197" s="3"/>
-      <c r="K197" s="4"/>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B198" s="5"/>
-      <c r="C198" s="13"/>
-      <c r="D198" s="13"/>
-      <c r="E198" s="13"/>
-      <c r="F198" s="13"/>
-      <c r="G198" s="13"/>
-      <c r="H198" s="13"/>
-      <c r="I198" s="13"/>
-      <c r="J198" s="13"/>
-      <c r="K198" s="6"/>
-    </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B199" s="5" t="s">
+      <c r="C200" s="3"/>
+      <c r="D200" s="3"/>
+      <c r="E200" s="3"/>
+      <c r="F200" s="3"/>
+      <c r="G200" s="3"/>
+      <c r="H200" s="3"/>
+      <c r="I200" s="3"/>
+      <c r="J200" s="3"/>
+      <c r="K200" s="4"/>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B201" s="5"/>
+      <c r="K201" s="6"/>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B202" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C199" s="13"/>
-      <c r="D199" s="13"/>
-      <c r="E199" s="13"/>
-      <c r="F199" s="13"/>
-      <c r="G199" s="13"/>
-      <c r="H199" s="13"/>
-      <c r="I199" s="13"/>
-      <c r="J199" s="13"/>
-      <c r="K199" s="6"/>
-    </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B200" s="5" t="s">
+      <c r="K202" s="6"/>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B203" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="C200" s="13"/>
-      <c r="D200" s="13"/>
-      <c r="E200" s="13"/>
-      <c r="F200" s="13"/>
-      <c r="G200" s="13"/>
-      <c r="H200" s="13"/>
-      <c r="I200" s="13"/>
-      <c r="J200" s="13"/>
-      <c r="K200" s="6"/>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B201" s="5" t="s">
+      <c r="K203" s="6"/>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B204" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="C201" s="13"/>
-      <c r="D201" s="13"/>
-      <c r="E201" s="13"/>
-      <c r="F201" s="13"/>
-      <c r="G201" s="13"/>
-      <c r="H201" s="13"/>
-      <c r="I201" s="13"/>
-      <c r="J201" s="13"/>
-      <c r="K201" s="6"/>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B202" s="5"/>
-      <c r="C202" s="13"/>
-      <c r="D202" s="13"/>
-      <c r="E202" s="13"/>
-      <c r="F202" s="13"/>
-      <c r="G202" s="13"/>
-      <c r="H202" s="13"/>
-      <c r="I202" s="13"/>
-      <c r="J202" s="13"/>
-      <c r="K202" s="6"/>
-    </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B203" s="11" t="s">
+      <c r="K204" s="6"/>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B205" s="5"/>
+      <c r="K205" s="6"/>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B206" s="11" t="s">
         <v>299</v>
       </c>
-      <c r="C203" s="13"/>
-      <c r="D203" s="13"/>
-      <c r="E203" s="13"/>
-      <c r="F203" s="13"/>
-      <c r="G203" s="13"/>
-      <c r="H203" s="13"/>
-      <c r="I203" s="13"/>
-      <c r="J203" s="13"/>
-      <c r="K203" s="6"/>
-      <c r="L203" t="s">
+      <c r="K206" s="6"/>
+      <c r="L206" t="s">
         <v>181</v>
       </c>
-      <c r="M203" t="s">
+      <c r="M206" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B204" s="11" t="s">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B207" s="11" t="s">
         <v>300</v>
       </c>
-      <c r="C204" s="13"/>
-      <c r="D204" s="13"/>
-      <c r="E204" s="13"/>
-      <c r="F204" s="13"/>
-      <c r="G204" s="13"/>
-      <c r="H204" s="13"/>
-      <c r="I204" s="13"/>
-      <c r="J204" s="13"/>
-      <c r="K204" s="6"/>
-    </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B205" s="11" t="s">
+      <c r="K207" s="6"/>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B208" s="11" t="s">
         <v>301</v>
       </c>
-      <c r="C205" s="13"/>
-      <c r="D205" s="13"/>
-      <c r="E205" s="13"/>
-      <c r="F205" s="13"/>
-      <c r="G205" s="13"/>
-      <c r="H205" s="13"/>
-      <c r="I205" s="13"/>
-      <c r="J205" s="13"/>
-      <c r="K205" s="6"/>
-    </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B206" s="11" t="s">
-        <v>302</v>
-      </c>
-      <c r="C206" s="13"/>
-      <c r="D206" s="13"/>
-      <c r="E206" s="13"/>
-      <c r="F206" s="13"/>
-      <c r="G206" s="13"/>
-      <c r="H206" s="13"/>
-      <c r="I206" s="13"/>
-      <c r="J206" s="13"/>
-      <c r="K206" s="6"/>
-    </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B207" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="C207" s="13"/>
-      <c r="D207" s="13"/>
-      <c r="E207" s="13"/>
-      <c r="F207" s="13"/>
-      <c r="G207" s="13"/>
-      <c r="H207" s="13"/>
-      <c r="I207" s="13"/>
-      <c r="J207" s="13"/>
-      <c r="K207" s="6"/>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B208" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="C208" s="13"/>
-      <c r="D208" s="13"/>
-      <c r="E208" s="13"/>
-      <c r="F208" s="13"/>
-      <c r="G208" s="13"/>
-      <c r="H208" s="13"/>
-      <c r="I208" s="13"/>
-      <c r="J208" s="13"/>
       <c r="K208" s="6"/>
     </row>
     <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B209" s="11" t="s">
-        <v>304</v>
-      </c>
-      <c r="C209" s="13"/>
-      <c r="D209" s="13"/>
-      <c r="E209" s="13"/>
-      <c r="F209" s="13"/>
-      <c r="G209" s="13"/>
-      <c r="H209" s="13"/>
-      <c r="I209" s="13"/>
-      <c r="J209" s="13"/>
+        <v>302</v>
+      </c>
       <c r="K209" s="6"/>
-      <c r="L209" t="s">
-        <v>181</v>
-      </c>
-      <c r="M209" t="s">
-        <v>308</v>
-      </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B210" s="11" t="s">
-        <v>305</v>
-      </c>
-      <c r="C210" s="13"/>
-      <c r="D210" s="13"/>
-      <c r="E210" s="13"/>
-      <c r="F210" s="13"/>
-      <c r="G210" s="13"/>
-      <c r="H210" s="13"/>
-      <c r="I210" s="13"/>
-      <c r="J210" s="13"/>
+        <v>205</v>
+      </c>
       <c r="K210" s="6"/>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B211" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="C211" s="13"/>
-      <c r="D211" s="13"/>
-      <c r="E211" s="13"/>
-      <c r="F211" s="13"/>
-      <c r="G211" s="13"/>
-      <c r="H211" s="13"/>
-      <c r="I211" s="13"/>
-      <c r="J211" s="13"/>
+        <v>303</v>
+      </c>
       <c r="K211" s="6"/>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B212" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="K212" s="6"/>
+      <c r="L212" t="s">
+        <v>181</v>
+      </c>
+      <c r="M212" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B213" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="K213" s="6"/>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B214" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="K214" s="6"/>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B215" s="11" t="s">
         <v>302</v>
       </c>
-      <c r="C212" s="13"/>
-      <c r="D212" s="13"/>
-      <c r="E212" s="13"/>
-      <c r="F212" s="13"/>
-      <c r="G212" s="13"/>
-      <c r="H212" s="13"/>
-      <c r="I212" s="13"/>
-      <c r="J212" s="13"/>
-      <c r="K212" s="6"/>
-    </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B213" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="C213" s="13"/>
-      <c r="D213" s="13"/>
-      <c r="E213" s="13"/>
-      <c r="F213" s="13"/>
-      <c r="G213" s="13"/>
-      <c r="H213" s="13"/>
-      <c r="I213" s="13"/>
-      <c r="J213" s="13"/>
-      <c r="K213" s="6"/>
-    </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B214" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="C214" s="13"/>
-      <c r="D214" s="13"/>
-      <c r="E214" s="13"/>
-      <c r="F214" s="13"/>
-      <c r="G214" s="13"/>
-      <c r="H214" s="13"/>
-      <c r="I214" s="13"/>
-      <c r="J214" s="13"/>
-      <c r="K214" s="6"/>
-    </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B215" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="C215" s="13"/>
-      <c r="D215" s="13"/>
-      <c r="E215" s="13"/>
-      <c r="F215" s="13"/>
-      <c r="G215" s="13"/>
-      <c r="H215" s="13"/>
-      <c r="I215" s="13"/>
-      <c r="J215" s="13"/>
       <c r="K215" s="6"/>
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B216" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="K216" s="6"/>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B217" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="K217" s="6"/>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B218" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="K218" s="6"/>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B219" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="C216" s="13"/>
-      <c r="D216" s="13"/>
-      <c r="E216" s="13"/>
-      <c r="F216" s="13"/>
-      <c r="G216" s="13"/>
-      <c r="H216" s="13"/>
-      <c r="I216" s="13"/>
-      <c r="J216" s="13"/>
-      <c r="K216" s="6"/>
-    </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B217" s="8" t="s">
+      <c r="K219" s="6"/>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B220" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="C217" s="9"/>
-      <c r="D217" s="9"/>
-      <c r="E217" s="9"/>
-      <c r="F217" s="9"/>
-      <c r="G217" s="9"/>
-      <c r="H217" s="9"/>
-      <c r="I217" s="9"/>
-      <c r="J217" s="9"/>
-      <c r="K217" s="10"/>
-    </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A220" s="1" t="s">
+      <c r="C220" s="9"/>
+      <c r="D220" s="9"/>
+      <c r="E220" s="9"/>
+      <c r="F220" s="9"/>
+      <c r="G220" s="9"/>
+      <c r="H220" s="9"/>
+      <c r="I220" s="9"/>
+      <c r="J220" s="9"/>
+      <c r="K220" s="10"/>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B221" t="s">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
         <v>310</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stylise Lightning Datatable - VSF Project
</commit_message>
<xml_diff>
--- a/me/13.Year-2021-Updates.xlsx
+++ b/me/13.Year-2021-Updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\LightningWebComponent\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40A19BC-0F5C-47F2-B054-988F797C4D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08E7BDF-E171-4BF2-B309-A84947BEA755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets in Javascript" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Making a CalloutFromLWC-VSF Pj" sheetId="4" r:id="rId4"/>
     <sheet name="ParseAndFormatTheCalloutRespons" sheetId="5" r:id="rId5"/>
     <sheet name="FinishFormattingtheCalloutRespo" sheetId="6" r:id="rId6"/>
+    <sheet name="Stylise Lightning Datatable" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="423">
   <si>
     <t>構成</t>
   </si>
@@ -1472,6 +1473,97 @@
   </si>
   <si>
     <t>check exist to avoid overwriting, if centers repeats value we do not want to override</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can see our data gets truncated </t>
+  </si>
+  <si>
+    <t>Wrap text feture will not get truncated</t>
+  </si>
+  <si>
+    <t>Adding Styles to Columns</t>
+  </si>
+  <si>
+    <t>use custom class</t>
+  </si>
+  <si>
+    <t>            wrapText: true</t>
+  </si>
+  <si>
+    <t>                    wrapText: true,</t>
+  </si>
+  <si>
+    <t>                    cellAttributes: { class: { fieldName: "className" } }</t>
+  </si>
+  <si>
+    <t>                centers.get(center.center_id).className =</t>
+  </si>
+  <si>
+    <t>                available_capacity &gt; 0</t>
+  </si>
+  <si>
+    <t>                    ? "slds-text-color_success"</t>
+  </si>
+  <si>
+    <t>                    : "slds-text-color_error";</t>
+  </si>
+  <si>
+    <r>
+      <t>            type: "text"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                    type: "text"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>default enable wrapText so we can read the text if there is not enough it on the screen(small screen) to show the complete data</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">stylize date column by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> atribute with custom class</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1600,7 +1692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1617,6 +1709,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3012,15 +3105,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>261</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>285749</xdr:colOff>
-      <xdr:row>309</xdr:row>
-      <xdr:rowOff>54444</xdr:rowOff>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>310</xdr:row>
+      <xdr:rowOff>111594</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3048,8 +3141,360 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="742950" y="49796700"/>
+          <a:off x="733425" y="50044350"/>
           <a:ext cx="10515599" cy="9122244"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>313</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>437030</xdr:colOff>
+      <xdr:row>342</xdr:row>
+      <xdr:rowOff>91757</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C3E2762-0A6F-C669-1B03-7D19AB2891E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="709893" y="59693175"/>
+          <a:ext cx="11224372" cy="5549582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>156881</xdr:colOff>
+      <xdr:row>343</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>224117</xdr:colOff>
+      <xdr:row>372</xdr:row>
+      <xdr:rowOff>75389</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E75E4438-5A47-0B03-5FA8-E8B83FF2FED3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="761999" y="65397529"/>
+          <a:ext cx="10959353" cy="5543860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>229</xdr:row>
+      <xdr:rowOff>30598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEE8E04-A202-F64A-D7B2-A173B35D1A63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="717096" y="38176200"/>
+          <a:ext cx="11202761" cy="5478898"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{147D7FE6-AC2A-F155-149D-C8FEA4CEC593}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3724275" y="39719250"/>
+          <a:ext cx="895350" cy="2609850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>225</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ED773F6-7001-E287-8B46-F27AD169DB94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4476750" y="41138475"/>
+          <a:ext cx="971550" cy="1866900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>276</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>285</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95B46A49-A731-F0C9-17FD-C706F546CD1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2943225" y="52711350"/>
+          <a:ext cx="466725" cy="1647825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>302</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>187356</xdr:colOff>
+      <xdr:row>373</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C1C2BD6-ABC1-D557-2A3B-E3709ECA1013}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="57588150"/>
+          <a:ext cx="10445781" cy="13496926"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9844,8 +10289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EF4FE4-2F69-4CAB-9444-72D9ABAD5624}">
   <dimension ref="A3:AI343"/>
   <sheetViews>
-    <sheetView topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="M333" sqref="M333"/>
+    <sheetView topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="O195" sqref="O195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12086,10 +12531,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF1CE59-FA7B-4457-A932-43D4831F36CE}">
-  <dimension ref="A2:N261"/>
+  <dimension ref="A2:T373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="B262" sqref="B262"/>
+    <sheetView topLeftCell="A136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S199" sqref="S199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13851,6 +14296,3626 @@
         <v>296</v>
       </c>
     </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B262" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="313" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B313" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="C313" s="3"/>
+      <c r="D313" s="3"/>
+      <c r="E313" s="3"/>
+      <c r="F313" s="3"/>
+      <c r="G313" s="3"/>
+      <c r="H313" s="3"/>
+      <c r="I313" s="3"/>
+      <c r="J313" s="3"/>
+      <c r="K313" s="3"/>
+      <c r="L313" s="3"/>
+      <c r="M313" s="3"/>
+      <c r="N313" s="3"/>
+      <c r="O313" s="3"/>
+      <c r="P313" s="3"/>
+      <c r="Q313" s="3"/>
+      <c r="R313" s="3"/>
+      <c r="S313" s="3"/>
+      <c r="T313" s="4"/>
+    </row>
+    <row r="314" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B314" s="5"/>
+      <c r="C314" s="16"/>
+      <c r="D314" s="16"/>
+      <c r="E314" s="16"/>
+      <c r="F314" s="16"/>
+      <c r="G314" s="16"/>
+      <c r="H314" s="16"/>
+      <c r="I314" s="16"/>
+      <c r="J314" s="16"/>
+      <c r="K314" s="16"/>
+      <c r="L314" s="16"/>
+      <c r="M314" s="16"/>
+      <c r="N314" s="16"/>
+      <c r="O314" s="16"/>
+      <c r="P314" s="16"/>
+      <c r="Q314" s="16"/>
+      <c r="R314" s="16"/>
+      <c r="S314" s="16"/>
+      <c r="T314" s="6"/>
+    </row>
+    <row r="315" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B315" s="5"/>
+      <c r="C315" s="16"/>
+      <c r="D315" s="16"/>
+      <c r="E315" s="16"/>
+      <c r="F315" s="16"/>
+      <c r="G315" s="16"/>
+      <c r="H315" s="16"/>
+      <c r="I315" s="16"/>
+      <c r="J315" s="16"/>
+      <c r="K315" s="16"/>
+      <c r="L315" s="16"/>
+      <c r="M315" s="16"/>
+      <c r="N315" s="16"/>
+      <c r="O315" s="16"/>
+      <c r="P315" s="16"/>
+      <c r="Q315" s="16"/>
+      <c r="R315" s="16"/>
+      <c r="S315" s="16"/>
+      <c r="T315" s="6"/>
+    </row>
+    <row r="316" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B316" s="5"/>
+      <c r="C316" s="16"/>
+      <c r="D316" s="16"/>
+      <c r="E316" s="16"/>
+      <c r="F316" s="16"/>
+      <c r="G316" s="16"/>
+      <c r="H316" s="16"/>
+      <c r="I316" s="16"/>
+      <c r="J316" s="16"/>
+      <c r="K316" s="16"/>
+      <c r="L316" s="16"/>
+      <c r="M316" s="16"/>
+      <c r="N316" s="16"/>
+      <c r="O316" s="16"/>
+      <c r="P316" s="16"/>
+      <c r="Q316" s="16"/>
+      <c r="R316" s="16"/>
+      <c r="S316" s="16"/>
+      <c r="T316" s="6"/>
+    </row>
+    <row r="317" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B317" s="5"/>
+      <c r="C317" s="16"/>
+      <c r="D317" s="16"/>
+      <c r="E317" s="16"/>
+      <c r="F317" s="16"/>
+      <c r="G317" s="16"/>
+      <c r="H317" s="16"/>
+      <c r="I317" s="16"/>
+      <c r="J317" s="16"/>
+      <c r="K317" s="16"/>
+      <c r="L317" s="16"/>
+      <c r="M317" s="16"/>
+      <c r="N317" s="16"/>
+      <c r="O317" s="16"/>
+      <c r="P317" s="16"/>
+      <c r="Q317" s="16"/>
+      <c r="R317" s="16"/>
+      <c r="S317" s="16"/>
+      <c r="T317" s="6"/>
+    </row>
+    <row r="318" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B318" s="5"/>
+      <c r="C318" s="16"/>
+      <c r="D318" s="16"/>
+      <c r="E318" s="16"/>
+      <c r="F318" s="16"/>
+      <c r="G318" s="16"/>
+      <c r="H318" s="16"/>
+      <c r="I318" s="16"/>
+      <c r="J318" s="16"/>
+      <c r="K318" s="16"/>
+      <c r="L318" s="16"/>
+      <c r="M318" s="16"/>
+      <c r="N318" s="16"/>
+      <c r="O318" s="16"/>
+      <c r="P318" s="16"/>
+      <c r="Q318" s="16"/>
+      <c r="R318" s="16"/>
+      <c r="S318" s="16"/>
+      <c r="T318" s="6"/>
+    </row>
+    <row r="319" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B319" s="5"/>
+      <c r="C319" s="16"/>
+      <c r="D319" s="16"/>
+      <c r="E319" s="16"/>
+      <c r="F319" s="16"/>
+      <c r="G319" s="16"/>
+      <c r="H319" s="16"/>
+      <c r="I319" s="16"/>
+      <c r="J319" s="16"/>
+      <c r="K319" s="16"/>
+      <c r="L319" s="16"/>
+      <c r="M319" s="16"/>
+      <c r="N319" s="16"/>
+      <c r="O319" s="16"/>
+      <c r="P319" s="16"/>
+      <c r="Q319" s="16"/>
+      <c r="R319" s="16"/>
+      <c r="S319" s="16"/>
+      <c r="T319" s="6"/>
+    </row>
+    <row r="320" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B320" s="5"/>
+      <c r="C320" s="16"/>
+      <c r="D320" s="16"/>
+      <c r="E320" s="16"/>
+      <c r="F320" s="16"/>
+      <c r="G320" s="16"/>
+      <c r="H320" s="16"/>
+      <c r="I320" s="16"/>
+      <c r="J320" s="16"/>
+      <c r="K320" s="16"/>
+      <c r="L320" s="16"/>
+      <c r="M320" s="16"/>
+      <c r="N320" s="16"/>
+      <c r="O320" s="16"/>
+      <c r="P320" s="16"/>
+      <c r="Q320" s="16"/>
+      <c r="R320" s="16"/>
+      <c r="S320" s="16"/>
+      <c r="T320" s="6"/>
+    </row>
+    <row r="321" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B321" s="5"/>
+      <c r="C321" s="16"/>
+      <c r="D321" s="16"/>
+      <c r="E321" s="16"/>
+      <c r="F321" s="16"/>
+      <c r="G321" s="16"/>
+      <c r="H321" s="16"/>
+      <c r="I321" s="16"/>
+      <c r="J321" s="16"/>
+      <c r="K321" s="16"/>
+      <c r="L321" s="16"/>
+      <c r="M321" s="16"/>
+      <c r="N321" s="16"/>
+      <c r="O321" s="16"/>
+      <c r="P321" s="16"/>
+      <c r="Q321" s="16"/>
+      <c r="R321" s="16"/>
+      <c r="S321" s="16"/>
+      <c r="T321" s="6"/>
+    </row>
+    <row r="322" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B322" s="5"/>
+      <c r="C322" s="16"/>
+      <c r="D322" s="16"/>
+      <c r="E322" s="16"/>
+      <c r="F322" s="16"/>
+      <c r="G322" s="16"/>
+      <c r="H322" s="16"/>
+      <c r="I322" s="16"/>
+      <c r="J322" s="16"/>
+      <c r="K322" s="16"/>
+      <c r="L322" s="16"/>
+      <c r="M322" s="16"/>
+      <c r="N322" s="16"/>
+      <c r="O322" s="16"/>
+      <c r="P322" s="16"/>
+      <c r="Q322" s="16"/>
+      <c r="R322" s="16"/>
+      <c r="S322" s="16"/>
+      <c r="T322" s="6"/>
+    </row>
+    <row r="323" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B323" s="5"/>
+      <c r="C323" s="16"/>
+      <c r="D323" s="16"/>
+      <c r="E323" s="16"/>
+      <c r="F323" s="16"/>
+      <c r="G323" s="16"/>
+      <c r="H323" s="16"/>
+      <c r="I323" s="16"/>
+      <c r="J323" s="16"/>
+      <c r="K323" s="16"/>
+      <c r="L323" s="16"/>
+      <c r="M323" s="16"/>
+      <c r="N323" s="16"/>
+      <c r="O323" s="16"/>
+      <c r="P323" s="16"/>
+      <c r="Q323" s="16"/>
+      <c r="R323" s="16"/>
+      <c r="S323" s="16"/>
+      <c r="T323" s="6"/>
+    </row>
+    <row r="324" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B324" s="5"/>
+      <c r="C324" s="16"/>
+      <c r="D324" s="16"/>
+      <c r="E324" s="16"/>
+      <c r="F324" s="16"/>
+      <c r="G324" s="16"/>
+      <c r="H324" s="16"/>
+      <c r="I324" s="16"/>
+      <c r="J324" s="16"/>
+      <c r="K324" s="16"/>
+      <c r="L324" s="16"/>
+      <c r="M324" s="16"/>
+      <c r="N324" s="16"/>
+      <c r="O324" s="16"/>
+      <c r="P324" s="16"/>
+      <c r="Q324" s="16"/>
+      <c r="R324" s="16"/>
+      <c r="S324" s="16"/>
+      <c r="T324" s="6"/>
+    </row>
+    <row r="325" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B325" s="5"/>
+      <c r="C325" s="16"/>
+      <c r="D325" s="16"/>
+      <c r="E325" s="16"/>
+      <c r="F325" s="16"/>
+      <c r="G325" s="16"/>
+      <c r="H325" s="16"/>
+      <c r="I325" s="16"/>
+      <c r="J325" s="16"/>
+      <c r="K325" s="16"/>
+      <c r="L325" s="16"/>
+      <c r="M325" s="16"/>
+      <c r="N325" s="16"/>
+      <c r="O325" s="16"/>
+      <c r="P325" s="16"/>
+      <c r="Q325" s="16"/>
+      <c r="R325" s="16"/>
+      <c r="S325" s="16"/>
+      <c r="T325" s="6"/>
+    </row>
+    <row r="326" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B326" s="5"/>
+      <c r="C326" s="16"/>
+      <c r="D326" s="16"/>
+      <c r="E326" s="16"/>
+      <c r="F326" s="16"/>
+      <c r="G326" s="16"/>
+      <c r="H326" s="16"/>
+      <c r="I326" s="16"/>
+      <c r="J326" s="16"/>
+      <c r="K326" s="16"/>
+      <c r="L326" s="16"/>
+      <c r="M326" s="16"/>
+      <c r="N326" s="16"/>
+      <c r="O326" s="16"/>
+      <c r="P326" s="16"/>
+      <c r="Q326" s="16"/>
+      <c r="R326" s="16"/>
+      <c r="S326" s="16"/>
+      <c r="T326" s="6"/>
+    </row>
+    <row r="327" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B327" s="5"/>
+      <c r="C327" s="16"/>
+      <c r="D327" s="16"/>
+      <c r="E327" s="16"/>
+      <c r="F327" s="16"/>
+      <c r="G327" s="16"/>
+      <c r="H327" s="16"/>
+      <c r="I327" s="16"/>
+      <c r="J327" s="16"/>
+      <c r="K327" s="16"/>
+      <c r="L327" s="16"/>
+      <c r="M327" s="16"/>
+      <c r="N327" s="16"/>
+      <c r="O327" s="16"/>
+      <c r="P327" s="16"/>
+      <c r="Q327" s="16"/>
+      <c r="R327" s="16"/>
+      <c r="S327" s="16"/>
+      <c r="T327" s="6"/>
+    </row>
+    <row r="328" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B328" s="5"/>
+      <c r="C328" s="16"/>
+      <c r="D328" s="16"/>
+      <c r="E328" s="16"/>
+      <c r="F328" s="16"/>
+      <c r="G328" s="16"/>
+      <c r="H328" s="16"/>
+      <c r="I328" s="16"/>
+      <c r="J328" s="16"/>
+      <c r="K328" s="16"/>
+      <c r="L328" s="16"/>
+      <c r="M328" s="16"/>
+      <c r="N328" s="16"/>
+      <c r="O328" s="16"/>
+      <c r="P328" s="16"/>
+      <c r="Q328" s="16"/>
+      <c r="R328" s="16"/>
+      <c r="S328" s="16"/>
+      <c r="T328" s="6"/>
+    </row>
+    <row r="329" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B329" s="5"/>
+      <c r="C329" s="16"/>
+      <c r="D329" s="16"/>
+      <c r="E329" s="16"/>
+      <c r="F329" s="16"/>
+      <c r="G329" s="16"/>
+      <c r="H329" s="16"/>
+      <c r="I329" s="16"/>
+      <c r="J329" s="16"/>
+      <c r="K329" s="16"/>
+      <c r="L329" s="16"/>
+      <c r="M329" s="16"/>
+      <c r="N329" s="16"/>
+      <c r="O329" s="16"/>
+      <c r="P329" s="16"/>
+      <c r="Q329" s="16"/>
+      <c r="R329" s="16"/>
+      <c r="S329" s="16"/>
+      <c r="T329" s="6"/>
+    </row>
+    <row r="330" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B330" s="5"/>
+      <c r="C330" s="16"/>
+      <c r="D330" s="16"/>
+      <c r="E330" s="16"/>
+      <c r="F330" s="16"/>
+      <c r="G330" s="16"/>
+      <c r="H330" s="16"/>
+      <c r="I330" s="16"/>
+      <c r="J330" s="16"/>
+      <c r="K330" s="16"/>
+      <c r="L330" s="16"/>
+      <c r="M330" s="16"/>
+      <c r="N330" s="16"/>
+      <c r="O330" s="16"/>
+      <c r="P330" s="16"/>
+      <c r="Q330" s="16"/>
+      <c r="R330" s="16"/>
+      <c r="S330" s="16"/>
+      <c r="T330" s="6"/>
+    </row>
+    <row r="331" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B331" s="5"/>
+      <c r="C331" s="16"/>
+      <c r="D331" s="16"/>
+      <c r="E331" s="16"/>
+      <c r="F331" s="16"/>
+      <c r="G331" s="16"/>
+      <c r="H331" s="16"/>
+      <c r="I331" s="16"/>
+      <c r="J331" s="16"/>
+      <c r="K331" s="16"/>
+      <c r="L331" s="16"/>
+      <c r="M331" s="16"/>
+      <c r="N331" s="16"/>
+      <c r="O331" s="16"/>
+      <c r="P331" s="16"/>
+      <c r="Q331" s="16"/>
+      <c r="R331" s="16"/>
+      <c r="S331" s="16"/>
+      <c r="T331" s="6"/>
+    </row>
+    <row r="332" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B332" s="5"/>
+      <c r="C332" s="16"/>
+      <c r="D332" s="16"/>
+      <c r="E332" s="16"/>
+      <c r="F332" s="16"/>
+      <c r="G332" s="16"/>
+      <c r="H332" s="16"/>
+      <c r="I332" s="16"/>
+      <c r="J332" s="16"/>
+      <c r="K332" s="16"/>
+      <c r="L332" s="16"/>
+      <c r="M332" s="16"/>
+      <c r="N332" s="16"/>
+      <c r="O332" s="16"/>
+      <c r="P332" s="16"/>
+      <c r="Q332" s="16"/>
+      <c r="R332" s="16"/>
+      <c r="S332" s="16"/>
+      <c r="T332" s="6"/>
+    </row>
+    <row r="333" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B333" s="5"/>
+      <c r="C333" s="16"/>
+      <c r="D333" s="16"/>
+      <c r="E333" s="16"/>
+      <c r="F333" s="16"/>
+      <c r="G333" s="16"/>
+      <c r="H333" s="16"/>
+      <c r="I333" s="16"/>
+      <c r="J333" s="16"/>
+      <c r="K333" s="16"/>
+      <c r="L333" s="16"/>
+      <c r="M333" s="16"/>
+      <c r="N333" s="16"/>
+      <c r="O333" s="16"/>
+      <c r="P333" s="16"/>
+      <c r="Q333" s="16"/>
+      <c r="R333" s="16"/>
+      <c r="S333" s="16"/>
+      <c r="T333" s="6"/>
+    </row>
+    <row r="334" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B334" s="5"/>
+      <c r="C334" s="16"/>
+      <c r="D334" s="16"/>
+      <c r="E334" s="16"/>
+      <c r="F334" s="16"/>
+      <c r="G334" s="16"/>
+      <c r="H334" s="16"/>
+      <c r="I334" s="16"/>
+      <c r="J334" s="16"/>
+      <c r="K334" s="16"/>
+      <c r="L334" s="16"/>
+      <c r="M334" s="16"/>
+      <c r="N334" s="16"/>
+      <c r="O334" s="16"/>
+      <c r="P334" s="16"/>
+      <c r="Q334" s="16"/>
+      <c r="R334" s="16"/>
+      <c r="S334" s="16"/>
+      <c r="T334" s="6"/>
+    </row>
+    <row r="335" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B335" s="5"/>
+      <c r="C335" s="16"/>
+      <c r="D335" s="16"/>
+      <c r="E335" s="16"/>
+      <c r="F335" s="16"/>
+      <c r="G335" s="16"/>
+      <c r="H335" s="16"/>
+      <c r="I335" s="16"/>
+      <c r="J335" s="16"/>
+      <c r="K335" s="16"/>
+      <c r="L335" s="16"/>
+      <c r="M335" s="16"/>
+      <c r="N335" s="16"/>
+      <c r="O335" s="16"/>
+      <c r="P335" s="16"/>
+      <c r="Q335" s="16"/>
+      <c r="R335" s="16"/>
+      <c r="S335" s="16"/>
+      <c r="T335" s="6"/>
+    </row>
+    <row r="336" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B336" s="5"/>
+      <c r="C336" s="16"/>
+      <c r="D336" s="16"/>
+      <c r="E336" s="16"/>
+      <c r="F336" s="16"/>
+      <c r="G336" s="16"/>
+      <c r="H336" s="16"/>
+      <c r="I336" s="16"/>
+      <c r="J336" s="16"/>
+      <c r="K336" s="16"/>
+      <c r="L336" s="16"/>
+      <c r="M336" s="16"/>
+      <c r="N336" s="16"/>
+      <c r="O336" s="16"/>
+      <c r="P336" s="16"/>
+      <c r="Q336" s="16"/>
+      <c r="R336" s="16"/>
+      <c r="S336" s="16"/>
+      <c r="T336" s="6"/>
+    </row>
+    <row r="337" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B337" s="5"/>
+      <c r="C337" s="16"/>
+      <c r="D337" s="16"/>
+      <c r="E337" s="16"/>
+      <c r="F337" s="16"/>
+      <c r="G337" s="16"/>
+      <c r="H337" s="16"/>
+      <c r="I337" s="16"/>
+      <c r="J337" s="16"/>
+      <c r="K337" s="16"/>
+      <c r="L337" s="16"/>
+      <c r="M337" s="16"/>
+      <c r="N337" s="16"/>
+      <c r="O337" s="16"/>
+      <c r="P337" s="16"/>
+      <c r="Q337" s="16"/>
+      <c r="R337" s="16"/>
+      <c r="S337" s="16"/>
+      <c r="T337" s="6"/>
+    </row>
+    <row r="338" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B338" s="5"/>
+      <c r="C338" s="16"/>
+      <c r="D338" s="16"/>
+      <c r="E338" s="16"/>
+      <c r="F338" s="16"/>
+      <c r="G338" s="16"/>
+      <c r="H338" s="16"/>
+      <c r="I338" s="16"/>
+      <c r="J338" s="16"/>
+      <c r="K338" s="16"/>
+      <c r="L338" s="16"/>
+      <c r="M338" s="16"/>
+      <c r="N338" s="16"/>
+      <c r="O338" s="16"/>
+      <c r="P338" s="16"/>
+      <c r="Q338" s="16"/>
+      <c r="R338" s="16"/>
+      <c r="S338" s="16"/>
+      <c r="T338" s="6"/>
+    </row>
+    <row r="339" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B339" s="5"/>
+      <c r="C339" s="16"/>
+      <c r="D339" s="16"/>
+      <c r="E339" s="16"/>
+      <c r="F339" s="16"/>
+      <c r="G339" s="16"/>
+      <c r="H339" s="16"/>
+      <c r="I339" s="16"/>
+      <c r="J339" s="16"/>
+      <c r="K339" s="16"/>
+      <c r="L339" s="16"/>
+      <c r="M339" s="16"/>
+      <c r="N339" s="16"/>
+      <c r="O339" s="16"/>
+      <c r="P339" s="16"/>
+      <c r="Q339" s="16"/>
+      <c r="R339" s="16"/>
+      <c r="S339" s="16"/>
+      <c r="T339" s="6"/>
+    </row>
+    <row r="340" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B340" s="5"/>
+      <c r="C340" s="16"/>
+      <c r="D340" s="16"/>
+      <c r="E340" s="16"/>
+      <c r="F340" s="16"/>
+      <c r="G340" s="16"/>
+      <c r="H340" s="16"/>
+      <c r="I340" s="16"/>
+      <c r="J340" s="16"/>
+      <c r="K340" s="16"/>
+      <c r="L340" s="16"/>
+      <c r="M340" s="16"/>
+      <c r="N340" s="16"/>
+      <c r="O340" s="16"/>
+      <c r="P340" s="16"/>
+      <c r="Q340" s="16"/>
+      <c r="R340" s="16"/>
+      <c r="S340" s="16"/>
+      <c r="T340" s="6"/>
+    </row>
+    <row r="341" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B341" s="5"/>
+      <c r="C341" s="16"/>
+      <c r="D341" s="16"/>
+      <c r="E341" s="16"/>
+      <c r="F341" s="16"/>
+      <c r="G341" s="16"/>
+      <c r="H341" s="16"/>
+      <c r="I341" s="16"/>
+      <c r="J341" s="16"/>
+      <c r="K341" s="16"/>
+      <c r="L341" s="16"/>
+      <c r="M341" s="16"/>
+      <c r="N341" s="16"/>
+      <c r="O341" s="16"/>
+      <c r="P341" s="16"/>
+      <c r="Q341" s="16"/>
+      <c r="R341" s="16"/>
+      <c r="S341" s="16"/>
+      <c r="T341" s="6"/>
+    </row>
+    <row r="342" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B342" s="5"/>
+      <c r="C342" s="16"/>
+      <c r="D342" s="16"/>
+      <c r="E342" s="16"/>
+      <c r="F342" s="16"/>
+      <c r="G342" s="16"/>
+      <c r="H342" s="16"/>
+      <c r="I342" s="16"/>
+      <c r="J342" s="16"/>
+      <c r="K342" s="16"/>
+      <c r="L342" s="16"/>
+      <c r="M342" s="16"/>
+      <c r="N342" s="16"/>
+      <c r="O342" s="16"/>
+      <c r="P342" s="16"/>
+      <c r="Q342" s="16"/>
+      <c r="R342" s="16"/>
+      <c r="S342" s="16"/>
+      <c r="T342" s="6"/>
+    </row>
+    <row r="343" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B343" s="5"/>
+      <c r="C343" s="16"/>
+      <c r="D343" s="16"/>
+      <c r="E343" s="16"/>
+      <c r="F343" s="16"/>
+      <c r="G343" s="16"/>
+      <c r="H343" s="16"/>
+      <c r="I343" s="16"/>
+      <c r="J343" s="16"/>
+      <c r="K343" s="16"/>
+      <c r="L343" s="16"/>
+      <c r="M343" s="16"/>
+      <c r="N343" s="16"/>
+      <c r="O343" s="16"/>
+      <c r="P343" s="16"/>
+      <c r="Q343" s="16"/>
+      <c r="R343" s="16"/>
+      <c r="S343" s="16"/>
+      <c r="T343" s="6"/>
+    </row>
+    <row r="344" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B344" s="5"/>
+      <c r="C344" s="16"/>
+      <c r="D344" s="16"/>
+      <c r="E344" s="16"/>
+      <c r="F344" s="16"/>
+      <c r="G344" s="16"/>
+      <c r="H344" s="16"/>
+      <c r="I344" s="16"/>
+      <c r="J344" s="16"/>
+      <c r="K344" s="16"/>
+      <c r="L344" s="16"/>
+      <c r="M344" s="16"/>
+      <c r="N344" s="16"/>
+      <c r="O344" s="16"/>
+      <c r="P344" s="16"/>
+      <c r="Q344" s="16"/>
+      <c r="R344" s="16"/>
+      <c r="S344" s="16"/>
+      <c r="T344" s="6"/>
+    </row>
+    <row r="345" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B345" s="5"/>
+      <c r="C345" s="16"/>
+      <c r="D345" s="16"/>
+      <c r="E345" s="16"/>
+      <c r="F345" s="16"/>
+      <c r="G345" s="16"/>
+      <c r="H345" s="16"/>
+      <c r="I345" s="16"/>
+      <c r="J345" s="16"/>
+      <c r="K345" s="16"/>
+      <c r="L345" s="16"/>
+      <c r="M345" s="16"/>
+      <c r="N345" s="16"/>
+      <c r="O345" s="16"/>
+      <c r="P345" s="16"/>
+      <c r="Q345" s="16"/>
+      <c r="R345" s="16"/>
+      <c r="S345" s="16"/>
+      <c r="T345" s="6"/>
+    </row>
+    <row r="346" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B346" s="5"/>
+      <c r="C346" s="16"/>
+      <c r="D346" s="16"/>
+      <c r="E346" s="16"/>
+      <c r="F346" s="16"/>
+      <c r="G346" s="16"/>
+      <c r="H346" s="16"/>
+      <c r="I346" s="16"/>
+      <c r="J346" s="16"/>
+      <c r="K346" s="16"/>
+      <c r="L346" s="16"/>
+      <c r="M346" s="16"/>
+      <c r="N346" s="16"/>
+      <c r="O346" s="16"/>
+      <c r="P346" s="16"/>
+      <c r="Q346" s="16"/>
+      <c r="R346" s="16"/>
+      <c r="S346" s="16"/>
+      <c r="T346" s="6"/>
+    </row>
+    <row r="347" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B347" s="5"/>
+      <c r="C347" s="16"/>
+      <c r="D347" s="16"/>
+      <c r="E347" s="16"/>
+      <c r="F347" s="16"/>
+      <c r="G347" s="16"/>
+      <c r="H347" s="16"/>
+      <c r="I347" s="16"/>
+      <c r="J347" s="16"/>
+      <c r="K347" s="16"/>
+      <c r="L347" s="16"/>
+      <c r="M347" s="16"/>
+      <c r="N347" s="16"/>
+      <c r="O347" s="16"/>
+      <c r="P347" s="16"/>
+      <c r="Q347" s="16"/>
+      <c r="R347" s="16"/>
+      <c r="S347" s="16"/>
+      <c r="T347" s="6"/>
+    </row>
+    <row r="348" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B348" s="5"/>
+      <c r="C348" s="16"/>
+      <c r="D348" s="16"/>
+      <c r="E348" s="16"/>
+      <c r="F348" s="16"/>
+      <c r="G348" s="16"/>
+      <c r="H348" s="16"/>
+      <c r="I348" s="16"/>
+      <c r="J348" s="16"/>
+      <c r="K348" s="16"/>
+      <c r="L348" s="16"/>
+      <c r="M348" s="16"/>
+      <c r="N348" s="16"/>
+      <c r="O348" s="16"/>
+      <c r="P348" s="16"/>
+      <c r="Q348" s="16"/>
+      <c r="R348" s="16"/>
+      <c r="S348" s="16"/>
+      <c r="T348" s="6"/>
+    </row>
+    <row r="349" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B349" s="5"/>
+      <c r="C349" s="16"/>
+      <c r="D349" s="16"/>
+      <c r="E349" s="16"/>
+      <c r="F349" s="16"/>
+      <c r="G349" s="16"/>
+      <c r="H349" s="16"/>
+      <c r="I349" s="16"/>
+      <c r="J349" s="16"/>
+      <c r="K349" s="16"/>
+      <c r="L349" s="16"/>
+      <c r="M349" s="16"/>
+      <c r="N349" s="16"/>
+      <c r="O349" s="16"/>
+      <c r="P349" s="16"/>
+      <c r="Q349" s="16"/>
+      <c r="R349" s="16"/>
+      <c r="S349" s="16"/>
+      <c r="T349" s="6"/>
+    </row>
+    <row r="350" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B350" s="5"/>
+      <c r="C350" s="16"/>
+      <c r="D350" s="16"/>
+      <c r="E350" s="16"/>
+      <c r="F350" s="16"/>
+      <c r="G350" s="16"/>
+      <c r="H350" s="16"/>
+      <c r="I350" s="16"/>
+      <c r="J350" s="16"/>
+      <c r="K350" s="16"/>
+      <c r="L350" s="16"/>
+      <c r="M350" s="16"/>
+      <c r="N350" s="16"/>
+      <c r="O350" s="16"/>
+      <c r="P350" s="16"/>
+      <c r="Q350" s="16"/>
+      <c r="R350" s="16"/>
+      <c r="S350" s="16"/>
+      <c r="T350" s="6"/>
+    </row>
+    <row r="351" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B351" s="5"/>
+      <c r="C351" s="16"/>
+      <c r="D351" s="16"/>
+      <c r="E351" s="16"/>
+      <c r="F351" s="16"/>
+      <c r="G351" s="16"/>
+      <c r="H351" s="16"/>
+      <c r="I351" s="16"/>
+      <c r="J351" s="16"/>
+      <c r="K351" s="16"/>
+      <c r="L351" s="16"/>
+      <c r="M351" s="16"/>
+      <c r="N351" s="16"/>
+      <c r="O351" s="16"/>
+      <c r="P351" s="16"/>
+      <c r="Q351" s="16"/>
+      <c r="R351" s="16"/>
+      <c r="S351" s="16"/>
+      <c r="T351" s="6"/>
+    </row>
+    <row r="352" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B352" s="5"/>
+      <c r="C352" s="16"/>
+      <c r="D352" s="16"/>
+      <c r="E352" s="16"/>
+      <c r="F352" s="16"/>
+      <c r="G352" s="16"/>
+      <c r="H352" s="16"/>
+      <c r="I352" s="16"/>
+      <c r="J352" s="16"/>
+      <c r="K352" s="16"/>
+      <c r="L352" s="16"/>
+      <c r="M352" s="16"/>
+      <c r="N352" s="16"/>
+      <c r="O352" s="16"/>
+      <c r="P352" s="16"/>
+      <c r="Q352" s="16"/>
+      <c r="R352" s="16"/>
+      <c r="S352" s="16"/>
+      <c r="T352" s="6"/>
+    </row>
+    <row r="353" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B353" s="5"/>
+      <c r="C353" s="16"/>
+      <c r="D353" s="16"/>
+      <c r="E353" s="16"/>
+      <c r="F353" s="16"/>
+      <c r="G353" s="16"/>
+      <c r="H353" s="16"/>
+      <c r="I353" s="16"/>
+      <c r="J353" s="16"/>
+      <c r="K353" s="16"/>
+      <c r="L353" s="16"/>
+      <c r="M353" s="16"/>
+      <c r="N353" s="16"/>
+      <c r="O353" s="16"/>
+      <c r="P353" s="16"/>
+      <c r="Q353" s="16"/>
+      <c r="R353" s="16"/>
+      <c r="S353" s="16"/>
+      <c r="T353" s="6"/>
+    </row>
+    <row r="354" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B354" s="5"/>
+      <c r="C354" s="16"/>
+      <c r="D354" s="16"/>
+      <c r="E354" s="16"/>
+      <c r="F354" s="16"/>
+      <c r="G354" s="16"/>
+      <c r="H354" s="16"/>
+      <c r="I354" s="16"/>
+      <c r="J354" s="16"/>
+      <c r="K354" s="16"/>
+      <c r="L354" s="16"/>
+      <c r="M354" s="16"/>
+      <c r="N354" s="16"/>
+      <c r="O354" s="16"/>
+      <c r="P354" s="16"/>
+      <c r="Q354" s="16"/>
+      <c r="R354" s="16"/>
+      <c r="S354" s="16"/>
+      <c r="T354" s="6"/>
+    </row>
+    <row r="355" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B355" s="5"/>
+      <c r="C355" s="16"/>
+      <c r="D355" s="16"/>
+      <c r="E355" s="16"/>
+      <c r="F355" s="16"/>
+      <c r="G355" s="16"/>
+      <c r="H355" s="16"/>
+      <c r="I355" s="16"/>
+      <c r="J355" s="16"/>
+      <c r="K355" s="16"/>
+      <c r="L355" s="16"/>
+      <c r="M355" s="16"/>
+      <c r="N355" s="16"/>
+      <c r="O355" s="16"/>
+      <c r="P355" s="16"/>
+      <c r="Q355" s="16"/>
+      <c r="R355" s="16"/>
+      <c r="S355" s="16"/>
+      <c r="T355" s="6"/>
+    </row>
+    <row r="356" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B356" s="5"/>
+      <c r="C356" s="16"/>
+      <c r="D356" s="16"/>
+      <c r="E356" s="16"/>
+      <c r="F356" s="16"/>
+      <c r="G356" s="16"/>
+      <c r="H356" s="16"/>
+      <c r="I356" s="16"/>
+      <c r="J356" s="16"/>
+      <c r="K356" s="16"/>
+      <c r="L356" s="16"/>
+      <c r="M356" s="16"/>
+      <c r="N356" s="16"/>
+      <c r="O356" s="16"/>
+      <c r="P356" s="16"/>
+      <c r="Q356" s="16"/>
+      <c r="R356" s="16"/>
+      <c r="S356" s="16"/>
+      <c r="T356" s="6"/>
+    </row>
+    <row r="357" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B357" s="5"/>
+      <c r="C357" s="16"/>
+      <c r="D357" s="16"/>
+      <c r="E357" s="16"/>
+      <c r="F357" s="16"/>
+      <c r="G357" s="16"/>
+      <c r="H357" s="16"/>
+      <c r="I357" s="16"/>
+      <c r="J357" s="16"/>
+      <c r="K357" s="16"/>
+      <c r="L357" s="16"/>
+      <c r="M357" s="16"/>
+      <c r="N357" s="16"/>
+      <c r="O357" s="16"/>
+      <c r="P357" s="16"/>
+      <c r="Q357" s="16"/>
+      <c r="R357" s="16"/>
+      <c r="S357" s="16"/>
+      <c r="T357" s="6"/>
+    </row>
+    <row r="358" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B358" s="5"/>
+      <c r="C358" s="16"/>
+      <c r="D358" s="16"/>
+      <c r="E358" s="16"/>
+      <c r="F358" s="16"/>
+      <c r="G358" s="16"/>
+      <c r="H358" s="16"/>
+      <c r="I358" s="16"/>
+      <c r="J358" s="16"/>
+      <c r="K358" s="16"/>
+      <c r="L358" s="16"/>
+      <c r="M358" s="16"/>
+      <c r="N358" s="16"/>
+      <c r="O358" s="16"/>
+      <c r="P358" s="16"/>
+      <c r="Q358" s="16"/>
+      <c r="R358" s="16"/>
+      <c r="S358" s="16"/>
+      <c r="T358" s="6"/>
+    </row>
+    <row r="359" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B359" s="5"/>
+      <c r="C359" s="16"/>
+      <c r="D359" s="16"/>
+      <c r="E359" s="16"/>
+      <c r="F359" s="16"/>
+      <c r="G359" s="16"/>
+      <c r="H359" s="16"/>
+      <c r="I359" s="16"/>
+      <c r="J359" s="16"/>
+      <c r="K359" s="16"/>
+      <c r="L359" s="16"/>
+      <c r="M359" s="16"/>
+      <c r="N359" s="16"/>
+      <c r="O359" s="16"/>
+      <c r="P359" s="16"/>
+      <c r="Q359" s="16"/>
+      <c r="R359" s="16"/>
+      <c r="S359" s="16"/>
+      <c r="T359" s="6"/>
+    </row>
+    <row r="360" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B360" s="5"/>
+      <c r="C360" s="16"/>
+      <c r="D360" s="16"/>
+      <c r="E360" s="16"/>
+      <c r="F360" s="16"/>
+      <c r="G360" s="16"/>
+      <c r="H360" s="16"/>
+      <c r="I360" s="16"/>
+      <c r="J360" s="16"/>
+      <c r="K360" s="16"/>
+      <c r="L360" s="16"/>
+      <c r="M360" s="16"/>
+      <c r="N360" s="16"/>
+      <c r="O360" s="16"/>
+      <c r="P360" s="16"/>
+      <c r="Q360" s="16"/>
+      <c r="R360" s="16"/>
+      <c r="S360" s="16"/>
+      <c r="T360" s="6"/>
+    </row>
+    <row r="361" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B361" s="5"/>
+      <c r="C361" s="16"/>
+      <c r="D361" s="16"/>
+      <c r="E361" s="16"/>
+      <c r="F361" s="16"/>
+      <c r="G361" s="16"/>
+      <c r="H361" s="16"/>
+      <c r="I361" s="16"/>
+      <c r="J361" s="16"/>
+      <c r="K361" s="16"/>
+      <c r="L361" s="16"/>
+      <c r="M361" s="16"/>
+      <c r="N361" s="16"/>
+      <c r="O361" s="16"/>
+      <c r="P361" s="16"/>
+      <c r="Q361" s="16"/>
+      <c r="R361" s="16"/>
+      <c r="S361" s="16"/>
+      <c r="T361" s="6"/>
+    </row>
+    <row r="362" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B362" s="5"/>
+      <c r="C362" s="16"/>
+      <c r="D362" s="16"/>
+      <c r="E362" s="16"/>
+      <c r="F362" s="16"/>
+      <c r="G362" s="16"/>
+      <c r="H362" s="16"/>
+      <c r="I362" s="16"/>
+      <c r="J362" s="16"/>
+      <c r="K362" s="16"/>
+      <c r="L362" s="16"/>
+      <c r="M362" s="16"/>
+      <c r="N362" s="16"/>
+      <c r="O362" s="16"/>
+      <c r="P362" s="16"/>
+      <c r="Q362" s="16"/>
+      <c r="R362" s="16"/>
+      <c r="S362" s="16"/>
+      <c r="T362" s="6"/>
+    </row>
+    <row r="363" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B363" s="5"/>
+      <c r="C363" s="16"/>
+      <c r="D363" s="16"/>
+      <c r="E363" s="16"/>
+      <c r="F363" s="16"/>
+      <c r="G363" s="16"/>
+      <c r="H363" s="16"/>
+      <c r="I363" s="16"/>
+      <c r="J363" s="16"/>
+      <c r="K363" s="16"/>
+      <c r="L363" s="16"/>
+      <c r="M363" s="16"/>
+      <c r="N363" s="16"/>
+      <c r="O363" s="16"/>
+      <c r="P363" s="16"/>
+      <c r="Q363" s="16"/>
+      <c r="R363" s="16"/>
+      <c r="S363" s="16"/>
+      <c r="T363" s="6"/>
+    </row>
+    <row r="364" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B364" s="5"/>
+      <c r="C364" s="16"/>
+      <c r="D364" s="16"/>
+      <c r="E364" s="16"/>
+      <c r="F364" s="16"/>
+      <c r="G364" s="16"/>
+      <c r="H364" s="16"/>
+      <c r="I364" s="16"/>
+      <c r="J364" s="16"/>
+      <c r="K364" s="16"/>
+      <c r="L364" s="16"/>
+      <c r="M364" s="16"/>
+      <c r="N364" s="16"/>
+      <c r="O364" s="16"/>
+      <c r="P364" s="16"/>
+      <c r="Q364" s="16"/>
+      <c r="R364" s="16"/>
+      <c r="S364" s="16"/>
+      <c r="T364" s="6"/>
+    </row>
+    <row r="365" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B365" s="5"/>
+      <c r="C365" s="16"/>
+      <c r="D365" s="16"/>
+      <c r="E365" s="16"/>
+      <c r="F365" s="16"/>
+      <c r="G365" s="16"/>
+      <c r="H365" s="16"/>
+      <c r="I365" s="16"/>
+      <c r="J365" s="16"/>
+      <c r="K365" s="16"/>
+      <c r="L365" s="16"/>
+      <c r="M365" s="16"/>
+      <c r="N365" s="16"/>
+      <c r="O365" s="16"/>
+      <c r="P365" s="16"/>
+      <c r="Q365" s="16"/>
+      <c r="R365" s="16"/>
+      <c r="S365" s="16"/>
+      <c r="T365" s="6"/>
+    </row>
+    <row r="366" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B366" s="5"/>
+      <c r="C366" s="16"/>
+      <c r="D366" s="16"/>
+      <c r="E366" s="16"/>
+      <c r="F366" s="16"/>
+      <c r="G366" s="16"/>
+      <c r="H366" s="16"/>
+      <c r="I366" s="16"/>
+      <c r="J366" s="16"/>
+      <c r="K366" s="16"/>
+      <c r="L366" s="16"/>
+      <c r="M366" s="16"/>
+      <c r="N366" s="16"/>
+      <c r="O366" s="16"/>
+      <c r="P366" s="16"/>
+      <c r="Q366" s="16"/>
+      <c r="R366" s="16"/>
+      <c r="S366" s="16"/>
+      <c r="T366" s="6"/>
+    </row>
+    <row r="367" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B367" s="5"/>
+      <c r="C367" s="16"/>
+      <c r="D367" s="16"/>
+      <c r="E367" s="16"/>
+      <c r="F367" s="16"/>
+      <c r="G367" s="16"/>
+      <c r="H367" s="16"/>
+      <c r="I367" s="16"/>
+      <c r="J367" s="16"/>
+      <c r="K367" s="16"/>
+      <c r="L367" s="16"/>
+      <c r="M367" s="16"/>
+      <c r="N367" s="16"/>
+      <c r="O367" s="16"/>
+      <c r="P367" s="16"/>
+      <c r="Q367" s="16"/>
+      <c r="R367" s="16"/>
+      <c r="S367" s="16"/>
+      <c r="T367" s="6"/>
+    </row>
+    <row r="368" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B368" s="5"/>
+      <c r="C368" s="16"/>
+      <c r="D368" s="16"/>
+      <c r="E368" s="16"/>
+      <c r="F368" s="16"/>
+      <c r="G368" s="16"/>
+      <c r="H368" s="16"/>
+      <c r="I368" s="16"/>
+      <c r="J368" s="16"/>
+      <c r="K368" s="16"/>
+      <c r="L368" s="16"/>
+      <c r="M368" s="16"/>
+      <c r="N368" s="16"/>
+      <c r="O368" s="16"/>
+      <c r="P368" s="16"/>
+      <c r="Q368" s="16"/>
+      <c r="R368" s="16"/>
+      <c r="S368" s="16"/>
+      <c r="T368" s="6"/>
+    </row>
+    <row r="369" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B369" s="5"/>
+      <c r="C369" s="16"/>
+      <c r="D369" s="16"/>
+      <c r="E369" s="16"/>
+      <c r="F369" s="16"/>
+      <c r="G369" s="16"/>
+      <c r="H369" s="16"/>
+      <c r="I369" s="16"/>
+      <c r="J369" s="16"/>
+      <c r="K369" s="16"/>
+      <c r="L369" s="16"/>
+      <c r="M369" s="16"/>
+      <c r="N369" s="16"/>
+      <c r="O369" s="16"/>
+      <c r="P369" s="16"/>
+      <c r="Q369" s="16"/>
+      <c r="R369" s="16"/>
+      <c r="S369" s="16"/>
+      <c r="T369" s="6"/>
+    </row>
+    <row r="370" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B370" s="5"/>
+      <c r="C370" s="16"/>
+      <c r="D370" s="16"/>
+      <c r="E370" s="16"/>
+      <c r="F370" s="16"/>
+      <c r="G370" s="16"/>
+      <c r="H370" s="16"/>
+      <c r="I370" s="16"/>
+      <c r="J370" s="16"/>
+      <c r="K370" s="16"/>
+      <c r="L370" s="16"/>
+      <c r="M370" s="16"/>
+      <c r="N370" s="16"/>
+      <c r="O370" s="16"/>
+      <c r="P370" s="16"/>
+      <c r="Q370" s="16"/>
+      <c r="R370" s="16"/>
+      <c r="S370" s="16"/>
+      <c r="T370" s="6"/>
+    </row>
+    <row r="371" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B371" s="5"/>
+      <c r="C371" s="16"/>
+      <c r="D371" s="16"/>
+      <c r="E371" s="16"/>
+      <c r="F371" s="16"/>
+      <c r="G371" s="16"/>
+      <c r="H371" s="16"/>
+      <c r="I371" s="16"/>
+      <c r="J371" s="16"/>
+      <c r="K371" s="16"/>
+      <c r="L371" s="16"/>
+      <c r="M371" s="16"/>
+      <c r="N371" s="16"/>
+      <c r="O371" s="16"/>
+      <c r="P371" s="16"/>
+      <c r="Q371" s="16"/>
+      <c r="R371" s="16"/>
+      <c r="S371" s="16"/>
+      <c r="T371" s="6"/>
+    </row>
+    <row r="372" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B372" s="5"/>
+      <c r="C372" s="16"/>
+      <c r="D372" s="16"/>
+      <c r="E372" s="16"/>
+      <c r="F372" s="16"/>
+      <c r="G372" s="16"/>
+      <c r="H372" s="16"/>
+      <c r="I372" s="16"/>
+      <c r="J372" s="16"/>
+      <c r="K372" s="16"/>
+      <c r="L372" s="16"/>
+      <c r="M372" s="16"/>
+      <c r="N372" s="16"/>
+      <c r="O372" s="16"/>
+      <c r="P372" s="16"/>
+      <c r="Q372" s="16"/>
+      <c r="R372" s="16"/>
+      <c r="S372" s="16"/>
+      <c r="T372" s="6"/>
+    </row>
+    <row r="373" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B373" s="8"/>
+      <c r="C373" s="9"/>
+      <c r="D373" s="9"/>
+      <c r="E373" s="9"/>
+      <c r="F373" s="9"/>
+      <c r="G373" s="9"/>
+      <c r="H373" s="9"/>
+      <c r="I373" s="9"/>
+      <c r="J373" s="9"/>
+      <c r="K373" s="9"/>
+      <c r="L373" s="9"/>
+      <c r="M373" s="9"/>
+      <c r="N373" s="9"/>
+      <c r="O373" s="9"/>
+      <c r="P373" s="9"/>
+      <c r="Q373" s="9"/>
+      <c r="R373" s="9"/>
+      <c r="S373" s="9"/>
+      <c r="T373" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0EA440-FB41-4A25-888F-10879DE1E42C}">
+  <dimension ref="A4:N302"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A363" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K379" sqref="K379"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="G20" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="G23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="H24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="H27" t="s">
+        <v>23</v>
+      </c>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="H28" t="s">
+        <v>24</v>
+      </c>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="G29" t="s">
+        <v>25</v>
+      </c>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="H30" t="s">
+        <v>26</v>
+      </c>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="H31" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="H32" t="s">
+        <v>28</v>
+      </c>
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="F33" t="s">
+        <v>29</v>
+      </c>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="G34" t="s">
+        <v>30</v>
+      </c>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="H35" t="s">
+        <v>31</v>
+      </c>
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="H36" t="s">
+        <v>32</v>
+      </c>
+      <c r="L36" s="6"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="H37" t="s">
+        <v>33</v>
+      </c>
+      <c r="L37" s="6"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="H38" t="s">
+        <v>34</v>
+      </c>
+      <c r="L38" s="6"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="G39" t="s">
+        <v>35</v>
+      </c>
+      <c r="L39" s="6"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="H40" t="s">
+        <v>36</v>
+      </c>
+      <c r="L40" s="6"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="H41" t="s">
+        <v>37</v>
+      </c>
+      <c r="L41" s="6"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="H42" t="s">
+        <v>38</v>
+      </c>
+      <c r="L42" s="6"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="G43" t="s">
+        <v>39</v>
+      </c>
+      <c r="L43" s="6"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="H44" t="s">
+        <v>40</v>
+      </c>
+      <c r="L44" s="6"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="H45" t="s">
+        <v>41</v>
+      </c>
+      <c r="L45" s="6"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="H46" t="s">
+        <v>42</v>
+      </c>
+      <c r="L46" s="6"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+      <c r="G47" t="s">
+        <v>43</v>
+      </c>
+      <c r="L47" s="6"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="H48" t="s">
+        <v>44</v>
+      </c>
+      <c r="L48" s="6"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+      <c r="H49" t="s">
+        <v>45</v>
+      </c>
+      <c r="L49" s="6"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
+      <c r="H50" t="s">
+        <v>46</v>
+      </c>
+      <c r="L50" s="6"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="G51" t="s">
+        <v>47</v>
+      </c>
+      <c r="L51" s="6"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="5"/>
+      <c r="H52" t="s">
+        <v>48</v>
+      </c>
+      <c r="L52" s="6"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="5"/>
+      <c r="H53" t="s">
+        <v>49</v>
+      </c>
+      <c r="L53" s="6"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="5"/>
+      <c r="G54" t="s">
+        <v>50</v>
+      </c>
+      <c r="L54" s="6"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" s="5"/>
+      <c r="H55" t="s">
+        <v>51</v>
+      </c>
+      <c r="L55" s="6"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="5"/>
+      <c r="H56" t="s">
+        <v>52</v>
+      </c>
+      <c r="L56" s="6"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" s="5"/>
+      <c r="G57" t="s">
+        <v>53</v>
+      </c>
+      <c r="L57" s="6"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" s="5"/>
+      <c r="H58" t="s">
+        <v>54</v>
+      </c>
+      <c r="L58" s="6"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B59" s="5"/>
+      <c r="G59" t="s">
+        <v>55</v>
+      </c>
+      <c r="L59" s="6"/>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B60" s="5"/>
+      <c r="H60" t="s">
+        <v>56</v>
+      </c>
+      <c r="L60" s="6"/>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B61" s="5"/>
+      <c r="H61" t="s">
+        <v>57</v>
+      </c>
+      <c r="L61" s="6"/>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B62" s="5"/>
+      <c r="H62" t="s">
+        <v>58</v>
+      </c>
+      <c r="L62" s="6"/>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B63" s="5"/>
+      <c r="G63" t="s">
+        <v>59</v>
+      </c>
+      <c r="L63" s="6"/>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B64" s="5"/>
+      <c r="H64" t="s">
+        <v>60</v>
+      </c>
+      <c r="L64" s="6"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="5"/>
+      <c r="H65" t="s">
+        <v>61</v>
+      </c>
+      <c r="L65" s="6"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="5"/>
+      <c r="H66" t="s">
+        <v>62</v>
+      </c>
+      <c r="L66" s="6"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B67" s="5"/>
+      <c r="G67" t="s">
+        <v>63</v>
+      </c>
+      <c r="L67" s="6"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B68" s="5"/>
+      <c r="H68" t="s">
+        <v>64</v>
+      </c>
+      <c r="L68" s="6"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="5"/>
+      <c r="H69" t="s">
+        <v>65</v>
+      </c>
+      <c r="L69" s="6"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B70" s="5"/>
+      <c r="H70" t="s">
+        <v>66</v>
+      </c>
+      <c r="L70" s="6"/>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="5"/>
+      <c r="G71" t="s">
+        <v>67</v>
+      </c>
+      <c r="L71" s="6"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="H72" t="s">
+        <v>68</v>
+      </c>
+      <c r="L72" s="6"/>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B73" s="5"/>
+      <c r="H73" t="s">
+        <v>69</v>
+      </c>
+      <c r="L73" s="6"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B74" s="5"/>
+      <c r="G74" t="s">
+        <v>70</v>
+      </c>
+      <c r="L74" s="6"/>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B75" s="5"/>
+      <c r="H75" t="s">
+        <v>71</v>
+      </c>
+      <c r="L75" s="6"/>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B76" s="5"/>
+      <c r="H76" t="s">
+        <v>72</v>
+      </c>
+      <c r="L76" s="6"/>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B77" s="5"/>
+      <c r="G77" t="s">
+        <v>73</v>
+      </c>
+      <c r="L77" s="6"/>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B78" s="5"/>
+      <c r="H78" t="s">
+        <v>74</v>
+      </c>
+      <c r="L78" s="6"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="5"/>
+      <c r="H79" t="s">
+        <v>75</v>
+      </c>
+      <c r="L79" s="6"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="5"/>
+      <c r="H80" t="s">
+        <v>76</v>
+      </c>
+      <c r="L80" s="6"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81" s="5"/>
+      <c r="G81" t="s">
+        <v>77</v>
+      </c>
+      <c r="L81" s="6"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82" s="5"/>
+      <c r="H82" t="s">
+        <v>78</v>
+      </c>
+      <c r="L82" s="6"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="H83" t="s">
+        <v>79</v>
+      </c>
+      <c r="L83" s="6"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" s="5"/>
+      <c r="H84" t="s">
+        <v>80</v>
+      </c>
+      <c r="L84" s="6"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" s="5"/>
+      <c r="G85" t="s">
+        <v>81</v>
+      </c>
+      <c r="L85" s="6"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" s="5"/>
+      <c r="H86" t="s">
+        <v>82</v>
+      </c>
+      <c r="L86" s="6"/>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B87" s="5"/>
+      <c r="H87" t="s">
+        <v>83</v>
+      </c>
+      <c r="L87" s="6"/>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B88" s="5"/>
+      <c r="H88" t="s">
+        <v>84</v>
+      </c>
+      <c r="L88" s="6"/>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B89" s="5"/>
+      <c r="G89" t="s">
+        <v>85</v>
+      </c>
+      <c r="L89" s="6"/>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B90" s="5"/>
+      <c r="H90" t="s">
+        <v>86</v>
+      </c>
+      <c r="L90" s="6"/>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B91" s="5"/>
+      <c r="H91" t="s">
+        <v>87</v>
+      </c>
+      <c r="L91" s="6"/>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B92" s="5"/>
+      <c r="G92" t="s">
+        <v>88</v>
+      </c>
+      <c r="L92" s="6"/>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B93" s="5"/>
+      <c r="H93" t="s">
+        <v>89</v>
+      </c>
+      <c r="L93" s="6"/>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B94" s="5"/>
+      <c r="H94" t="s">
+        <v>90</v>
+      </c>
+      <c r="L94" s="6"/>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B95" s="5"/>
+      <c r="H95" t="s">
+        <v>91</v>
+      </c>
+      <c r="L95" s="6"/>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B96" s="5"/>
+      <c r="G96" t="s">
+        <v>92</v>
+      </c>
+      <c r="L96" s="6"/>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B97" s="5"/>
+      <c r="H97" t="s">
+        <v>93</v>
+      </c>
+      <c r="L97" s="6"/>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B98" s="5"/>
+      <c r="H98" t="s">
+        <v>94</v>
+      </c>
+      <c r="L98" s="6"/>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B99" s="5"/>
+      <c r="H99" t="s">
+        <v>95</v>
+      </c>
+      <c r="L99" s="6"/>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B100" s="5"/>
+      <c r="G100" t="s">
+        <v>96</v>
+      </c>
+      <c r="L100" s="6"/>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B101" s="5"/>
+      <c r="H101" t="s">
+        <v>97</v>
+      </c>
+      <c r="L101" s="6"/>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B102" s="5"/>
+      <c r="H102" t="s">
+        <v>98</v>
+      </c>
+      <c r="L102" s="6"/>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B103" s="5"/>
+      <c r="H103" t="s">
+        <v>99</v>
+      </c>
+      <c r="L103" s="6"/>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B104" s="5"/>
+      <c r="H104" t="s">
+        <v>100</v>
+      </c>
+      <c r="L104" s="6"/>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B105" s="5"/>
+      <c r="G105" t="s">
+        <v>101</v>
+      </c>
+      <c r="L105" s="6"/>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B106" s="5"/>
+      <c r="H106" t="s">
+        <v>102</v>
+      </c>
+      <c r="L106" s="6"/>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B107" s="5"/>
+      <c r="H107" t="s">
+        <v>103</v>
+      </c>
+      <c r="L107" s="6"/>
+    </row>
+    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B108" s="5"/>
+      <c r="H108" t="s">
+        <v>104</v>
+      </c>
+      <c r="L108" s="6"/>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B109" s="5"/>
+      <c r="G109" t="s">
+        <v>105</v>
+      </c>
+      <c r="L109" s="6"/>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B110" s="5"/>
+      <c r="H110" t="s">
+        <v>106</v>
+      </c>
+      <c r="L110" s="6"/>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B111" s="5"/>
+      <c r="H111" t="s">
+        <v>107</v>
+      </c>
+      <c r="L111" s="6"/>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B112" s="5"/>
+      <c r="H112" t="s">
+        <v>108</v>
+      </c>
+      <c r="L112" s="6"/>
+    </row>
+    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B113" s="5"/>
+      <c r="G113" t="s">
+        <v>109</v>
+      </c>
+      <c r="L113" s="6"/>
+    </row>
+    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B114" s="5"/>
+      <c r="H114" t="s">
+        <v>110</v>
+      </c>
+      <c r="L114" s="6"/>
+    </row>
+    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B115" s="5"/>
+      <c r="I115" t="s">
+        <v>111</v>
+      </c>
+      <c r="L115" s="6"/>
+    </row>
+    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B116" s="5"/>
+      <c r="H116" t="s">
+        <v>112</v>
+      </c>
+      <c r="L116" s="6"/>
+    </row>
+    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B117" s="5"/>
+      <c r="H117" t="s">
+        <v>113</v>
+      </c>
+      <c r="L117" s="6"/>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B118" s="5"/>
+      <c r="G118" t="s">
+        <v>114</v>
+      </c>
+      <c r="L118" s="6"/>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B119" s="5"/>
+      <c r="H119" t="s">
+        <v>115</v>
+      </c>
+      <c r="L119" s="6"/>
+    </row>
+    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B120" s="5"/>
+      <c r="H120" t="s">
+        <v>116</v>
+      </c>
+      <c r="L120" s="6"/>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B121" s="5"/>
+      <c r="H121" t="s">
+        <v>117</v>
+      </c>
+      <c r="L121" s="6"/>
+    </row>
+    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B122" s="5"/>
+      <c r="H122" t="s">
+        <v>118</v>
+      </c>
+      <c r="L122" s="6"/>
+    </row>
+    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B123" s="5"/>
+      <c r="G123" t="s">
+        <v>119</v>
+      </c>
+      <c r="L123" s="6"/>
+    </row>
+    <row r="124" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B124" s="5"/>
+      <c r="H124" t="s">
+        <v>120</v>
+      </c>
+      <c r="L124" s="6"/>
+    </row>
+    <row r="125" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B125" s="5"/>
+      <c r="H125" t="s">
+        <v>121</v>
+      </c>
+      <c r="L125" s="6"/>
+    </row>
+    <row r="126" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B126" s="5"/>
+      <c r="H126" t="s">
+        <v>122</v>
+      </c>
+      <c r="L126" s="6"/>
+    </row>
+    <row r="127" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B127" s="5"/>
+      <c r="G127" t="s">
+        <v>123</v>
+      </c>
+      <c r="L127" s="6"/>
+    </row>
+    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B128" s="5"/>
+      <c r="H128" t="s">
+        <v>124</v>
+      </c>
+      <c r="L128" s="6"/>
+    </row>
+    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B129" s="5"/>
+      <c r="H129" t="s">
+        <v>125</v>
+      </c>
+      <c r="L129" s="6"/>
+    </row>
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B130" s="5"/>
+      <c r="H130" t="s">
+        <v>126</v>
+      </c>
+      <c r="L130" s="6"/>
+    </row>
+    <row r="131" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B131" s="5"/>
+      <c r="H131" t="s">
+        <v>127</v>
+      </c>
+      <c r="L131" s="6"/>
+    </row>
+    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B132" s="5"/>
+      <c r="G132" t="s">
+        <v>128</v>
+      </c>
+      <c r="L132" s="6"/>
+    </row>
+    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B133" s="5"/>
+      <c r="H133" t="s">
+        <v>129</v>
+      </c>
+      <c r="L133" s="6"/>
+    </row>
+    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B134" s="5"/>
+      <c r="H134" t="s">
+        <v>130</v>
+      </c>
+      <c r="L134" s="6"/>
+    </row>
+    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B135" s="5"/>
+      <c r="H135" t="s">
+        <v>131</v>
+      </c>
+      <c r="L135" s="6"/>
+    </row>
+    <row r="136" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B136" s="5"/>
+      <c r="H136" t="s">
+        <v>132</v>
+      </c>
+      <c r="L136" s="6"/>
+    </row>
+    <row r="137" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B137" s="5"/>
+      <c r="G137" t="s">
+        <v>133</v>
+      </c>
+      <c r="L137" s="6"/>
+    </row>
+    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B138" s="5"/>
+      <c r="H138" t="s">
+        <v>134</v>
+      </c>
+      <c r="L138" s="6"/>
+    </row>
+    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B139" s="5"/>
+      <c r="H139" t="s">
+        <v>135</v>
+      </c>
+      <c r="L139" s="6"/>
+    </row>
+    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B140" s="5"/>
+      <c r="G140" t="s">
+        <v>136</v>
+      </c>
+      <c r="L140" s="6"/>
+    </row>
+    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B141" s="5"/>
+      <c r="G141" t="s">
+        <v>137</v>
+      </c>
+      <c r="L141" s="6"/>
+    </row>
+    <row r="142" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B142" s="5"/>
+      <c r="H142" t="s">
+        <v>138</v>
+      </c>
+      <c r="L142" s="6"/>
+    </row>
+    <row r="143" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B143" s="5"/>
+      <c r="H143" t="s">
+        <v>139</v>
+      </c>
+      <c r="L143" s="6"/>
+    </row>
+    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B144" s="5"/>
+      <c r="G144" t="s">
+        <v>140</v>
+      </c>
+      <c r="L144" s="6"/>
+    </row>
+    <row r="145" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B145" s="5"/>
+      <c r="H145" t="s">
+        <v>141</v>
+      </c>
+      <c r="L145" s="6"/>
+    </row>
+    <row r="146" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B146" s="5"/>
+      <c r="H146" t="s">
+        <v>142</v>
+      </c>
+      <c r="L146" s="6"/>
+    </row>
+    <row r="147" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B147" s="5"/>
+      <c r="H147" t="s">
+        <v>143</v>
+      </c>
+      <c r="L147" s="6"/>
+    </row>
+    <row r="148" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B148" s="5"/>
+      <c r="G148" t="s">
+        <v>144</v>
+      </c>
+      <c r="L148" s="6"/>
+    </row>
+    <row r="149" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B149" s="5"/>
+      <c r="H149" t="s">
+        <v>145</v>
+      </c>
+      <c r="L149" s="6"/>
+    </row>
+    <row r="150" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B150" s="5"/>
+      <c r="H150" t="s">
+        <v>146</v>
+      </c>
+      <c r="L150" s="6"/>
+    </row>
+    <row r="151" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B151" s="5"/>
+      <c r="H151" t="s">
+        <v>147</v>
+      </c>
+      <c r="L151" s="6"/>
+    </row>
+    <row r="152" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B152" s="5"/>
+      <c r="G152" t="s">
+        <v>148</v>
+      </c>
+      <c r="L152" s="6"/>
+    </row>
+    <row r="153" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B153" s="5"/>
+      <c r="H153" t="s">
+        <v>149</v>
+      </c>
+      <c r="L153" s="6"/>
+    </row>
+    <row r="154" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B154" s="5"/>
+      <c r="H154" t="s">
+        <v>150</v>
+      </c>
+      <c r="L154" s="6"/>
+    </row>
+    <row r="155" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B155" s="5"/>
+      <c r="H155" t="s">
+        <v>151</v>
+      </c>
+      <c r="L155" s="6"/>
+    </row>
+    <row r="156" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B156" s="5"/>
+      <c r="H156" t="s">
+        <v>152</v>
+      </c>
+      <c r="L156" s="6"/>
+    </row>
+    <row r="157" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B157" s="5"/>
+      <c r="G157" t="s">
+        <v>230</v>
+      </c>
+      <c r="L157" s="6"/>
+    </row>
+    <row r="158" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B158" s="5"/>
+      <c r="H158" t="s">
+        <v>231</v>
+      </c>
+      <c r="L158" s="6"/>
+    </row>
+    <row r="159" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B159" s="5"/>
+      <c r="H159" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="L159" s="6"/>
+      <c r="M159" t="s">
+        <v>181</v>
+      </c>
+      <c r="N159" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="160" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B160" s="5"/>
+      <c r="H160" t="s">
+        <v>233</v>
+      </c>
+      <c r="L160" s="6"/>
+    </row>
+    <row r="161" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B161" s="5"/>
+      <c r="F161" t="s">
+        <v>153</v>
+      </c>
+      <c r="L161" s="6"/>
+    </row>
+    <row r="162" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B162" s="5"/>
+      <c r="G162" t="s">
+        <v>154</v>
+      </c>
+      <c r="L162" s="6"/>
+    </row>
+    <row r="163" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B163" s="5"/>
+      <c r="F163" t="s">
+        <v>155</v>
+      </c>
+      <c r="L163" s="6"/>
+    </row>
+    <row r="164" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B164" s="5"/>
+      <c r="G164" t="s">
+        <v>156</v>
+      </c>
+      <c r="L164" s="6"/>
+    </row>
+    <row r="165" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B165" s="5"/>
+      <c r="G165" t="s">
+        <v>157</v>
+      </c>
+      <c r="L165" s="6"/>
+    </row>
+    <row r="166" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B166" s="5"/>
+      <c r="G166" t="s">
+        <v>158</v>
+      </c>
+      <c r="L166" s="6"/>
+    </row>
+    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B167" s="5"/>
+      <c r="F167" t="s">
+        <v>159</v>
+      </c>
+      <c r="L167" s="6"/>
+    </row>
+    <row r="168" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B168" s="5"/>
+      <c r="G168" t="s">
+        <v>160</v>
+      </c>
+      <c r="L168" s="6"/>
+    </row>
+    <row r="169" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B169" s="5"/>
+      <c r="H169" t="s">
+        <v>161</v>
+      </c>
+      <c r="L169" s="6"/>
+    </row>
+    <row r="170" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B170" s="5"/>
+      <c r="H170" t="s">
+        <v>162</v>
+      </c>
+      <c r="L170" s="6"/>
+    </row>
+    <row r="171" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B171" s="5"/>
+      <c r="H171" t="s">
+        <v>163</v>
+      </c>
+      <c r="L171" s="6"/>
+    </row>
+    <row r="172" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B172" s="5"/>
+      <c r="H172" t="s">
+        <v>164</v>
+      </c>
+      <c r="L172" s="6"/>
+    </row>
+    <row r="173" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B173" s="5"/>
+      <c r="G173" t="s">
+        <v>165</v>
+      </c>
+      <c r="L173" s="6"/>
+    </row>
+    <row r="174" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B174" s="5"/>
+      <c r="H174" t="s">
+        <v>166</v>
+      </c>
+      <c r="L174" s="6"/>
+    </row>
+    <row r="175" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B175" s="5"/>
+      <c r="H175" t="s">
+        <v>167</v>
+      </c>
+      <c r="L175" s="6"/>
+    </row>
+    <row r="176" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B176" s="5"/>
+      <c r="H176" t="s">
+        <v>168</v>
+      </c>
+      <c r="L176" s="6"/>
+    </row>
+    <row r="177" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B177" s="5"/>
+      <c r="H177" t="s">
+        <v>169</v>
+      </c>
+      <c r="L177" s="6"/>
+    </row>
+    <row r="178" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B178" s="5"/>
+      <c r="H178" t="s">
+        <v>170</v>
+      </c>
+      <c r="L178" s="6"/>
+    </row>
+    <row r="179" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B179" s="5"/>
+      <c r="H179" t="s">
+        <v>171</v>
+      </c>
+      <c r="L179" s="6"/>
+    </row>
+    <row r="180" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B180" s="5"/>
+      <c r="F180" t="s">
+        <v>172</v>
+      </c>
+      <c r="L180" s="6"/>
+    </row>
+    <row r="181" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B181" s="5"/>
+      <c r="G181" t="s">
+        <v>173</v>
+      </c>
+      <c r="L181" s="6"/>
+    </row>
+    <row r="182" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B182" s="5"/>
+      <c r="G182" t="s">
+        <v>174</v>
+      </c>
+      <c r="L182" s="6"/>
+    </row>
+    <row r="183" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B183" s="5"/>
+      <c r="G183" t="s">
+        <v>175</v>
+      </c>
+      <c r="L183" s="6"/>
+    </row>
+    <row r="184" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B184" s="5"/>
+      <c r="D184" t="s">
+        <v>176</v>
+      </c>
+      <c r="L184" s="6"/>
+    </row>
+    <row r="185" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B185" s="5"/>
+      <c r="C185" t="s">
+        <v>177</v>
+      </c>
+      <c r="L185" s="6"/>
+    </row>
+    <row r="186" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B186" s="5"/>
+      <c r="D186" t="s">
+        <v>207</v>
+      </c>
+      <c r="L186" s="6"/>
+    </row>
+    <row r="187" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B187" s="5"/>
+      <c r="E187" t="s">
+        <v>178</v>
+      </c>
+      <c r="L187" s="6"/>
+    </row>
+    <row r="188" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B188" s="5"/>
+      <c r="E188" t="s">
+        <v>179</v>
+      </c>
+      <c r="L188" s="6"/>
+    </row>
+    <row r="189" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B189" s="5"/>
+      <c r="D189" t="s">
+        <v>212</v>
+      </c>
+      <c r="L189" s="6"/>
+    </row>
+    <row r="190" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B190" s="5"/>
+      <c r="E190" t="s">
+        <v>178</v>
+      </c>
+      <c r="L190" s="6"/>
+    </row>
+    <row r="191" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B191" s="5"/>
+      <c r="E191" t="s">
+        <v>179</v>
+      </c>
+      <c r="L191" s="6"/>
+    </row>
+    <row r="192" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B192" s="5"/>
+      <c r="D192" t="s">
+        <v>312</v>
+      </c>
+      <c r="L192" s="6"/>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B193" s="5"/>
+      <c r="E193" t="s">
+        <v>313</v>
+      </c>
+      <c r="L193" s="6"/>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B194" s="5"/>
+      <c r="F194" t="s">
+        <v>314</v>
+      </c>
+      <c r="L194" s="6"/>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B195" s="8"/>
+      <c r="C195" s="9"/>
+      <c r="D195" s="9"/>
+      <c r="E195" s="9"/>
+      <c r="F195" s="9"/>
+      <c r="G195" s="9"/>
+      <c r="H195" s="9"/>
+      <c r="I195" s="9"/>
+      <c r="J195" s="9"/>
+      <c r="K195" s="9"/>
+      <c r="L195" s="10"/>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B199" s="12" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B233" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C233" s="3"/>
+      <c r="D233" s="3"/>
+      <c r="E233" s="3"/>
+      <c r="F233" s="3"/>
+      <c r="G233" s="3"/>
+      <c r="H233" s="3"/>
+      <c r="I233" s="3"/>
+      <c r="J233" s="3"/>
+      <c r="K233" s="4"/>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B234" s="5"/>
+      <c r="C234" s="16"/>
+      <c r="D234" s="16"/>
+      <c r="E234" s="16"/>
+      <c r="F234" s="16"/>
+      <c r="G234" s="16"/>
+      <c r="H234" s="16"/>
+      <c r="I234" s="16"/>
+      <c r="J234" s="16"/>
+      <c r="K234" s="6"/>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B235" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C235" s="16"/>
+      <c r="D235" s="16"/>
+      <c r="E235" s="16"/>
+      <c r="F235" s="16"/>
+      <c r="G235" s="16"/>
+      <c r="H235" s="16"/>
+      <c r="I235" s="16"/>
+      <c r="J235" s="16"/>
+      <c r="K235" s="6"/>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B236" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C236" s="16"/>
+      <c r="D236" s="16"/>
+      <c r="E236" s="16"/>
+      <c r="F236" s="16"/>
+      <c r="G236" s="16"/>
+      <c r="H236" s="16"/>
+      <c r="I236" s="16"/>
+      <c r="J236" s="16"/>
+      <c r="K236" s="6"/>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B237" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C237" s="16"/>
+      <c r="D237" s="16"/>
+      <c r="E237" s="16"/>
+      <c r="F237" s="16"/>
+      <c r="G237" s="16"/>
+      <c r="H237" s="16"/>
+      <c r="I237" s="16"/>
+      <c r="J237" s="16"/>
+      <c r="K237" s="6"/>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B238" s="5"/>
+      <c r="C238" s="16"/>
+      <c r="D238" s="16"/>
+      <c r="E238" s="16"/>
+      <c r="F238" s="16"/>
+      <c r="G238" s="16"/>
+      <c r="H238" s="16"/>
+      <c r="I238" s="16"/>
+      <c r="J238" s="16"/>
+      <c r="K238" s="6"/>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B239" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C239" s="16"/>
+      <c r="D239" s="16"/>
+      <c r="E239" s="16"/>
+      <c r="F239" s="16"/>
+      <c r="G239" s="16"/>
+      <c r="H239" s="16"/>
+      <c r="I239" s="16"/>
+      <c r="J239" s="16"/>
+      <c r="K239" s="6"/>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B240" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C240" s="16"/>
+      <c r="D240" s="16"/>
+      <c r="E240" s="16"/>
+      <c r="F240" s="16"/>
+      <c r="G240" s="16"/>
+      <c r="H240" s="16"/>
+      <c r="I240" s="16"/>
+      <c r="J240" s="16"/>
+      <c r="K240" s="6"/>
+    </row>
+    <row r="241" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B241" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C241" s="16"/>
+      <c r="D241" s="16"/>
+      <c r="E241" s="16"/>
+      <c r="F241" s="16"/>
+      <c r="G241" s="16"/>
+      <c r="H241" s="16"/>
+      <c r="I241" s="16"/>
+      <c r="J241" s="16"/>
+      <c r="K241" s="6"/>
+    </row>
+    <row r="242" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B242" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C242" s="16"/>
+      <c r="D242" s="16"/>
+      <c r="E242" s="16"/>
+      <c r="F242" s="16"/>
+      <c r="G242" s="16"/>
+      <c r="H242" s="16"/>
+      <c r="I242" s="16"/>
+      <c r="J242" s="16"/>
+      <c r="K242" s="6"/>
+    </row>
+    <row r="243" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B243" s="5"/>
+      <c r="C243" s="16"/>
+      <c r="D243" s="16"/>
+      <c r="E243" s="16"/>
+      <c r="F243" s="16"/>
+      <c r="G243" s="16"/>
+      <c r="H243" s="16"/>
+      <c r="I243" s="16"/>
+      <c r="J243" s="16"/>
+      <c r="K243" s="6"/>
+    </row>
+    <row r="244" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B244" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C244" s="16"/>
+      <c r="D244" s="16"/>
+      <c r="E244" s="16"/>
+      <c r="F244" s="16"/>
+      <c r="G244" s="16"/>
+      <c r="H244" s="16"/>
+      <c r="I244" s="16"/>
+      <c r="J244" s="16"/>
+      <c r="K244" s="6"/>
+    </row>
+    <row r="245" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B245" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C245" s="16"/>
+      <c r="D245" s="16"/>
+      <c r="E245" s="16"/>
+      <c r="F245" s="16"/>
+      <c r="G245" s="16"/>
+      <c r="H245" s="16"/>
+      <c r="I245" s="16"/>
+      <c r="J245" s="16"/>
+      <c r="K245" s="6"/>
+    </row>
+    <row r="246" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B246" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C246" s="16"/>
+      <c r="D246" s="16"/>
+      <c r="E246" s="16"/>
+      <c r="F246" s="16"/>
+      <c r="G246" s="16"/>
+      <c r="H246" s="16"/>
+      <c r="I246" s="16"/>
+      <c r="J246" s="16"/>
+      <c r="K246" s="6"/>
+    </row>
+    <row r="247" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B247" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C247" s="16"/>
+      <c r="D247" s="16"/>
+      <c r="E247" s="16"/>
+      <c r="F247" s="16"/>
+      <c r="G247" s="16"/>
+      <c r="H247" s="16"/>
+      <c r="I247" s="16"/>
+      <c r="J247" s="16"/>
+      <c r="K247" s="6"/>
+    </row>
+    <row r="248" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B248" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C248" s="16"/>
+      <c r="D248" s="16"/>
+      <c r="E248" s="16"/>
+      <c r="F248" s="16"/>
+      <c r="G248" s="16"/>
+      <c r="H248" s="16"/>
+      <c r="I248" s="16"/>
+      <c r="J248" s="16"/>
+      <c r="K248" s="6"/>
+    </row>
+    <row r="249" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B249" s="5"/>
+      <c r="C249" s="16"/>
+      <c r="D249" s="16"/>
+      <c r="E249" s="16"/>
+      <c r="F249" s="16"/>
+      <c r="G249" s="16"/>
+      <c r="H249" s="16"/>
+      <c r="I249" s="16"/>
+      <c r="J249" s="16"/>
+      <c r="K249" s="6"/>
+    </row>
+    <row r="250" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B250" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C250" s="16"/>
+      <c r="D250" s="16"/>
+      <c r="E250" s="16"/>
+      <c r="F250" s="16"/>
+      <c r="G250" s="16"/>
+      <c r="H250" s="16"/>
+      <c r="I250" s="16"/>
+      <c r="J250" s="16"/>
+      <c r="K250" s="6"/>
+    </row>
+    <row r="251" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B251" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C251" s="16"/>
+      <c r="D251" s="16"/>
+      <c r="E251" s="16"/>
+      <c r="F251" s="16"/>
+      <c r="G251" s="16"/>
+      <c r="H251" s="16"/>
+      <c r="I251" s="16"/>
+      <c r="J251" s="16"/>
+      <c r="K251" s="6"/>
+    </row>
+    <row r="252" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B252" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C252" s="16"/>
+      <c r="D252" s="16"/>
+      <c r="E252" s="16"/>
+      <c r="F252" s="16"/>
+      <c r="G252" s="16"/>
+      <c r="H252" s="16"/>
+      <c r="I252" s="16"/>
+      <c r="J252" s="16"/>
+      <c r="K252" s="6"/>
+    </row>
+    <row r="253" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B253" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C253" s="16"/>
+      <c r="D253" s="16"/>
+      <c r="E253" s="16"/>
+      <c r="F253" s="16"/>
+      <c r="G253" s="16"/>
+      <c r="H253" s="16"/>
+      <c r="I253" s="16"/>
+      <c r="J253" s="16"/>
+      <c r="K253" s="6"/>
+    </row>
+    <row r="254" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B254" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C254" s="16"/>
+      <c r="D254" s="16"/>
+      <c r="E254" s="16"/>
+      <c r="F254" s="16"/>
+      <c r="G254" s="16"/>
+      <c r="H254" s="16"/>
+      <c r="I254" s="16"/>
+      <c r="J254" s="16"/>
+      <c r="K254" s="6"/>
+    </row>
+    <row r="255" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B255" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="C255" s="16"/>
+      <c r="D255" s="16"/>
+      <c r="E255" s="16"/>
+      <c r="F255" s="16"/>
+      <c r="G255" s="16"/>
+      <c r="H255" s="16"/>
+      <c r="I255" s="16"/>
+      <c r="J255" s="16"/>
+      <c r="K255" s="6"/>
+    </row>
+    <row r="256" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B256" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C256" s="16"/>
+      <c r="D256" s="16"/>
+      <c r="E256" s="16"/>
+      <c r="F256" s="16"/>
+      <c r="G256" s="16"/>
+      <c r="H256" s="16"/>
+      <c r="I256" s="16"/>
+      <c r="J256" s="16"/>
+      <c r="K256" s="6"/>
+    </row>
+    <row r="257" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B257" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="C257" s="16"/>
+      <c r="D257" s="16"/>
+      <c r="E257" s="16"/>
+      <c r="F257" s="16"/>
+      <c r="G257" s="16"/>
+      <c r="H257" s="16"/>
+      <c r="I257" s="16"/>
+      <c r="J257" s="16"/>
+      <c r="K257" s="6"/>
+      <c r="L257" t="s">
+        <v>181</v>
+      </c>
+      <c r="M257" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="258" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B258" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C258" s="16"/>
+      <c r="D258" s="16"/>
+      <c r="E258" s="16"/>
+      <c r="F258" s="16"/>
+      <c r="G258" s="16"/>
+      <c r="H258" s="16"/>
+      <c r="I258" s="16"/>
+      <c r="J258" s="16"/>
+      <c r="K258" s="6"/>
+    </row>
+    <row r="259" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B259" s="5"/>
+      <c r="C259" s="16"/>
+      <c r="D259" s="16"/>
+      <c r="E259" s="16"/>
+      <c r="F259" s="16"/>
+      <c r="G259" s="16"/>
+      <c r="H259" s="16"/>
+      <c r="I259" s="16"/>
+      <c r="J259" s="16"/>
+      <c r="K259" s="6"/>
+    </row>
+    <row r="260" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B260" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C260" s="16"/>
+      <c r="D260" s="16"/>
+      <c r="E260" s="16"/>
+      <c r="F260" s="16"/>
+      <c r="G260" s="16"/>
+      <c r="H260" s="16"/>
+      <c r="I260" s="16"/>
+      <c r="J260" s="16"/>
+      <c r="K260" s="6"/>
+    </row>
+    <row r="261" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B261" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C261" s="16"/>
+      <c r="D261" s="16"/>
+      <c r="E261" s="16"/>
+      <c r="F261" s="16"/>
+      <c r="G261" s="16"/>
+      <c r="H261" s="16"/>
+      <c r="I261" s="16"/>
+      <c r="J261" s="16"/>
+      <c r="K261" s="6"/>
+    </row>
+    <row r="262" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B262" s="5"/>
+      <c r="C262" s="16"/>
+      <c r="D262" s="16"/>
+      <c r="E262" s="16"/>
+      <c r="F262" s="16"/>
+      <c r="G262" s="16"/>
+      <c r="H262" s="16"/>
+      <c r="I262" s="16"/>
+      <c r="J262" s="16"/>
+      <c r="K262" s="6"/>
+    </row>
+    <row r="263" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B263" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C263" s="16"/>
+      <c r="D263" s="16"/>
+      <c r="E263" s="16"/>
+      <c r="F263" s="16"/>
+      <c r="G263" s="16"/>
+      <c r="H263" s="16"/>
+      <c r="I263" s="16"/>
+      <c r="J263" s="16"/>
+      <c r="K263" s="6"/>
+    </row>
+    <row r="264" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B264" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="C264" s="16"/>
+      <c r="D264" s="16"/>
+      <c r="E264" s="16"/>
+      <c r="F264" s="16"/>
+      <c r="G264" s="16"/>
+      <c r="H264" s="16"/>
+      <c r="I264" s="16"/>
+      <c r="J264" s="16"/>
+      <c r="K264" s="6"/>
+    </row>
+    <row r="265" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B265" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="C265" s="16"/>
+      <c r="D265" s="16"/>
+      <c r="E265" s="16"/>
+      <c r="F265" s="16"/>
+      <c r="G265" s="16"/>
+      <c r="H265" s="16"/>
+      <c r="I265" s="16"/>
+      <c r="J265" s="16"/>
+      <c r="K265" s="6"/>
+    </row>
+    <row r="266" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B266" s="5"/>
+      <c r="C266" s="16"/>
+      <c r="D266" s="16"/>
+      <c r="E266" s="16"/>
+      <c r="F266" s="16"/>
+      <c r="G266" s="16"/>
+      <c r="H266" s="16"/>
+      <c r="I266" s="16"/>
+      <c r="J266" s="16"/>
+      <c r="K266" s="6"/>
+    </row>
+    <row r="267" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B267" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="C267" s="16"/>
+      <c r="D267" s="16"/>
+      <c r="E267" s="16"/>
+      <c r="F267" s="16"/>
+      <c r="G267" s="16"/>
+      <c r="H267" s="16"/>
+      <c r="I267" s="16"/>
+      <c r="J267" s="16"/>
+      <c r="K267" s="6"/>
+    </row>
+    <row r="268" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B268" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="C268" s="16"/>
+      <c r="D268" s="16"/>
+      <c r="E268" s="16"/>
+      <c r="F268" s="16"/>
+      <c r="G268" s="16"/>
+      <c r="H268" s="16"/>
+      <c r="I268" s="16"/>
+      <c r="J268" s="16"/>
+      <c r="K268" s="6"/>
+    </row>
+    <row r="269" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B269" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C269" s="16"/>
+      <c r="D269" s="16"/>
+      <c r="E269" s="16"/>
+      <c r="F269" s="16"/>
+      <c r="G269" s="16"/>
+      <c r="H269" s="16"/>
+      <c r="I269" s="16"/>
+      <c r="J269" s="16"/>
+      <c r="K269" s="6"/>
+    </row>
+    <row r="270" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B270" s="5"/>
+      <c r="C270" s="16"/>
+      <c r="D270" s="16"/>
+      <c r="E270" s="16"/>
+      <c r="F270" s="16"/>
+      <c r="G270" s="16"/>
+      <c r="H270" s="16"/>
+      <c r="I270" s="16"/>
+      <c r="J270" s="16"/>
+      <c r="K270" s="6"/>
+    </row>
+    <row r="271" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B271" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="C271" s="16"/>
+      <c r="D271" s="16"/>
+      <c r="E271" s="16"/>
+      <c r="F271" s="16"/>
+      <c r="G271" s="16"/>
+      <c r="H271" s="16"/>
+      <c r="I271" s="16"/>
+      <c r="J271" s="16"/>
+      <c r="K271" s="6"/>
+    </row>
+    <row r="272" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B272" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C272" s="16"/>
+      <c r="D272" s="16"/>
+      <c r="E272" s="16"/>
+      <c r="F272" s="16"/>
+      <c r="G272" s="16"/>
+      <c r="H272" s="16"/>
+      <c r="I272" s="16"/>
+      <c r="J272" s="16"/>
+      <c r="K272" s="6"/>
+    </row>
+    <row r="273" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B273" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="C273" s="16"/>
+      <c r="D273" s="16"/>
+      <c r="E273" s="16"/>
+      <c r="F273" s="16"/>
+      <c r="G273" s="16"/>
+      <c r="H273" s="16"/>
+      <c r="I273" s="16"/>
+      <c r="J273" s="16"/>
+      <c r="K273" s="6"/>
+    </row>
+    <row r="274" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B274" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C274" s="16"/>
+      <c r="D274" s="16"/>
+      <c r="E274" s="16"/>
+      <c r="F274" s="16"/>
+      <c r="G274" s="16"/>
+      <c r="H274" s="16"/>
+      <c r="I274" s="16"/>
+      <c r="J274" s="16"/>
+      <c r="K274" s="6"/>
+    </row>
+    <row r="275" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B275" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C275" s="16"/>
+      <c r="D275" s="16"/>
+      <c r="E275" s="16"/>
+      <c r="F275" s="16"/>
+      <c r="G275" s="16"/>
+      <c r="H275" s="16"/>
+      <c r="I275" s="16"/>
+      <c r="J275" s="16"/>
+      <c r="K275" s="6"/>
+    </row>
+    <row r="276" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B276" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="C276" s="16"/>
+      <c r="D276" s="16"/>
+      <c r="E276" s="16"/>
+      <c r="F276" s="16"/>
+      <c r="G276" s="16"/>
+      <c r="H276" s="16"/>
+      <c r="I276" s="16"/>
+      <c r="J276" s="16"/>
+      <c r="K276" s="6"/>
+    </row>
+    <row r="277" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B277" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C277" s="16"/>
+      <c r="D277" s="16"/>
+      <c r="E277" s="16"/>
+      <c r="F277" s="16"/>
+      <c r="G277" s="16"/>
+      <c r="H277" s="16"/>
+      <c r="I277" s="16"/>
+      <c r="J277" s="16"/>
+      <c r="K277" s="6"/>
+      <c r="L277" t="s">
+        <v>181</v>
+      </c>
+      <c r="M277" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="278" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B278" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="C278" s="16"/>
+      <c r="D278" s="16"/>
+      <c r="E278" s="16"/>
+      <c r="F278" s="16"/>
+      <c r="G278" s="16"/>
+      <c r="H278" s="16"/>
+      <c r="I278" s="16"/>
+      <c r="J278" s="16"/>
+      <c r="K278" s="6"/>
+    </row>
+    <row r="279" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B279" s="5"/>
+      <c r="C279" s="16"/>
+      <c r="D279" s="16"/>
+      <c r="E279" s="16"/>
+      <c r="F279" s="16"/>
+      <c r="G279" s="16"/>
+      <c r="H279" s="16"/>
+      <c r="I279" s="16"/>
+      <c r="J279" s="16"/>
+      <c r="K279" s="6"/>
+    </row>
+    <row r="280" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B280" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C280" s="16"/>
+      <c r="D280" s="16"/>
+      <c r="E280" s="16"/>
+      <c r="F280" s="16"/>
+      <c r="G280" s="16"/>
+      <c r="H280" s="16"/>
+      <c r="I280" s="16"/>
+      <c r="J280" s="16"/>
+      <c r="K280" s="6"/>
+    </row>
+    <row r="281" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B281" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="C281" s="16"/>
+      <c r="D281" s="16"/>
+      <c r="E281" s="16"/>
+      <c r="F281" s="16"/>
+      <c r="G281" s="16"/>
+      <c r="H281" s="16"/>
+      <c r="I281" s="16"/>
+      <c r="J281" s="16"/>
+      <c r="K281" s="6"/>
+    </row>
+    <row r="282" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B282" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C282" s="16"/>
+      <c r="D282" s="16"/>
+      <c r="E282" s="16"/>
+      <c r="F282" s="16"/>
+      <c r="G282" s="16"/>
+      <c r="H282" s="16"/>
+      <c r="I282" s="16"/>
+      <c r="J282" s="16"/>
+      <c r="K282" s="6"/>
+    </row>
+    <row r="283" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B283" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="C283" s="16"/>
+      <c r="D283" s="16"/>
+      <c r="E283" s="16"/>
+      <c r="F283" s="16"/>
+      <c r="G283" s="16"/>
+      <c r="H283" s="16"/>
+      <c r="I283" s="16"/>
+      <c r="J283" s="16"/>
+      <c r="K283" s="6"/>
+    </row>
+    <row r="284" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B284" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="C284" s="16"/>
+      <c r="D284" s="16"/>
+      <c r="E284" s="16"/>
+      <c r="F284" s="16"/>
+      <c r="G284" s="16"/>
+      <c r="H284" s="16"/>
+      <c r="I284" s="16"/>
+      <c r="J284" s="16"/>
+      <c r="K284" s="6"/>
+    </row>
+    <row r="285" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B285" s="5"/>
+      <c r="C285" s="16"/>
+      <c r="D285" s="16"/>
+      <c r="E285" s="16"/>
+      <c r="F285" s="16"/>
+      <c r="G285" s="16"/>
+      <c r="H285" s="16"/>
+      <c r="I285" s="16"/>
+      <c r="J285" s="16"/>
+      <c r="K285" s="6"/>
+    </row>
+    <row r="286" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B286" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="C286" s="16"/>
+      <c r="D286" s="16"/>
+      <c r="E286" s="16"/>
+      <c r="F286" s="16"/>
+      <c r="G286" s="16"/>
+      <c r="H286" s="16"/>
+      <c r="I286" s="16"/>
+      <c r="J286" s="16"/>
+      <c r="K286" s="6"/>
+    </row>
+    <row r="287" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B287" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="C287" s="16"/>
+      <c r="D287" s="16"/>
+      <c r="E287" s="16"/>
+      <c r="F287" s="16"/>
+      <c r="G287" s="16"/>
+      <c r="H287" s="16"/>
+      <c r="I287" s="16"/>
+      <c r="J287" s="16"/>
+      <c r="K287" s="6"/>
+    </row>
+    <row r="288" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B288" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="C288" s="16"/>
+      <c r="D288" s="16"/>
+      <c r="E288" s="16"/>
+      <c r="F288" s="16"/>
+      <c r="G288" s="16"/>
+      <c r="H288" s="16"/>
+      <c r="I288" s="16"/>
+      <c r="J288" s="16"/>
+      <c r="K288" s="6"/>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B289" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="C289" s="16"/>
+      <c r="D289" s="16"/>
+      <c r="E289" s="16"/>
+      <c r="F289" s="16"/>
+      <c r="G289" s="16"/>
+      <c r="H289" s="16"/>
+      <c r="I289" s="16"/>
+      <c r="J289" s="16"/>
+      <c r="K289" s="6"/>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B290" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="C290" s="16"/>
+      <c r="D290" s="16"/>
+      <c r="E290" s="16"/>
+      <c r="F290" s="16"/>
+      <c r="G290" s="16"/>
+      <c r="H290" s="16"/>
+      <c r="I290" s="16"/>
+      <c r="J290" s="16"/>
+      <c r="K290" s="6"/>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B291" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C291" s="16"/>
+      <c r="D291" s="16"/>
+      <c r="E291" s="16"/>
+      <c r="F291" s="16"/>
+      <c r="G291" s="16"/>
+      <c r="H291" s="16"/>
+      <c r="I291" s="16"/>
+      <c r="J291" s="16"/>
+      <c r="K291" s="6"/>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B292" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C292" s="16"/>
+      <c r="D292" s="16"/>
+      <c r="E292" s="16"/>
+      <c r="F292" s="16"/>
+      <c r="G292" s="16"/>
+      <c r="H292" s="16"/>
+      <c r="I292" s="16"/>
+      <c r="J292" s="16"/>
+      <c r="K292" s="6"/>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B293" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C293" s="16"/>
+      <c r="D293" s="16"/>
+      <c r="E293" s="16"/>
+      <c r="F293" s="16"/>
+      <c r="G293" s="16"/>
+      <c r="H293" s="16"/>
+      <c r="I293" s="16"/>
+      <c r="J293" s="16"/>
+      <c r="K293" s="6"/>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B294" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C294" s="16"/>
+      <c r="D294" s="16"/>
+      <c r="E294" s="16"/>
+      <c r="F294" s="16"/>
+      <c r="G294" s="16"/>
+      <c r="H294" s="16"/>
+      <c r="I294" s="16"/>
+      <c r="J294" s="16"/>
+      <c r="K294" s="6"/>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B295" s="5"/>
+      <c r="C295" s="16"/>
+      <c r="D295" s="16"/>
+      <c r="E295" s="16"/>
+      <c r="F295" s="16"/>
+      <c r="G295" s="16"/>
+      <c r="H295" s="16"/>
+      <c r="I295" s="16"/>
+      <c r="J295" s="16"/>
+      <c r="K295" s="6"/>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B296" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C296" s="16"/>
+      <c r="D296" s="16"/>
+      <c r="E296" s="16"/>
+      <c r="F296" s="16"/>
+      <c r="G296" s="16"/>
+      <c r="H296" s="16"/>
+      <c r="I296" s="16"/>
+      <c r="J296" s="16"/>
+      <c r="K296" s="6"/>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B297" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="C297" s="16"/>
+      <c r="D297" s="16"/>
+      <c r="E297" s="16"/>
+      <c r="F297" s="16"/>
+      <c r="G297" s="16"/>
+      <c r="H297" s="16"/>
+      <c r="I297" s="16"/>
+      <c r="J297" s="16"/>
+      <c r="K297" s="6"/>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B298" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C298" s="16"/>
+      <c r="D298" s="16"/>
+      <c r="E298" s="16"/>
+      <c r="F298" s="16"/>
+      <c r="G298" s="16"/>
+      <c r="H298" s="16"/>
+      <c r="I298" s="16"/>
+      <c r="J298" s="16"/>
+      <c r="K298" s="6"/>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B299" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="C299" s="9"/>
+      <c r="D299" s="9"/>
+      <c r="E299" s="9"/>
+      <c r="F299" s="9"/>
+      <c r="G299" s="9"/>
+      <c r="H299" s="9"/>
+      <c r="I299" s="9"/>
+      <c r="J299" s="9"/>
+      <c r="K299" s="10"/>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A302" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Lightning Tab - Add LWC as a Custom Tab
</commit_message>
<xml_diff>
--- a/me/13.Year-2021-Updates.xlsx
+++ b/me/13.Year-2021-Updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\LightningWebComponent\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08E7BDF-E171-4BF2-B309-A84947BEA755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5E0D55-060A-4A18-8362-33AFF00A0CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets in Javascript" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="ParseAndFormatTheCalloutRespons" sheetId="5" r:id="rId5"/>
     <sheet name="FinishFormattingtheCalloutRespo" sheetId="6" r:id="rId6"/>
     <sheet name="Stylise Lightning Datatable" sheetId="7" r:id="rId7"/>
+    <sheet name="Add LWC as a Custom Tab" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1939" uniqueCount="431">
   <si>
     <t>構成</t>
   </si>
@@ -1564,6 +1565,52 @@
       </rPr>
       <t xml:space="preserve"> atribute with custom class</t>
     </r>
+  </si>
+  <si>
+    <t>Lightning Tab - Add LWC as a Custom Tab</t>
+  </si>
+  <si>
+    <t>Add component in the utility bar of Salesforce application</t>
+  </si>
+  <si>
+    <t>https://developer.salesforce.com/docs/component-library/documentation/en/lwc/lwc.reference_configuration_tags</t>
+  </si>
+  <si>
+    <t>    &lt;isExposed&gt;true&lt;/isExposed&gt;</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Make it comes after </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Home</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tab</t>
+    </r>
+  </si>
+  <si>
+    <t>Open Sales</t>
+  </si>
+  <si>
+    <t>App</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1710,6 +1757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3506,6 +3554,566 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>312964</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>30336</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58E69C66-705D-FAAD-30CA-BDA5218E101E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="736146" y="1228726"/>
+          <a:ext cx="11210925" cy="5278610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>239</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD346F0D-958C-17F2-9628-4FE602365B08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2143125" y="4362450"/>
+          <a:ext cx="2552700" cy="4267200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>139513</xdr:colOff>
+      <xdr:row>245</xdr:row>
+      <xdr:rowOff>132230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>14161</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CEC59FF-C7C9-C9DB-6D0D-4DFB388ABFE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="744631" y="9657230"/>
+          <a:ext cx="10943104" cy="5406431"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>100854</xdr:colOff>
+      <xdr:row>275</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>303</xdr:row>
+      <xdr:rowOff>69418</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D64F7019-6B4B-4232-2EA6-C1DEB3202CCB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="705972" y="52342677"/>
+          <a:ext cx="10981764" cy="5257741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>304</xdr:row>
+      <xdr:rowOff>100854</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>392206</xdr:colOff>
+      <xdr:row>334</xdr:row>
+      <xdr:rowOff>18524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{514968B0-20B6-CB4C-B5A5-1DA3BCB3DA32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="705971" y="58012854"/>
+          <a:ext cx="11183470" cy="5632670"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>89647</xdr:colOff>
+      <xdr:row>337</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>347383</xdr:colOff>
+      <xdr:row>366</xdr:row>
+      <xdr:rowOff>29802</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB69AA72-376D-B5F7-F822-06890FA3F461}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="694765" y="63907148"/>
+          <a:ext cx="11149853" cy="5464654"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>367</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>358589</xdr:colOff>
+      <xdr:row>396</xdr:row>
+      <xdr:rowOff>110057</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA90606A-72A5-E255-6305-704D22219A54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="739588" y="69633353"/>
+          <a:ext cx="11116236" cy="5533704"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123265</xdr:colOff>
+      <xdr:row>399</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>358589</xdr:colOff>
+      <xdr:row>428</xdr:row>
+      <xdr:rowOff>185891</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B716DA9-3390-8F3A-C128-3C526B6626ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="728383" y="75718148"/>
+          <a:ext cx="11127441" cy="5620743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>414618</xdr:colOff>
+      <xdr:row>398</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>416</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B4065FD-E7D0-6BC4-F633-551C56DE51F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2229971" y="75594882"/>
+          <a:ext cx="7687235" cy="3406589"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>425823</xdr:colOff>
+      <xdr:row>398</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>280147</xdr:colOff>
+      <xdr:row>411</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2151AE49-666D-54C2-5477-B5342283FC79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2241176" y="75594882"/>
+          <a:ext cx="4695265" cy="2319618"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>112059</xdr:colOff>
+      <xdr:row>431</xdr:row>
+      <xdr:rowOff>134472</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>448236</xdr:colOff>
+      <xdr:row>460</xdr:row>
+      <xdr:rowOff>100822</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C848B805-4394-C709-83E0-B1674CAC39F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="717177" y="81858972"/>
+          <a:ext cx="11228294" cy="5490850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>461</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>403412</xdr:colOff>
+      <xdr:row>489</xdr:row>
+      <xdr:rowOff>3601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5DE5233-2F5E-3760-BFE9-088BAEA68A20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="705971" y="87540353"/>
+          <a:ext cx="11194676" cy="5236748"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -14326,1241 +14934,238 @@
     </row>
     <row r="314" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B314" s="5"/>
-      <c r="C314" s="16"/>
-      <c r="D314" s="16"/>
-      <c r="E314" s="16"/>
-      <c r="F314" s="16"/>
-      <c r="G314" s="16"/>
-      <c r="H314" s="16"/>
-      <c r="I314" s="16"/>
-      <c r="J314" s="16"/>
-      <c r="K314" s="16"/>
-      <c r="L314" s="16"/>
-      <c r="M314" s="16"/>
-      <c r="N314" s="16"/>
-      <c r="O314" s="16"/>
-      <c r="P314" s="16"/>
-      <c r="Q314" s="16"/>
-      <c r="R314" s="16"/>
-      <c r="S314" s="16"/>
       <c r="T314" s="6"/>
     </row>
     <row r="315" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B315" s="5"/>
-      <c r="C315" s="16"/>
-      <c r="D315" s="16"/>
-      <c r="E315" s="16"/>
-      <c r="F315" s="16"/>
-      <c r="G315" s="16"/>
-      <c r="H315" s="16"/>
-      <c r="I315" s="16"/>
-      <c r="J315" s="16"/>
-      <c r="K315" s="16"/>
-      <c r="L315" s="16"/>
-      <c r="M315" s="16"/>
-      <c r="N315" s="16"/>
-      <c r="O315" s="16"/>
-      <c r="P315" s="16"/>
-      <c r="Q315" s="16"/>
-      <c r="R315" s="16"/>
-      <c r="S315" s="16"/>
       <c r="T315" s="6"/>
     </row>
     <row r="316" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B316" s="5"/>
-      <c r="C316" s="16"/>
-      <c r="D316" s="16"/>
-      <c r="E316" s="16"/>
-      <c r="F316" s="16"/>
-      <c r="G316" s="16"/>
-      <c r="H316" s="16"/>
-      <c r="I316" s="16"/>
-      <c r="J316" s="16"/>
-      <c r="K316" s="16"/>
-      <c r="L316" s="16"/>
-      <c r="M316" s="16"/>
-      <c r="N316" s="16"/>
-      <c r="O316" s="16"/>
-      <c r="P316" s="16"/>
-      <c r="Q316" s="16"/>
-      <c r="R316" s="16"/>
-      <c r="S316" s="16"/>
       <c r="T316" s="6"/>
     </row>
     <row r="317" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B317" s="5"/>
-      <c r="C317" s="16"/>
-      <c r="D317" s="16"/>
-      <c r="E317" s="16"/>
-      <c r="F317" s="16"/>
-      <c r="G317" s="16"/>
-      <c r="H317" s="16"/>
-      <c r="I317" s="16"/>
-      <c r="J317" s="16"/>
-      <c r="K317" s="16"/>
-      <c r="L317" s="16"/>
-      <c r="M317" s="16"/>
-      <c r="N317" s="16"/>
-      <c r="O317" s="16"/>
-      <c r="P317" s="16"/>
-      <c r="Q317" s="16"/>
-      <c r="R317" s="16"/>
-      <c r="S317" s="16"/>
       <c r="T317" s="6"/>
     </row>
     <row r="318" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B318" s="5"/>
-      <c r="C318" s="16"/>
-      <c r="D318" s="16"/>
-      <c r="E318" s="16"/>
-      <c r="F318" s="16"/>
-      <c r="G318" s="16"/>
-      <c r="H318" s="16"/>
-      <c r="I318" s="16"/>
-      <c r="J318" s="16"/>
-      <c r="K318" s="16"/>
-      <c r="L318" s="16"/>
-      <c r="M318" s="16"/>
-      <c r="N318" s="16"/>
-      <c r="O318" s="16"/>
-      <c r="P318" s="16"/>
-      <c r="Q318" s="16"/>
-      <c r="R318" s="16"/>
-      <c r="S318" s="16"/>
       <c r="T318" s="6"/>
     </row>
     <row r="319" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B319" s="5"/>
-      <c r="C319" s="16"/>
-      <c r="D319" s="16"/>
-      <c r="E319" s="16"/>
-      <c r="F319" s="16"/>
-      <c r="G319" s="16"/>
-      <c r="H319" s="16"/>
-      <c r="I319" s="16"/>
-      <c r="J319" s="16"/>
-      <c r="K319" s="16"/>
-      <c r="L319" s="16"/>
-      <c r="M319" s="16"/>
-      <c r="N319" s="16"/>
-      <c r="O319" s="16"/>
-      <c r="P319" s="16"/>
-      <c r="Q319" s="16"/>
-      <c r="R319" s="16"/>
-      <c r="S319" s="16"/>
       <c r="T319" s="6"/>
     </row>
     <row r="320" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B320" s="5"/>
-      <c r="C320" s="16"/>
-      <c r="D320" s="16"/>
-      <c r="E320" s="16"/>
-      <c r="F320" s="16"/>
-      <c r="G320" s="16"/>
-      <c r="H320" s="16"/>
-      <c r="I320" s="16"/>
-      <c r="J320" s="16"/>
-      <c r="K320" s="16"/>
-      <c r="L320" s="16"/>
-      <c r="M320" s="16"/>
-      <c r="N320" s="16"/>
-      <c r="O320" s="16"/>
-      <c r="P320" s="16"/>
-      <c r="Q320" s="16"/>
-      <c r="R320" s="16"/>
-      <c r="S320" s="16"/>
       <c r="T320" s="6"/>
     </row>
     <row r="321" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B321" s="5"/>
-      <c r="C321" s="16"/>
-      <c r="D321" s="16"/>
-      <c r="E321" s="16"/>
-      <c r="F321" s="16"/>
-      <c r="G321" s="16"/>
-      <c r="H321" s="16"/>
-      <c r="I321" s="16"/>
-      <c r="J321" s="16"/>
-      <c r="K321" s="16"/>
-      <c r="L321" s="16"/>
-      <c r="M321" s="16"/>
-      <c r="N321" s="16"/>
-      <c r="O321" s="16"/>
-      <c r="P321" s="16"/>
-      <c r="Q321" s="16"/>
-      <c r="R321" s="16"/>
-      <c r="S321" s="16"/>
       <c r="T321" s="6"/>
     </row>
     <row r="322" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B322" s="5"/>
-      <c r="C322" s="16"/>
-      <c r="D322" s="16"/>
-      <c r="E322" s="16"/>
-      <c r="F322" s="16"/>
-      <c r="G322" s="16"/>
-      <c r="H322" s="16"/>
-      <c r="I322" s="16"/>
-      <c r="J322" s="16"/>
-      <c r="K322" s="16"/>
-      <c r="L322" s="16"/>
-      <c r="M322" s="16"/>
-      <c r="N322" s="16"/>
-      <c r="O322" s="16"/>
-      <c r="P322" s="16"/>
-      <c r="Q322" s="16"/>
-      <c r="R322" s="16"/>
-      <c r="S322" s="16"/>
       <c r="T322" s="6"/>
     </row>
     <row r="323" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B323" s="5"/>
-      <c r="C323" s="16"/>
-      <c r="D323" s="16"/>
-      <c r="E323" s="16"/>
-      <c r="F323" s="16"/>
-      <c r="G323" s="16"/>
-      <c r="H323" s="16"/>
-      <c r="I323" s="16"/>
-      <c r="J323" s="16"/>
-      <c r="K323" s="16"/>
-      <c r="L323" s="16"/>
-      <c r="M323" s="16"/>
-      <c r="N323" s="16"/>
-      <c r="O323" s="16"/>
-      <c r="P323" s="16"/>
-      <c r="Q323" s="16"/>
-      <c r="R323" s="16"/>
-      <c r="S323" s="16"/>
       <c r="T323" s="6"/>
     </row>
     <row r="324" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B324" s="5"/>
-      <c r="C324" s="16"/>
-      <c r="D324" s="16"/>
-      <c r="E324" s="16"/>
-      <c r="F324" s="16"/>
-      <c r="G324" s="16"/>
-      <c r="H324" s="16"/>
-      <c r="I324" s="16"/>
-      <c r="J324" s="16"/>
-      <c r="K324" s="16"/>
-      <c r="L324" s="16"/>
-      <c r="M324" s="16"/>
-      <c r="N324" s="16"/>
-      <c r="O324" s="16"/>
-      <c r="P324" s="16"/>
-      <c r="Q324" s="16"/>
-      <c r="R324" s="16"/>
-      <c r="S324" s="16"/>
       <c r="T324" s="6"/>
     </row>
     <row r="325" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B325" s="5"/>
-      <c r="C325" s="16"/>
-      <c r="D325" s="16"/>
-      <c r="E325" s="16"/>
-      <c r="F325" s="16"/>
-      <c r="G325" s="16"/>
-      <c r="H325" s="16"/>
-      <c r="I325" s="16"/>
-      <c r="J325" s="16"/>
-      <c r="K325" s="16"/>
-      <c r="L325" s="16"/>
-      <c r="M325" s="16"/>
-      <c r="N325" s="16"/>
-      <c r="O325" s="16"/>
-      <c r="P325" s="16"/>
-      <c r="Q325" s="16"/>
-      <c r="R325" s="16"/>
-      <c r="S325" s="16"/>
       <c r="T325" s="6"/>
     </row>
     <row r="326" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B326" s="5"/>
-      <c r="C326" s="16"/>
-      <c r="D326" s="16"/>
-      <c r="E326" s="16"/>
-      <c r="F326" s="16"/>
-      <c r="G326" s="16"/>
-      <c r="H326" s="16"/>
-      <c r="I326" s="16"/>
-      <c r="J326" s="16"/>
-      <c r="K326" s="16"/>
-      <c r="L326" s="16"/>
-      <c r="M326" s="16"/>
-      <c r="N326" s="16"/>
-      <c r="O326" s="16"/>
-      <c r="P326" s="16"/>
-      <c r="Q326" s="16"/>
-      <c r="R326" s="16"/>
-      <c r="S326" s="16"/>
       <c r="T326" s="6"/>
     </row>
     <row r="327" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B327" s="5"/>
-      <c r="C327" s="16"/>
-      <c r="D327" s="16"/>
-      <c r="E327" s="16"/>
-      <c r="F327" s="16"/>
-      <c r="G327" s="16"/>
-      <c r="H327" s="16"/>
-      <c r="I327" s="16"/>
-      <c r="J327" s="16"/>
-      <c r="K327" s="16"/>
-      <c r="L327" s="16"/>
-      <c r="M327" s="16"/>
-      <c r="N327" s="16"/>
-      <c r="O327" s="16"/>
-      <c r="P327" s="16"/>
-      <c r="Q327" s="16"/>
-      <c r="R327" s="16"/>
-      <c r="S327" s="16"/>
       <c r="T327" s="6"/>
     </row>
     <row r="328" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B328" s="5"/>
-      <c r="C328" s="16"/>
-      <c r="D328" s="16"/>
-      <c r="E328" s="16"/>
-      <c r="F328" s="16"/>
-      <c r="G328" s="16"/>
-      <c r="H328" s="16"/>
-      <c r="I328" s="16"/>
-      <c r="J328" s="16"/>
-      <c r="K328" s="16"/>
-      <c r="L328" s="16"/>
-      <c r="M328" s="16"/>
-      <c r="N328" s="16"/>
-      <c r="O328" s="16"/>
-      <c r="P328" s="16"/>
-      <c r="Q328" s="16"/>
-      <c r="R328" s="16"/>
-      <c r="S328" s="16"/>
       <c r="T328" s="6"/>
     </row>
     <row r="329" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B329" s="5"/>
-      <c r="C329" s="16"/>
-      <c r="D329" s="16"/>
-      <c r="E329" s="16"/>
-      <c r="F329" s="16"/>
-      <c r="G329" s="16"/>
-      <c r="H329" s="16"/>
-      <c r="I329" s="16"/>
-      <c r="J329" s="16"/>
-      <c r="K329" s="16"/>
-      <c r="L329" s="16"/>
-      <c r="M329" s="16"/>
-      <c r="N329" s="16"/>
-      <c r="O329" s="16"/>
-      <c r="P329" s="16"/>
-      <c r="Q329" s="16"/>
-      <c r="R329" s="16"/>
-      <c r="S329" s="16"/>
       <c r="T329" s="6"/>
     </row>
     <row r="330" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B330" s="5"/>
-      <c r="C330" s="16"/>
-      <c r="D330" s="16"/>
-      <c r="E330" s="16"/>
-      <c r="F330" s="16"/>
-      <c r="G330" s="16"/>
-      <c r="H330" s="16"/>
-      <c r="I330" s="16"/>
-      <c r="J330" s="16"/>
-      <c r="K330" s="16"/>
-      <c r="L330" s="16"/>
-      <c r="M330" s="16"/>
-      <c r="N330" s="16"/>
-      <c r="O330" s="16"/>
-      <c r="P330" s="16"/>
-      <c r="Q330" s="16"/>
-      <c r="R330" s="16"/>
-      <c r="S330" s="16"/>
       <c r="T330" s="6"/>
     </row>
     <row r="331" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B331" s="5"/>
-      <c r="C331" s="16"/>
-      <c r="D331" s="16"/>
-      <c r="E331" s="16"/>
-      <c r="F331" s="16"/>
-      <c r="G331" s="16"/>
-      <c r="H331" s="16"/>
-      <c r="I331" s="16"/>
-      <c r="J331" s="16"/>
-      <c r="K331" s="16"/>
-      <c r="L331" s="16"/>
-      <c r="M331" s="16"/>
-      <c r="N331" s="16"/>
-      <c r="O331" s="16"/>
-      <c r="P331" s="16"/>
-      <c r="Q331" s="16"/>
-      <c r="R331" s="16"/>
-      <c r="S331" s="16"/>
       <c r="T331" s="6"/>
     </row>
     <row r="332" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B332" s="5"/>
-      <c r="C332" s="16"/>
-      <c r="D332" s="16"/>
-      <c r="E332" s="16"/>
-      <c r="F332" s="16"/>
-      <c r="G332" s="16"/>
-      <c r="H332" s="16"/>
-      <c r="I332" s="16"/>
-      <c r="J332" s="16"/>
-      <c r="K332" s="16"/>
-      <c r="L332" s="16"/>
-      <c r="M332" s="16"/>
-      <c r="N332" s="16"/>
-      <c r="O332" s="16"/>
-      <c r="P332" s="16"/>
-      <c r="Q332" s="16"/>
-      <c r="R332" s="16"/>
-      <c r="S332" s="16"/>
       <c r="T332" s="6"/>
     </row>
     <row r="333" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B333" s="5"/>
-      <c r="C333" s="16"/>
-      <c r="D333" s="16"/>
-      <c r="E333" s="16"/>
-      <c r="F333" s="16"/>
-      <c r="G333" s="16"/>
-      <c r="H333" s="16"/>
-      <c r="I333" s="16"/>
-      <c r="J333" s="16"/>
-      <c r="K333" s="16"/>
-      <c r="L333" s="16"/>
-      <c r="M333" s="16"/>
-      <c r="N333" s="16"/>
-      <c r="O333" s="16"/>
-      <c r="P333" s="16"/>
-      <c r="Q333" s="16"/>
-      <c r="R333" s="16"/>
-      <c r="S333" s="16"/>
       <c r="T333" s="6"/>
     </row>
     <row r="334" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B334" s="5"/>
-      <c r="C334" s="16"/>
-      <c r="D334" s="16"/>
-      <c r="E334" s="16"/>
-      <c r="F334" s="16"/>
-      <c r="G334" s="16"/>
-      <c r="H334" s="16"/>
-      <c r="I334" s="16"/>
-      <c r="J334" s="16"/>
-      <c r="K334" s="16"/>
-      <c r="L334" s="16"/>
-      <c r="M334" s="16"/>
-      <c r="N334" s="16"/>
-      <c r="O334" s="16"/>
-      <c r="P334" s="16"/>
-      <c r="Q334" s="16"/>
-      <c r="R334" s="16"/>
-      <c r="S334" s="16"/>
       <c r="T334" s="6"/>
     </row>
     <row r="335" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B335" s="5"/>
-      <c r="C335" s="16"/>
-      <c r="D335" s="16"/>
-      <c r="E335" s="16"/>
-      <c r="F335" s="16"/>
-      <c r="G335" s="16"/>
-      <c r="H335" s="16"/>
-      <c r="I335" s="16"/>
-      <c r="J335" s="16"/>
-      <c r="K335" s="16"/>
-      <c r="L335" s="16"/>
-      <c r="M335" s="16"/>
-      <c r="N335" s="16"/>
-      <c r="O335" s="16"/>
-      <c r="P335" s="16"/>
-      <c r="Q335" s="16"/>
-      <c r="R335" s="16"/>
-      <c r="S335" s="16"/>
       <c r="T335" s="6"/>
     </row>
     <row r="336" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B336" s="5"/>
-      <c r="C336" s="16"/>
-      <c r="D336" s="16"/>
-      <c r="E336" s="16"/>
-      <c r="F336" s="16"/>
-      <c r="G336" s="16"/>
-      <c r="H336" s="16"/>
-      <c r="I336" s="16"/>
-      <c r="J336" s="16"/>
-      <c r="K336" s="16"/>
-      <c r="L336" s="16"/>
-      <c r="M336" s="16"/>
-      <c r="N336" s="16"/>
-      <c r="O336" s="16"/>
-      <c r="P336" s="16"/>
-      <c r="Q336" s="16"/>
-      <c r="R336" s="16"/>
-      <c r="S336" s="16"/>
       <c r="T336" s="6"/>
     </row>
     <row r="337" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B337" s="5"/>
-      <c r="C337" s="16"/>
-      <c r="D337" s="16"/>
-      <c r="E337" s="16"/>
-      <c r="F337" s="16"/>
-      <c r="G337" s="16"/>
-      <c r="H337" s="16"/>
-      <c r="I337" s="16"/>
-      <c r="J337" s="16"/>
-      <c r="K337" s="16"/>
-      <c r="L337" s="16"/>
-      <c r="M337" s="16"/>
-      <c r="N337" s="16"/>
-      <c r="O337" s="16"/>
-      <c r="P337" s="16"/>
-      <c r="Q337" s="16"/>
-      <c r="R337" s="16"/>
-      <c r="S337" s="16"/>
       <c r="T337" s="6"/>
     </row>
     <row r="338" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B338" s="5"/>
-      <c r="C338" s="16"/>
-      <c r="D338" s="16"/>
-      <c r="E338" s="16"/>
-      <c r="F338" s="16"/>
-      <c r="G338" s="16"/>
-      <c r="H338" s="16"/>
-      <c r="I338" s="16"/>
-      <c r="J338" s="16"/>
-      <c r="K338" s="16"/>
-      <c r="L338" s="16"/>
-      <c r="M338" s="16"/>
-      <c r="N338" s="16"/>
-      <c r="O338" s="16"/>
-      <c r="P338" s="16"/>
-      <c r="Q338" s="16"/>
-      <c r="R338" s="16"/>
-      <c r="S338" s="16"/>
       <c r="T338" s="6"/>
     </row>
     <row r="339" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B339" s="5"/>
-      <c r="C339" s="16"/>
-      <c r="D339" s="16"/>
-      <c r="E339" s="16"/>
-      <c r="F339" s="16"/>
-      <c r="G339" s="16"/>
-      <c r="H339" s="16"/>
-      <c r="I339" s="16"/>
-      <c r="J339" s="16"/>
-      <c r="K339" s="16"/>
-      <c r="L339" s="16"/>
-      <c r="M339" s="16"/>
-      <c r="N339" s="16"/>
-      <c r="O339" s="16"/>
-      <c r="P339" s="16"/>
-      <c r="Q339" s="16"/>
-      <c r="R339" s="16"/>
-      <c r="S339" s="16"/>
       <c r="T339" s="6"/>
     </row>
     <row r="340" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B340" s="5"/>
-      <c r="C340" s="16"/>
-      <c r="D340" s="16"/>
-      <c r="E340" s="16"/>
-      <c r="F340" s="16"/>
-      <c r="G340" s="16"/>
-      <c r="H340" s="16"/>
-      <c r="I340" s="16"/>
-      <c r="J340" s="16"/>
-      <c r="K340" s="16"/>
-      <c r="L340" s="16"/>
-      <c r="M340" s="16"/>
-      <c r="N340" s="16"/>
-      <c r="O340" s="16"/>
-      <c r="P340" s="16"/>
-      <c r="Q340" s="16"/>
-      <c r="R340" s="16"/>
-      <c r="S340" s="16"/>
       <c r="T340" s="6"/>
     </row>
     <row r="341" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B341" s="5"/>
-      <c r="C341" s="16"/>
-      <c r="D341" s="16"/>
-      <c r="E341" s="16"/>
-      <c r="F341" s="16"/>
-      <c r="G341" s="16"/>
-      <c r="H341" s="16"/>
-      <c r="I341" s="16"/>
-      <c r="J341" s="16"/>
-      <c r="K341" s="16"/>
-      <c r="L341" s="16"/>
-      <c r="M341" s="16"/>
-      <c r="N341" s="16"/>
-      <c r="O341" s="16"/>
-      <c r="P341" s="16"/>
-      <c r="Q341" s="16"/>
-      <c r="R341" s="16"/>
-      <c r="S341" s="16"/>
       <c r="T341" s="6"/>
     </row>
     <row r="342" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B342" s="5"/>
-      <c r="C342" s="16"/>
-      <c r="D342" s="16"/>
-      <c r="E342" s="16"/>
-      <c r="F342" s="16"/>
-      <c r="G342" s="16"/>
-      <c r="H342" s="16"/>
-      <c r="I342" s="16"/>
-      <c r="J342" s="16"/>
-      <c r="K342" s="16"/>
-      <c r="L342" s="16"/>
-      <c r="M342" s="16"/>
-      <c r="N342" s="16"/>
-      <c r="O342" s="16"/>
-      <c r="P342" s="16"/>
-      <c r="Q342" s="16"/>
-      <c r="R342" s="16"/>
-      <c r="S342" s="16"/>
       <c r="T342" s="6"/>
     </row>
     <row r="343" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B343" s="5"/>
-      <c r="C343" s="16"/>
-      <c r="D343" s="16"/>
-      <c r="E343" s="16"/>
-      <c r="F343" s="16"/>
-      <c r="G343" s="16"/>
-      <c r="H343" s="16"/>
-      <c r="I343" s="16"/>
-      <c r="J343" s="16"/>
-      <c r="K343" s="16"/>
-      <c r="L343" s="16"/>
-      <c r="M343" s="16"/>
-      <c r="N343" s="16"/>
-      <c r="O343" s="16"/>
-      <c r="P343" s="16"/>
-      <c r="Q343" s="16"/>
-      <c r="R343" s="16"/>
-      <c r="S343" s="16"/>
       <c r="T343" s="6"/>
     </row>
     <row r="344" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B344" s="5"/>
-      <c r="C344" s="16"/>
-      <c r="D344" s="16"/>
-      <c r="E344" s="16"/>
-      <c r="F344" s="16"/>
-      <c r="G344" s="16"/>
-      <c r="H344" s="16"/>
-      <c r="I344" s="16"/>
-      <c r="J344" s="16"/>
-      <c r="K344" s="16"/>
-      <c r="L344" s="16"/>
-      <c r="M344" s="16"/>
-      <c r="N344" s="16"/>
-      <c r="O344" s="16"/>
-      <c r="P344" s="16"/>
-      <c r="Q344" s="16"/>
-      <c r="R344" s="16"/>
-      <c r="S344" s="16"/>
       <c r="T344" s="6"/>
     </row>
     <row r="345" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B345" s="5"/>
-      <c r="C345" s="16"/>
-      <c r="D345" s="16"/>
-      <c r="E345" s="16"/>
-      <c r="F345" s="16"/>
-      <c r="G345" s="16"/>
-      <c r="H345" s="16"/>
-      <c r="I345" s="16"/>
-      <c r="J345" s="16"/>
-      <c r="K345" s="16"/>
-      <c r="L345" s="16"/>
-      <c r="M345" s="16"/>
-      <c r="N345" s="16"/>
-      <c r="O345" s="16"/>
-      <c r="P345" s="16"/>
-      <c r="Q345" s="16"/>
-      <c r="R345" s="16"/>
-      <c r="S345" s="16"/>
       <c r="T345" s="6"/>
     </row>
     <row r="346" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B346" s="5"/>
-      <c r="C346" s="16"/>
-      <c r="D346" s="16"/>
-      <c r="E346" s="16"/>
-      <c r="F346" s="16"/>
-      <c r="G346" s="16"/>
-      <c r="H346" s="16"/>
-      <c r="I346" s="16"/>
-      <c r="J346" s="16"/>
-      <c r="K346" s="16"/>
-      <c r="L346" s="16"/>
-      <c r="M346" s="16"/>
-      <c r="N346" s="16"/>
-      <c r="O346" s="16"/>
-      <c r="P346" s="16"/>
-      <c r="Q346" s="16"/>
-      <c r="R346" s="16"/>
-      <c r="S346" s="16"/>
       <c r="T346" s="6"/>
     </row>
     <row r="347" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B347" s="5"/>
-      <c r="C347" s="16"/>
-      <c r="D347" s="16"/>
-      <c r="E347" s="16"/>
-      <c r="F347" s="16"/>
-      <c r="G347" s="16"/>
-      <c r="H347" s="16"/>
-      <c r="I347" s="16"/>
-      <c r="J347" s="16"/>
-      <c r="K347" s="16"/>
-      <c r="L347" s="16"/>
-      <c r="M347" s="16"/>
-      <c r="N347" s="16"/>
-      <c r="O347" s="16"/>
-      <c r="P347" s="16"/>
-      <c r="Q347" s="16"/>
-      <c r="R347" s="16"/>
-      <c r="S347" s="16"/>
       <c r="T347" s="6"/>
     </row>
     <row r="348" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B348" s="5"/>
-      <c r="C348" s="16"/>
-      <c r="D348" s="16"/>
-      <c r="E348" s="16"/>
-      <c r="F348" s="16"/>
-      <c r="G348" s="16"/>
-      <c r="H348" s="16"/>
-      <c r="I348" s="16"/>
-      <c r="J348" s="16"/>
-      <c r="K348" s="16"/>
-      <c r="L348" s="16"/>
-      <c r="M348" s="16"/>
-      <c r="N348" s="16"/>
-      <c r="O348" s="16"/>
-      <c r="P348" s="16"/>
-      <c r="Q348" s="16"/>
-      <c r="R348" s="16"/>
-      <c r="S348" s="16"/>
       <c r="T348" s="6"/>
     </row>
     <row r="349" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B349" s="5"/>
-      <c r="C349" s="16"/>
-      <c r="D349" s="16"/>
-      <c r="E349" s="16"/>
-      <c r="F349" s="16"/>
-      <c r="G349" s="16"/>
-      <c r="H349" s="16"/>
-      <c r="I349" s="16"/>
-      <c r="J349" s="16"/>
-      <c r="K349" s="16"/>
-      <c r="L349" s="16"/>
-      <c r="M349" s="16"/>
-      <c r="N349" s="16"/>
-      <c r="O349" s="16"/>
-      <c r="P349" s="16"/>
-      <c r="Q349" s="16"/>
-      <c r="R349" s="16"/>
-      <c r="S349" s="16"/>
       <c r="T349" s="6"/>
     </row>
     <row r="350" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B350" s="5"/>
-      <c r="C350" s="16"/>
-      <c r="D350" s="16"/>
-      <c r="E350" s="16"/>
-      <c r="F350" s="16"/>
-      <c r="G350" s="16"/>
-      <c r="H350" s="16"/>
-      <c r="I350" s="16"/>
-      <c r="J350" s="16"/>
-      <c r="K350" s="16"/>
-      <c r="L350" s="16"/>
-      <c r="M350" s="16"/>
-      <c r="N350" s="16"/>
-      <c r="O350" s="16"/>
-      <c r="P350" s="16"/>
-      <c r="Q350" s="16"/>
-      <c r="R350" s="16"/>
-      <c r="S350" s="16"/>
       <c r="T350" s="6"/>
     </row>
     <row r="351" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B351" s="5"/>
-      <c r="C351" s="16"/>
-      <c r="D351" s="16"/>
-      <c r="E351" s="16"/>
-      <c r="F351" s="16"/>
-      <c r="G351" s="16"/>
-      <c r="H351" s="16"/>
-      <c r="I351" s="16"/>
-      <c r="J351" s="16"/>
-      <c r="K351" s="16"/>
-      <c r="L351" s="16"/>
-      <c r="M351" s="16"/>
-      <c r="N351" s="16"/>
-      <c r="O351" s="16"/>
-      <c r="P351" s="16"/>
-      <c r="Q351" s="16"/>
-      <c r="R351" s="16"/>
-      <c r="S351" s="16"/>
       <c r="T351" s="6"/>
     </row>
     <row r="352" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B352" s="5"/>
-      <c r="C352" s="16"/>
-      <c r="D352" s="16"/>
-      <c r="E352" s="16"/>
-      <c r="F352" s="16"/>
-      <c r="G352" s="16"/>
-      <c r="H352" s="16"/>
-      <c r="I352" s="16"/>
-      <c r="J352" s="16"/>
-      <c r="K352" s="16"/>
-      <c r="L352" s="16"/>
-      <c r="M352" s="16"/>
-      <c r="N352" s="16"/>
-      <c r="O352" s="16"/>
-      <c r="P352" s="16"/>
-      <c r="Q352" s="16"/>
-      <c r="R352" s="16"/>
-      <c r="S352" s="16"/>
       <c r="T352" s="6"/>
     </row>
     <row r="353" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B353" s="5"/>
-      <c r="C353" s="16"/>
-      <c r="D353" s="16"/>
-      <c r="E353" s="16"/>
-      <c r="F353" s="16"/>
-      <c r="G353" s="16"/>
-      <c r="H353" s="16"/>
-      <c r="I353" s="16"/>
-      <c r="J353" s="16"/>
-      <c r="K353" s="16"/>
-      <c r="L353" s="16"/>
-      <c r="M353" s="16"/>
-      <c r="N353" s="16"/>
-      <c r="O353" s="16"/>
-      <c r="P353" s="16"/>
-      <c r="Q353" s="16"/>
-      <c r="R353" s="16"/>
-      <c r="S353" s="16"/>
       <c r="T353" s="6"/>
     </row>
     <row r="354" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B354" s="5"/>
-      <c r="C354" s="16"/>
-      <c r="D354" s="16"/>
-      <c r="E354" s="16"/>
-      <c r="F354" s="16"/>
-      <c r="G354" s="16"/>
-      <c r="H354" s="16"/>
-      <c r="I354" s="16"/>
-      <c r="J354" s="16"/>
-      <c r="K354" s="16"/>
-      <c r="L354" s="16"/>
-      <c r="M354" s="16"/>
-      <c r="N354" s="16"/>
-      <c r="O354" s="16"/>
-      <c r="P354" s="16"/>
-      <c r="Q354" s="16"/>
-      <c r="R354" s="16"/>
-      <c r="S354" s="16"/>
       <c r="T354" s="6"/>
     </row>
     <row r="355" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B355" s="5"/>
-      <c r="C355" s="16"/>
-      <c r="D355" s="16"/>
-      <c r="E355" s="16"/>
-      <c r="F355" s="16"/>
-      <c r="G355" s="16"/>
-      <c r="H355" s="16"/>
-      <c r="I355" s="16"/>
-      <c r="J355" s="16"/>
-      <c r="K355" s="16"/>
-      <c r="L355" s="16"/>
-      <c r="M355" s="16"/>
-      <c r="N355" s="16"/>
-      <c r="O355" s="16"/>
-      <c r="P355" s="16"/>
-      <c r="Q355" s="16"/>
-      <c r="R355" s="16"/>
-      <c r="S355" s="16"/>
       <c r="T355" s="6"/>
     </row>
     <row r="356" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B356" s="5"/>
-      <c r="C356" s="16"/>
-      <c r="D356" s="16"/>
-      <c r="E356" s="16"/>
-      <c r="F356" s="16"/>
-      <c r="G356" s="16"/>
-      <c r="H356" s="16"/>
-      <c r="I356" s="16"/>
-      <c r="J356" s="16"/>
-      <c r="K356" s="16"/>
-      <c r="L356" s="16"/>
-      <c r="M356" s="16"/>
-      <c r="N356" s="16"/>
-      <c r="O356" s="16"/>
-      <c r="P356" s="16"/>
-      <c r="Q356" s="16"/>
-      <c r="R356" s="16"/>
-      <c r="S356" s="16"/>
       <c r="T356" s="6"/>
     </row>
     <row r="357" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B357" s="5"/>
-      <c r="C357" s="16"/>
-      <c r="D357" s="16"/>
-      <c r="E357" s="16"/>
-      <c r="F357" s="16"/>
-      <c r="G357" s="16"/>
-      <c r="H357" s="16"/>
-      <c r="I357" s="16"/>
-      <c r="J357" s="16"/>
-      <c r="K357" s="16"/>
-      <c r="L357" s="16"/>
-      <c r="M357" s="16"/>
-      <c r="N357" s="16"/>
-      <c r="O357" s="16"/>
-      <c r="P357" s="16"/>
-      <c r="Q357" s="16"/>
-      <c r="R357" s="16"/>
-      <c r="S357" s="16"/>
       <c r="T357" s="6"/>
     </row>
     <row r="358" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B358" s="5"/>
-      <c r="C358" s="16"/>
-      <c r="D358" s="16"/>
-      <c r="E358" s="16"/>
-      <c r="F358" s="16"/>
-      <c r="G358" s="16"/>
-      <c r="H358" s="16"/>
-      <c r="I358" s="16"/>
-      <c r="J358" s="16"/>
-      <c r="K358" s="16"/>
-      <c r="L358" s="16"/>
-      <c r="M358" s="16"/>
-      <c r="N358" s="16"/>
-      <c r="O358" s="16"/>
-      <c r="P358" s="16"/>
-      <c r="Q358" s="16"/>
-      <c r="R358" s="16"/>
-      <c r="S358" s="16"/>
       <c r="T358" s="6"/>
     </row>
     <row r="359" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B359" s="5"/>
-      <c r="C359" s="16"/>
-      <c r="D359" s="16"/>
-      <c r="E359" s="16"/>
-      <c r="F359" s="16"/>
-      <c r="G359" s="16"/>
-      <c r="H359" s="16"/>
-      <c r="I359" s="16"/>
-      <c r="J359" s="16"/>
-      <c r="K359" s="16"/>
-      <c r="L359" s="16"/>
-      <c r="M359" s="16"/>
-      <c r="N359" s="16"/>
-      <c r="O359" s="16"/>
-      <c r="P359" s="16"/>
-      <c r="Q359" s="16"/>
-      <c r="R359" s="16"/>
-      <c r="S359" s="16"/>
       <c r="T359" s="6"/>
     </row>
     <row r="360" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B360" s="5"/>
-      <c r="C360" s="16"/>
-      <c r="D360" s="16"/>
-      <c r="E360" s="16"/>
-      <c r="F360" s="16"/>
-      <c r="G360" s="16"/>
-      <c r="H360" s="16"/>
-      <c r="I360" s="16"/>
-      <c r="J360" s="16"/>
-      <c r="K360" s="16"/>
-      <c r="L360" s="16"/>
-      <c r="M360" s="16"/>
-      <c r="N360" s="16"/>
-      <c r="O360" s="16"/>
-      <c r="P360" s="16"/>
-      <c r="Q360" s="16"/>
-      <c r="R360" s="16"/>
-      <c r="S360" s="16"/>
       <c r="T360" s="6"/>
     </row>
     <row r="361" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B361" s="5"/>
-      <c r="C361" s="16"/>
-      <c r="D361" s="16"/>
-      <c r="E361" s="16"/>
-      <c r="F361" s="16"/>
-      <c r="G361" s="16"/>
-      <c r="H361" s="16"/>
-      <c r="I361" s="16"/>
-      <c r="J361" s="16"/>
-      <c r="K361" s="16"/>
-      <c r="L361" s="16"/>
-      <c r="M361" s="16"/>
-      <c r="N361" s="16"/>
-      <c r="O361" s="16"/>
-      <c r="P361" s="16"/>
-      <c r="Q361" s="16"/>
-      <c r="R361" s="16"/>
-      <c r="S361" s="16"/>
       <c r="T361" s="6"/>
     </row>
     <row r="362" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B362" s="5"/>
-      <c r="C362" s="16"/>
-      <c r="D362" s="16"/>
-      <c r="E362" s="16"/>
-      <c r="F362" s="16"/>
-      <c r="G362" s="16"/>
-      <c r="H362" s="16"/>
-      <c r="I362" s="16"/>
-      <c r="J362" s="16"/>
-      <c r="K362" s="16"/>
-      <c r="L362" s="16"/>
-      <c r="M362" s="16"/>
-      <c r="N362" s="16"/>
-      <c r="O362" s="16"/>
-      <c r="P362" s="16"/>
-      <c r="Q362" s="16"/>
-      <c r="R362" s="16"/>
-      <c r="S362" s="16"/>
       <c r="T362" s="6"/>
     </row>
     <row r="363" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B363" s="5"/>
-      <c r="C363" s="16"/>
-      <c r="D363" s="16"/>
-      <c r="E363" s="16"/>
-      <c r="F363" s="16"/>
-      <c r="G363" s="16"/>
-      <c r="H363" s="16"/>
-      <c r="I363" s="16"/>
-      <c r="J363" s="16"/>
-      <c r="K363" s="16"/>
-      <c r="L363" s="16"/>
-      <c r="M363" s="16"/>
-      <c r="N363" s="16"/>
-      <c r="O363" s="16"/>
-      <c r="P363" s="16"/>
-      <c r="Q363" s="16"/>
-      <c r="R363" s="16"/>
-      <c r="S363" s="16"/>
       <c r="T363" s="6"/>
     </row>
     <row r="364" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B364" s="5"/>
-      <c r="C364" s="16"/>
-      <c r="D364" s="16"/>
-      <c r="E364" s="16"/>
-      <c r="F364" s="16"/>
-      <c r="G364" s="16"/>
-      <c r="H364" s="16"/>
-      <c r="I364" s="16"/>
-      <c r="J364" s="16"/>
-      <c r="K364" s="16"/>
-      <c r="L364" s="16"/>
-      <c r="M364" s="16"/>
-      <c r="N364" s="16"/>
-      <c r="O364" s="16"/>
-      <c r="P364" s="16"/>
-      <c r="Q364" s="16"/>
-      <c r="R364" s="16"/>
-      <c r="S364" s="16"/>
       <c r="T364" s="6"/>
     </row>
     <row r="365" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B365" s="5"/>
-      <c r="C365" s="16"/>
-      <c r="D365" s="16"/>
-      <c r="E365" s="16"/>
-      <c r="F365" s="16"/>
-      <c r="G365" s="16"/>
-      <c r="H365" s="16"/>
-      <c r="I365" s="16"/>
-      <c r="J365" s="16"/>
-      <c r="K365" s="16"/>
-      <c r="L365" s="16"/>
-      <c r="M365" s="16"/>
-      <c r="N365" s="16"/>
-      <c r="O365" s="16"/>
-      <c r="P365" s="16"/>
-      <c r="Q365" s="16"/>
-      <c r="R365" s="16"/>
-      <c r="S365" s="16"/>
       <c r="T365" s="6"/>
     </row>
     <row r="366" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B366" s="5"/>
-      <c r="C366" s="16"/>
-      <c r="D366" s="16"/>
-      <c r="E366" s="16"/>
-      <c r="F366" s="16"/>
-      <c r="G366" s="16"/>
-      <c r="H366" s="16"/>
-      <c r="I366" s="16"/>
-      <c r="J366" s="16"/>
-      <c r="K366" s="16"/>
-      <c r="L366" s="16"/>
-      <c r="M366" s="16"/>
-      <c r="N366" s="16"/>
-      <c r="O366" s="16"/>
-      <c r="P366" s="16"/>
-      <c r="Q366" s="16"/>
-      <c r="R366" s="16"/>
-      <c r="S366" s="16"/>
       <c r="T366" s="6"/>
     </row>
     <row r="367" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B367" s="5"/>
-      <c r="C367" s="16"/>
-      <c r="D367" s="16"/>
-      <c r="E367" s="16"/>
-      <c r="F367" s="16"/>
-      <c r="G367" s="16"/>
-      <c r="H367" s="16"/>
-      <c r="I367" s="16"/>
-      <c r="J367" s="16"/>
-      <c r="K367" s="16"/>
-      <c r="L367" s="16"/>
-      <c r="M367" s="16"/>
-      <c r="N367" s="16"/>
-      <c r="O367" s="16"/>
-      <c r="P367" s="16"/>
-      <c r="Q367" s="16"/>
-      <c r="R367" s="16"/>
-      <c r="S367" s="16"/>
       <c r="T367" s="6"/>
     </row>
     <row r="368" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B368" s="5"/>
-      <c r="C368" s="16"/>
-      <c r="D368" s="16"/>
-      <c r="E368" s="16"/>
-      <c r="F368" s="16"/>
-      <c r="G368" s="16"/>
-      <c r="H368" s="16"/>
-      <c r="I368" s="16"/>
-      <c r="J368" s="16"/>
-      <c r="K368" s="16"/>
-      <c r="L368" s="16"/>
-      <c r="M368" s="16"/>
-      <c r="N368" s="16"/>
-      <c r="O368" s="16"/>
-      <c r="P368" s="16"/>
-      <c r="Q368" s="16"/>
-      <c r="R368" s="16"/>
-      <c r="S368" s="16"/>
       <c r="T368" s="6"/>
     </row>
     <row r="369" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B369" s="5"/>
-      <c r="C369" s="16"/>
-      <c r="D369" s="16"/>
-      <c r="E369" s="16"/>
-      <c r="F369" s="16"/>
-      <c r="G369" s="16"/>
-      <c r="H369" s="16"/>
-      <c r="I369" s="16"/>
-      <c r="J369" s="16"/>
-      <c r="K369" s="16"/>
-      <c r="L369" s="16"/>
-      <c r="M369" s="16"/>
-      <c r="N369" s="16"/>
-      <c r="O369" s="16"/>
-      <c r="P369" s="16"/>
-      <c r="Q369" s="16"/>
-      <c r="R369" s="16"/>
-      <c r="S369" s="16"/>
       <c r="T369" s="6"/>
     </row>
     <row r="370" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B370" s="5"/>
-      <c r="C370" s="16"/>
-      <c r="D370" s="16"/>
-      <c r="E370" s="16"/>
-      <c r="F370" s="16"/>
-      <c r="G370" s="16"/>
-      <c r="H370" s="16"/>
-      <c r="I370" s="16"/>
-      <c r="J370" s="16"/>
-      <c r="K370" s="16"/>
-      <c r="L370" s="16"/>
-      <c r="M370" s="16"/>
-      <c r="N370" s="16"/>
-      <c r="O370" s="16"/>
-      <c r="P370" s="16"/>
-      <c r="Q370" s="16"/>
-      <c r="R370" s="16"/>
-      <c r="S370" s="16"/>
       <c r="T370" s="6"/>
     </row>
     <row r="371" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B371" s="5"/>
-      <c r="C371" s="16"/>
-      <c r="D371" s="16"/>
-      <c r="E371" s="16"/>
-      <c r="F371" s="16"/>
-      <c r="G371" s="16"/>
-      <c r="H371" s="16"/>
-      <c r="I371" s="16"/>
-      <c r="J371" s="16"/>
-      <c r="K371" s="16"/>
-      <c r="L371" s="16"/>
-      <c r="M371" s="16"/>
-      <c r="N371" s="16"/>
-      <c r="O371" s="16"/>
-      <c r="P371" s="16"/>
-      <c r="Q371" s="16"/>
-      <c r="R371" s="16"/>
-      <c r="S371" s="16"/>
       <c r="T371" s="6"/>
     </row>
     <row r="372" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B372" s="5"/>
-      <c r="C372" s="16"/>
-      <c r="D372" s="16"/>
-      <c r="E372" s="16"/>
-      <c r="F372" s="16"/>
-      <c r="G372" s="16"/>
-      <c r="H372" s="16"/>
-      <c r="I372" s="16"/>
-      <c r="J372" s="16"/>
-      <c r="K372" s="16"/>
-      <c r="L372" s="16"/>
-      <c r="M372" s="16"/>
-      <c r="N372" s="16"/>
-      <c r="O372" s="16"/>
-      <c r="P372" s="16"/>
-      <c r="Q372" s="16"/>
-      <c r="R372" s="16"/>
-      <c r="S372" s="16"/>
       <c r="T372" s="6"/>
     </row>
     <row r="373" spans="2:20" x14ac:dyDescent="0.25">
@@ -15595,8 +15200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0EA440-FB41-4A25-888F-10879DE1E42C}">
   <dimension ref="A4:N302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A363" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K379" sqref="K379"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16999,330 +16604,138 @@
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B234" s="5"/>
-      <c r="C234" s="16"/>
-      <c r="D234" s="16"/>
-      <c r="E234" s="16"/>
-      <c r="F234" s="16"/>
-      <c r="G234" s="16"/>
-      <c r="H234" s="16"/>
-      <c r="I234" s="16"/>
-      <c r="J234" s="16"/>
       <c r="K234" s="6"/>
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B235" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C235" s="16"/>
-      <c r="D235" s="16"/>
-      <c r="E235" s="16"/>
-      <c r="F235" s="16"/>
-      <c r="G235" s="16"/>
-      <c r="H235" s="16"/>
-      <c r="I235" s="16"/>
-      <c r="J235" s="16"/>
       <c r="K235" s="6"/>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B236" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="C236" s="16"/>
-      <c r="D236" s="16"/>
-      <c r="E236" s="16"/>
-      <c r="F236" s="16"/>
-      <c r="G236" s="16"/>
-      <c r="H236" s="16"/>
-      <c r="I236" s="16"/>
-      <c r="J236" s="16"/>
       <c r="K236" s="6"/>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B237" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="C237" s="16"/>
-      <c r="D237" s="16"/>
-      <c r="E237" s="16"/>
-      <c r="F237" s="16"/>
-      <c r="G237" s="16"/>
-      <c r="H237" s="16"/>
-      <c r="I237" s="16"/>
-      <c r="J237" s="16"/>
       <c r="K237" s="6"/>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B238" s="5"/>
-      <c r="C238" s="16"/>
-      <c r="D238" s="16"/>
-      <c r="E238" s="16"/>
-      <c r="F238" s="16"/>
-      <c r="G238" s="16"/>
-      <c r="H238" s="16"/>
-      <c r="I238" s="16"/>
-      <c r="J238" s="16"/>
       <c r="K238" s="6"/>
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B239" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="C239" s="16"/>
-      <c r="D239" s="16"/>
-      <c r="E239" s="16"/>
-      <c r="F239" s="16"/>
-      <c r="G239" s="16"/>
-      <c r="H239" s="16"/>
-      <c r="I239" s="16"/>
-      <c r="J239" s="16"/>
       <c r="K239" s="6"/>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B240" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="C240" s="16"/>
-      <c r="D240" s="16"/>
-      <c r="E240" s="16"/>
-      <c r="F240" s="16"/>
-      <c r="G240" s="16"/>
-      <c r="H240" s="16"/>
-      <c r="I240" s="16"/>
-      <c r="J240" s="16"/>
       <c r="K240" s="6"/>
     </row>
     <row r="241" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B241" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="C241" s="16"/>
-      <c r="D241" s="16"/>
-      <c r="E241" s="16"/>
-      <c r="F241" s="16"/>
-      <c r="G241" s="16"/>
-      <c r="H241" s="16"/>
-      <c r="I241" s="16"/>
-      <c r="J241" s="16"/>
       <c r="K241" s="6"/>
     </row>
     <row r="242" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B242" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="C242" s="16"/>
-      <c r="D242" s="16"/>
-      <c r="E242" s="16"/>
-      <c r="F242" s="16"/>
-      <c r="G242" s="16"/>
-      <c r="H242" s="16"/>
-      <c r="I242" s="16"/>
-      <c r="J242" s="16"/>
       <c r="K242" s="6"/>
     </row>
     <row r="243" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B243" s="5"/>
-      <c r="C243" s="16"/>
-      <c r="D243" s="16"/>
-      <c r="E243" s="16"/>
-      <c r="F243" s="16"/>
-      <c r="G243" s="16"/>
-      <c r="H243" s="16"/>
-      <c r="I243" s="16"/>
-      <c r="J243" s="16"/>
       <c r="K243" s="6"/>
     </row>
     <row r="244" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B244" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="C244" s="16"/>
-      <c r="D244" s="16"/>
-      <c r="E244" s="16"/>
-      <c r="F244" s="16"/>
-      <c r="G244" s="16"/>
-      <c r="H244" s="16"/>
-      <c r="I244" s="16"/>
-      <c r="J244" s="16"/>
       <c r="K244" s="6"/>
     </row>
     <row r="245" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B245" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="C245" s="16"/>
-      <c r="D245" s="16"/>
-      <c r="E245" s="16"/>
-      <c r="F245" s="16"/>
-      <c r="G245" s="16"/>
-      <c r="H245" s="16"/>
-      <c r="I245" s="16"/>
-      <c r="J245" s="16"/>
       <c r="K245" s="6"/>
     </row>
     <row r="246" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B246" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="C246" s="16"/>
-      <c r="D246" s="16"/>
-      <c r="E246" s="16"/>
-      <c r="F246" s="16"/>
-      <c r="G246" s="16"/>
-      <c r="H246" s="16"/>
-      <c r="I246" s="16"/>
-      <c r="J246" s="16"/>
       <c r="K246" s="6"/>
     </row>
     <row r="247" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B247" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="C247" s="16"/>
-      <c r="D247" s="16"/>
-      <c r="E247" s="16"/>
-      <c r="F247" s="16"/>
-      <c r="G247" s="16"/>
-      <c r="H247" s="16"/>
-      <c r="I247" s="16"/>
-      <c r="J247" s="16"/>
       <c r="K247" s="6"/>
     </row>
     <row r="248" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B248" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="C248" s="16"/>
-      <c r="D248" s="16"/>
-      <c r="E248" s="16"/>
-      <c r="F248" s="16"/>
-      <c r="G248" s="16"/>
-      <c r="H248" s="16"/>
-      <c r="I248" s="16"/>
-      <c r="J248" s="16"/>
       <c r="K248" s="6"/>
     </row>
     <row r="249" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B249" s="5"/>
-      <c r="C249" s="16"/>
-      <c r="D249" s="16"/>
-      <c r="E249" s="16"/>
-      <c r="F249" s="16"/>
-      <c r="G249" s="16"/>
-      <c r="H249" s="16"/>
-      <c r="I249" s="16"/>
-      <c r="J249" s="16"/>
       <c r="K249" s="6"/>
     </row>
     <row r="250" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B250" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="C250" s="16"/>
-      <c r="D250" s="16"/>
-      <c r="E250" s="16"/>
-      <c r="F250" s="16"/>
-      <c r="G250" s="16"/>
-      <c r="H250" s="16"/>
-      <c r="I250" s="16"/>
-      <c r="J250" s="16"/>
       <c r="K250" s="6"/>
     </row>
     <row r="251" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B251" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="C251" s="16"/>
-      <c r="D251" s="16"/>
-      <c r="E251" s="16"/>
-      <c r="F251" s="16"/>
-      <c r="G251" s="16"/>
-      <c r="H251" s="16"/>
-      <c r="I251" s="16"/>
-      <c r="J251" s="16"/>
       <c r="K251" s="6"/>
     </row>
     <row r="252" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B252" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="C252" s="16"/>
-      <c r="D252" s="16"/>
-      <c r="E252" s="16"/>
-      <c r="F252" s="16"/>
-      <c r="G252" s="16"/>
-      <c r="H252" s="16"/>
-      <c r="I252" s="16"/>
-      <c r="J252" s="16"/>
       <c r="K252" s="6"/>
     </row>
     <row r="253" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B253" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="C253" s="16"/>
-      <c r="D253" s="16"/>
-      <c r="E253" s="16"/>
-      <c r="F253" s="16"/>
-      <c r="G253" s="16"/>
-      <c r="H253" s="16"/>
-      <c r="I253" s="16"/>
-      <c r="J253" s="16"/>
       <c r="K253" s="6"/>
     </row>
     <row r="254" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B254" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="C254" s="16"/>
-      <c r="D254" s="16"/>
-      <c r="E254" s="16"/>
-      <c r="F254" s="16"/>
-      <c r="G254" s="16"/>
-      <c r="H254" s="16"/>
-      <c r="I254" s="16"/>
-      <c r="J254" s="16"/>
       <c r="K254" s="6"/>
     </row>
     <row r="255" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B255" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="C255" s="16"/>
-      <c r="D255" s="16"/>
-      <c r="E255" s="16"/>
-      <c r="F255" s="16"/>
-      <c r="G255" s="16"/>
-      <c r="H255" s="16"/>
-      <c r="I255" s="16"/>
-      <c r="J255" s="16"/>
       <c r="K255" s="6"/>
     </row>
     <row r="256" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B256" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="C256" s="16"/>
-      <c r="D256" s="16"/>
-      <c r="E256" s="16"/>
-      <c r="F256" s="16"/>
-      <c r="G256" s="16"/>
-      <c r="H256" s="16"/>
-      <c r="I256" s="16"/>
-      <c r="J256" s="16"/>
       <c r="K256" s="6"/>
     </row>
     <row r="257" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B257" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="C257" s="16"/>
-      <c r="D257" s="16"/>
-      <c r="E257" s="16"/>
-      <c r="F257" s="16"/>
-      <c r="G257" s="16"/>
-      <c r="H257" s="16"/>
-      <c r="I257" s="16"/>
-      <c r="J257" s="16"/>
       <c r="K257" s="6"/>
       <c r="L257" t="s">
         <v>181</v>
@@ -17335,272 +16748,112 @@
       <c r="B258" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="C258" s="16"/>
-      <c r="D258" s="16"/>
-      <c r="E258" s="16"/>
-      <c r="F258" s="16"/>
-      <c r="G258" s="16"/>
-      <c r="H258" s="16"/>
-      <c r="I258" s="16"/>
-      <c r="J258" s="16"/>
       <c r="K258" s="6"/>
     </row>
     <row r="259" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B259" s="5"/>
-      <c r="C259" s="16"/>
-      <c r="D259" s="16"/>
-      <c r="E259" s="16"/>
-      <c r="F259" s="16"/>
-      <c r="G259" s="16"/>
-      <c r="H259" s="16"/>
-      <c r="I259" s="16"/>
-      <c r="J259" s="16"/>
       <c r="K259" s="6"/>
     </row>
     <row r="260" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B260" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="C260" s="16"/>
-      <c r="D260" s="16"/>
-      <c r="E260" s="16"/>
-      <c r="F260" s="16"/>
-      <c r="G260" s="16"/>
-      <c r="H260" s="16"/>
-      <c r="I260" s="16"/>
-      <c r="J260" s="16"/>
       <c r="K260" s="6"/>
     </row>
     <row r="261" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B261" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="C261" s="16"/>
-      <c r="D261" s="16"/>
-      <c r="E261" s="16"/>
-      <c r="F261" s="16"/>
-      <c r="G261" s="16"/>
-      <c r="H261" s="16"/>
-      <c r="I261" s="16"/>
-      <c r="J261" s="16"/>
       <c r="K261" s="6"/>
     </row>
     <row r="262" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B262" s="5"/>
-      <c r="C262" s="16"/>
-      <c r="D262" s="16"/>
-      <c r="E262" s="16"/>
-      <c r="F262" s="16"/>
-      <c r="G262" s="16"/>
-      <c r="H262" s="16"/>
-      <c r="I262" s="16"/>
-      <c r="J262" s="16"/>
       <c r="K262" s="6"/>
     </row>
     <row r="263" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B263" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="C263" s="16"/>
-      <c r="D263" s="16"/>
-      <c r="E263" s="16"/>
-      <c r="F263" s="16"/>
-      <c r="G263" s="16"/>
-      <c r="H263" s="16"/>
-      <c r="I263" s="16"/>
-      <c r="J263" s="16"/>
       <c r="K263" s="6"/>
     </row>
     <row r="264" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B264" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="C264" s="16"/>
-      <c r="D264" s="16"/>
-      <c r="E264" s="16"/>
-      <c r="F264" s="16"/>
-      <c r="G264" s="16"/>
-      <c r="H264" s="16"/>
-      <c r="I264" s="16"/>
-      <c r="J264" s="16"/>
       <c r="K264" s="6"/>
     </row>
     <row r="265" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B265" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="C265" s="16"/>
-      <c r="D265" s="16"/>
-      <c r="E265" s="16"/>
-      <c r="F265" s="16"/>
-      <c r="G265" s="16"/>
-      <c r="H265" s="16"/>
-      <c r="I265" s="16"/>
-      <c r="J265" s="16"/>
       <c r="K265" s="6"/>
     </row>
     <row r="266" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B266" s="5"/>
-      <c r="C266" s="16"/>
-      <c r="D266" s="16"/>
-      <c r="E266" s="16"/>
-      <c r="F266" s="16"/>
-      <c r="G266" s="16"/>
-      <c r="H266" s="16"/>
-      <c r="I266" s="16"/>
-      <c r="J266" s="16"/>
       <c r="K266" s="6"/>
     </row>
     <row r="267" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B267" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="C267" s="16"/>
-      <c r="D267" s="16"/>
-      <c r="E267" s="16"/>
-      <c r="F267" s="16"/>
-      <c r="G267" s="16"/>
-      <c r="H267" s="16"/>
-      <c r="I267" s="16"/>
-      <c r="J267" s="16"/>
       <c r="K267" s="6"/>
     </row>
     <row r="268" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B268" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="C268" s="16"/>
-      <c r="D268" s="16"/>
-      <c r="E268" s="16"/>
-      <c r="F268" s="16"/>
-      <c r="G268" s="16"/>
-      <c r="H268" s="16"/>
-      <c r="I268" s="16"/>
-      <c r="J268" s="16"/>
       <c r="K268" s="6"/>
     </row>
     <row r="269" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B269" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="C269" s="16"/>
-      <c r="D269" s="16"/>
-      <c r="E269" s="16"/>
-      <c r="F269" s="16"/>
-      <c r="G269" s="16"/>
-      <c r="H269" s="16"/>
-      <c r="I269" s="16"/>
-      <c r="J269" s="16"/>
       <c r="K269" s="6"/>
     </row>
     <row r="270" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B270" s="5"/>
-      <c r="C270" s="16"/>
-      <c r="D270" s="16"/>
-      <c r="E270" s="16"/>
-      <c r="F270" s="16"/>
-      <c r="G270" s="16"/>
-      <c r="H270" s="16"/>
-      <c r="I270" s="16"/>
-      <c r="J270" s="16"/>
       <c r="K270" s="6"/>
     </row>
     <row r="271" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B271" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="C271" s="16"/>
-      <c r="D271" s="16"/>
-      <c r="E271" s="16"/>
-      <c r="F271" s="16"/>
-      <c r="G271" s="16"/>
-      <c r="H271" s="16"/>
-      <c r="I271" s="16"/>
-      <c r="J271" s="16"/>
       <c r="K271" s="6"/>
     </row>
     <row r="272" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B272" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="C272" s="16"/>
-      <c r="D272" s="16"/>
-      <c r="E272" s="16"/>
-      <c r="F272" s="16"/>
-      <c r="G272" s="16"/>
-      <c r="H272" s="16"/>
-      <c r="I272" s="16"/>
-      <c r="J272" s="16"/>
       <c r="K272" s="6"/>
     </row>
     <row r="273" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B273" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="C273" s="16"/>
-      <c r="D273" s="16"/>
-      <c r="E273" s="16"/>
-      <c r="F273" s="16"/>
-      <c r="G273" s="16"/>
-      <c r="H273" s="16"/>
-      <c r="I273" s="16"/>
-      <c r="J273" s="16"/>
       <c r="K273" s="6"/>
     </row>
     <row r="274" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B274" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="C274" s="16"/>
-      <c r="D274" s="16"/>
-      <c r="E274" s="16"/>
-      <c r="F274" s="16"/>
-      <c r="G274" s="16"/>
-      <c r="H274" s="16"/>
-      <c r="I274" s="16"/>
-      <c r="J274" s="16"/>
       <c r="K274" s="6"/>
     </row>
     <row r="275" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B275" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="C275" s="16"/>
-      <c r="D275" s="16"/>
-      <c r="E275" s="16"/>
-      <c r="F275" s="16"/>
-      <c r="G275" s="16"/>
-      <c r="H275" s="16"/>
-      <c r="I275" s="16"/>
-      <c r="J275" s="16"/>
       <c r="K275" s="6"/>
     </row>
     <row r="276" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B276" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="C276" s="16"/>
-      <c r="D276" s="16"/>
-      <c r="E276" s="16"/>
-      <c r="F276" s="16"/>
-      <c r="G276" s="16"/>
-      <c r="H276" s="16"/>
-      <c r="I276" s="16"/>
-      <c r="J276" s="16"/>
       <c r="K276" s="6"/>
     </row>
     <row r="277" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B277" s="11" t="s">
         <v>414</v>
       </c>
-      <c r="C277" s="16"/>
-      <c r="D277" s="16"/>
-      <c r="E277" s="16"/>
-      <c r="F277" s="16"/>
-      <c r="G277" s="16"/>
-      <c r="H277" s="16"/>
-      <c r="I277" s="16"/>
-      <c r="J277" s="16"/>
       <c r="K277" s="6"/>
       <c r="L277" t="s">
         <v>181</v>
@@ -17613,288 +16866,120 @@
       <c r="B278" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="C278" s="16"/>
-      <c r="D278" s="16"/>
-      <c r="E278" s="16"/>
-      <c r="F278" s="16"/>
-      <c r="G278" s="16"/>
-      <c r="H278" s="16"/>
-      <c r="I278" s="16"/>
-      <c r="J278" s="16"/>
       <c r="K278" s="6"/>
     </row>
     <row r="279" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B279" s="5"/>
-      <c r="C279" s="16"/>
-      <c r="D279" s="16"/>
-      <c r="E279" s="16"/>
-      <c r="F279" s="16"/>
-      <c r="G279" s="16"/>
-      <c r="H279" s="16"/>
-      <c r="I279" s="16"/>
-      <c r="J279" s="16"/>
       <c r="K279" s="6"/>
     </row>
     <row r="280" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B280" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="C280" s="16"/>
-      <c r="D280" s="16"/>
-      <c r="E280" s="16"/>
-      <c r="F280" s="16"/>
-      <c r="G280" s="16"/>
-      <c r="H280" s="16"/>
-      <c r="I280" s="16"/>
-      <c r="J280" s="16"/>
       <c r="K280" s="6"/>
     </row>
     <row r="281" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B281" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="C281" s="16"/>
-      <c r="D281" s="16"/>
-      <c r="E281" s="16"/>
-      <c r="F281" s="16"/>
-      <c r="G281" s="16"/>
-      <c r="H281" s="16"/>
-      <c r="I281" s="16"/>
-      <c r="J281" s="16"/>
       <c r="K281" s="6"/>
     </row>
     <row r="282" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B282" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="C282" s="16"/>
-      <c r="D282" s="16"/>
-      <c r="E282" s="16"/>
-      <c r="F282" s="16"/>
-      <c r="G282" s="16"/>
-      <c r="H282" s="16"/>
-      <c r="I282" s="16"/>
-      <c r="J282" s="16"/>
       <c r="K282" s="6"/>
     </row>
     <row r="283" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B283" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="C283" s="16"/>
-      <c r="D283" s="16"/>
-      <c r="E283" s="16"/>
-      <c r="F283" s="16"/>
-      <c r="G283" s="16"/>
-      <c r="H283" s="16"/>
-      <c r="I283" s="16"/>
-      <c r="J283" s="16"/>
       <c r="K283" s="6"/>
     </row>
     <row r="284" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B284" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="C284" s="16"/>
-      <c r="D284" s="16"/>
-      <c r="E284" s="16"/>
-      <c r="F284" s="16"/>
-      <c r="G284" s="16"/>
-      <c r="H284" s="16"/>
-      <c r="I284" s="16"/>
-      <c r="J284" s="16"/>
       <c r="K284" s="6"/>
     </row>
     <row r="285" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B285" s="5"/>
-      <c r="C285" s="16"/>
-      <c r="D285" s="16"/>
-      <c r="E285" s="16"/>
-      <c r="F285" s="16"/>
-      <c r="G285" s="16"/>
-      <c r="H285" s="16"/>
-      <c r="I285" s="16"/>
-      <c r="J285" s="16"/>
       <c r="K285" s="6"/>
     </row>
     <row r="286" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B286" s="11" t="s">
         <v>415</v>
       </c>
-      <c r="C286" s="16"/>
-      <c r="D286" s="16"/>
-      <c r="E286" s="16"/>
-      <c r="F286" s="16"/>
-      <c r="G286" s="16"/>
-      <c r="H286" s="16"/>
-      <c r="I286" s="16"/>
-      <c r="J286" s="16"/>
       <c r="K286" s="6"/>
     </row>
     <row r="287" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B287" s="11" t="s">
         <v>416</v>
       </c>
-      <c r="C287" s="16"/>
-      <c r="D287" s="16"/>
-      <c r="E287" s="16"/>
-      <c r="F287" s="16"/>
-      <c r="G287" s="16"/>
-      <c r="H287" s="16"/>
-      <c r="I287" s="16"/>
-      <c r="J287" s="16"/>
       <c r="K287" s="6"/>
     </row>
     <row r="288" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B288" s="11" t="s">
         <v>417</v>
       </c>
-      <c r="C288" s="16"/>
-      <c r="D288" s="16"/>
-      <c r="E288" s="16"/>
-      <c r="F288" s="16"/>
-      <c r="G288" s="16"/>
-      <c r="H288" s="16"/>
-      <c r="I288" s="16"/>
-      <c r="J288" s="16"/>
       <c r="K288" s="6"/>
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B289" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="C289" s="16"/>
-      <c r="D289" s="16"/>
-      <c r="E289" s="16"/>
-      <c r="F289" s="16"/>
-      <c r="G289" s="16"/>
-      <c r="H289" s="16"/>
-      <c r="I289" s="16"/>
-      <c r="J289" s="16"/>
       <c r="K289" s="6"/>
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B290" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="C290" s="16"/>
-      <c r="D290" s="16"/>
-      <c r="E290" s="16"/>
-      <c r="F290" s="16"/>
-      <c r="G290" s="16"/>
-      <c r="H290" s="16"/>
-      <c r="I290" s="16"/>
-      <c r="J290" s="16"/>
       <c r="K290" s="6"/>
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B291" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="C291" s="16"/>
-      <c r="D291" s="16"/>
-      <c r="E291" s="16"/>
-      <c r="F291" s="16"/>
-      <c r="G291" s="16"/>
-      <c r="H291" s="16"/>
-      <c r="I291" s="16"/>
-      <c r="J291" s="16"/>
       <c r="K291" s="6"/>
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B292" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="C292" s="16"/>
-      <c r="D292" s="16"/>
-      <c r="E292" s="16"/>
-      <c r="F292" s="16"/>
-      <c r="G292" s="16"/>
-      <c r="H292" s="16"/>
-      <c r="I292" s="16"/>
-      <c r="J292" s="16"/>
       <c r="K292" s="6"/>
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B293" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="C293" s="16"/>
-      <c r="D293" s="16"/>
-      <c r="E293" s="16"/>
-      <c r="F293" s="16"/>
-      <c r="G293" s="16"/>
-      <c r="H293" s="16"/>
-      <c r="I293" s="16"/>
-      <c r="J293" s="16"/>
       <c r="K293" s="6"/>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B294" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="C294" s="16"/>
-      <c r="D294" s="16"/>
-      <c r="E294" s="16"/>
-      <c r="F294" s="16"/>
-      <c r="G294" s="16"/>
-      <c r="H294" s="16"/>
-      <c r="I294" s="16"/>
-      <c r="J294" s="16"/>
       <c r="K294" s="6"/>
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B295" s="5"/>
-      <c r="C295" s="16"/>
-      <c r="D295" s="16"/>
-      <c r="E295" s="16"/>
-      <c r="F295" s="16"/>
-      <c r="G295" s="16"/>
-      <c r="H295" s="16"/>
-      <c r="I295" s="16"/>
-      <c r="J295" s="16"/>
       <c r="K295" s="6"/>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B296" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="C296" s="16"/>
-      <c r="D296" s="16"/>
-      <c r="E296" s="16"/>
-      <c r="F296" s="16"/>
-      <c r="G296" s="16"/>
-      <c r="H296" s="16"/>
-      <c r="I296" s="16"/>
-      <c r="J296" s="16"/>
       <c r="K296" s="6"/>
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B297" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="C297" s="16"/>
-      <c r="D297" s="16"/>
-      <c r="E297" s="16"/>
-      <c r="F297" s="16"/>
-      <c r="G297" s="16"/>
-      <c r="H297" s="16"/>
-      <c r="I297" s="16"/>
-      <c r="J297" s="16"/>
       <c r="K297" s="6"/>
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B298" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="C298" s="16"/>
-      <c r="D298" s="16"/>
-      <c r="E298" s="16"/>
-      <c r="F298" s="16"/>
-      <c r="G298" s="16"/>
-      <c r="H298" s="16"/>
-      <c r="I298" s="16"/>
-      <c r="J298" s="16"/>
       <c r="K298" s="6"/>
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.25">
@@ -17921,4 +17006,1583 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3BEE62-B343-4535-92D2-143F8CAE2485}">
+  <dimension ref="A2:L431"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A335" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V349" sqref="V349"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="4"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="L38" s="6"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="L39" s="6"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="L40" s="6"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="L41" s="6"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" s="6"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="L43" s="6"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="G44" t="s">
+        <v>8</v>
+      </c>
+      <c r="L44" s="6"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="G45" t="s">
+        <v>9</v>
+      </c>
+      <c r="L45" s="6"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="G46" t="s">
+        <v>10</v>
+      </c>
+      <c r="L46" s="6"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+      <c r="G47" t="s">
+        <v>11</v>
+      </c>
+      <c r="L47" s="6"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="G48" t="s">
+        <v>12</v>
+      </c>
+      <c r="L48" s="6"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+      <c r="G49" t="s">
+        <v>13</v>
+      </c>
+      <c r="L49" s="6"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
+      <c r="G50" t="s">
+        <v>14</v>
+      </c>
+      <c r="L50" s="6"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="G51" t="s">
+        <v>15</v>
+      </c>
+      <c r="L51" s="6"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="5"/>
+      <c r="G52" t="s">
+        <v>16</v>
+      </c>
+      <c r="L52" s="6"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="5"/>
+      <c r="G53" t="s">
+        <v>17</v>
+      </c>
+      <c r="L53" s="6"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="5"/>
+      <c r="F54" t="s">
+        <v>18</v>
+      </c>
+      <c r="L54" s="6"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" s="5"/>
+      <c r="G55" t="s">
+        <v>19</v>
+      </c>
+      <c r="L55" s="6"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="5"/>
+      <c r="H56" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56" s="6"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" s="5"/>
+      <c r="H57" t="s">
+        <v>21</v>
+      </c>
+      <c r="L57" s="6"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" s="5"/>
+      <c r="G58" t="s">
+        <v>22</v>
+      </c>
+      <c r="L58" s="6"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B59" s="5"/>
+      <c r="H59" t="s">
+        <v>23</v>
+      </c>
+      <c r="L59" s="6"/>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B60" s="5"/>
+      <c r="H60" t="s">
+        <v>24</v>
+      </c>
+      <c r="L60" s="6"/>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B61" s="5"/>
+      <c r="G61" t="s">
+        <v>25</v>
+      </c>
+      <c r="L61" s="6"/>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B62" s="5"/>
+      <c r="H62" t="s">
+        <v>26</v>
+      </c>
+      <c r="L62" s="6"/>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B63" s="5"/>
+      <c r="H63" t="s">
+        <v>27</v>
+      </c>
+      <c r="L63" s="6"/>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B64" s="5"/>
+      <c r="H64" t="s">
+        <v>28</v>
+      </c>
+      <c r="L64" s="6"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="5"/>
+      <c r="F65" t="s">
+        <v>29</v>
+      </c>
+      <c r="L65" s="6"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="5"/>
+      <c r="G66" t="s">
+        <v>30</v>
+      </c>
+      <c r="L66" s="6"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B67" s="5"/>
+      <c r="H67" t="s">
+        <v>31</v>
+      </c>
+      <c r="L67" s="6"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B68" s="5"/>
+      <c r="H68" t="s">
+        <v>32</v>
+      </c>
+      <c r="L68" s="6"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="5"/>
+      <c r="H69" t="s">
+        <v>33</v>
+      </c>
+      <c r="L69" s="6"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B70" s="5"/>
+      <c r="H70" t="s">
+        <v>34</v>
+      </c>
+      <c r="L70" s="6"/>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="5"/>
+      <c r="G71" t="s">
+        <v>35</v>
+      </c>
+      <c r="L71" s="6"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="H72" t="s">
+        <v>36</v>
+      </c>
+      <c r="L72" s="6"/>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B73" s="5"/>
+      <c r="H73" t="s">
+        <v>37</v>
+      </c>
+      <c r="L73" s="6"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B74" s="5"/>
+      <c r="H74" t="s">
+        <v>38</v>
+      </c>
+      <c r="L74" s="6"/>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B75" s="5"/>
+      <c r="G75" t="s">
+        <v>39</v>
+      </c>
+      <c r="L75" s="6"/>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B76" s="5"/>
+      <c r="H76" t="s">
+        <v>40</v>
+      </c>
+      <c r="L76" s="6"/>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B77" s="5"/>
+      <c r="H77" t="s">
+        <v>41</v>
+      </c>
+      <c r="L77" s="6"/>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B78" s="5"/>
+      <c r="H78" t="s">
+        <v>42</v>
+      </c>
+      <c r="L78" s="6"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="5"/>
+      <c r="G79" t="s">
+        <v>43</v>
+      </c>
+      <c r="L79" s="6"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="5"/>
+      <c r="H80" t="s">
+        <v>44</v>
+      </c>
+      <c r="L80" s="6"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81" s="5"/>
+      <c r="H81" t="s">
+        <v>45</v>
+      </c>
+      <c r="L81" s="6"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82" s="5"/>
+      <c r="H82" t="s">
+        <v>46</v>
+      </c>
+      <c r="L82" s="6"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="G83" t="s">
+        <v>47</v>
+      </c>
+      <c r="L83" s="6"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" s="5"/>
+      <c r="H84" t="s">
+        <v>48</v>
+      </c>
+      <c r="L84" s="6"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" s="5"/>
+      <c r="H85" t="s">
+        <v>49</v>
+      </c>
+      <c r="L85" s="6"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" s="5"/>
+      <c r="G86" t="s">
+        <v>50</v>
+      </c>
+      <c r="L86" s="6"/>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B87" s="5"/>
+      <c r="H87" t="s">
+        <v>51</v>
+      </c>
+      <c r="L87" s="6"/>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B88" s="5"/>
+      <c r="H88" t="s">
+        <v>52</v>
+      </c>
+      <c r="L88" s="6"/>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B89" s="5"/>
+      <c r="G89" t="s">
+        <v>53</v>
+      </c>
+      <c r="L89" s="6"/>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B90" s="5"/>
+      <c r="H90" t="s">
+        <v>54</v>
+      </c>
+      <c r="L90" s="6"/>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B91" s="5"/>
+      <c r="G91" t="s">
+        <v>55</v>
+      </c>
+      <c r="L91" s="6"/>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B92" s="5"/>
+      <c r="H92" t="s">
+        <v>56</v>
+      </c>
+      <c r="L92" s="6"/>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B93" s="5"/>
+      <c r="H93" t="s">
+        <v>57</v>
+      </c>
+      <c r="L93" s="6"/>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B94" s="5"/>
+      <c r="H94" t="s">
+        <v>58</v>
+      </c>
+      <c r="L94" s="6"/>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B95" s="5"/>
+      <c r="G95" t="s">
+        <v>59</v>
+      </c>
+      <c r="L95" s="6"/>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B96" s="5"/>
+      <c r="H96" t="s">
+        <v>60</v>
+      </c>
+      <c r="L96" s="6"/>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B97" s="5"/>
+      <c r="H97" t="s">
+        <v>61</v>
+      </c>
+      <c r="L97" s="6"/>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B98" s="5"/>
+      <c r="H98" t="s">
+        <v>62</v>
+      </c>
+      <c r="L98" s="6"/>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B99" s="5"/>
+      <c r="G99" t="s">
+        <v>63</v>
+      </c>
+      <c r="L99" s="6"/>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B100" s="5"/>
+      <c r="H100" t="s">
+        <v>64</v>
+      </c>
+      <c r="L100" s="6"/>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B101" s="5"/>
+      <c r="H101" t="s">
+        <v>65</v>
+      </c>
+      <c r="L101" s="6"/>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B102" s="5"/>
+      <c r="H102" t="s">
+        <v>66</v>
+      </c>
+      <c r="L102" s="6"/>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B103" s="5"/>
+      <c r="G103" t="s">
+        <v>67</v>
+      </c>
+      <c r="L103" s="6"/>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B104" s="5"/>
+      <c r="H104" t="s">
+        <v>68</v>
+      </c>
+      <c r="L104" s="6"/>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B105" s="5"/>
+      <c r="H105" t="s">
+        <v>69</v>
+      </c>
+      <c r="L105" s="6"/>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B106" s="5"/>
+      <c r="G106" t="s">
+        <v>70</v>
+      </c>
+      <c r="L106" s="6"/>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B107" s="5"/>
+      <c r="H107" t="s">
+        <v>71</v>
+      </c>
+      <c r="L107" s="6"/>
+    </row>
+    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B108" s="5"/>
+      <c r="H108" t="s">
+        <v>72</v>
+      </c>
+      <c r="L108" s="6"/>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B109" s="5"/>
+      <c r="G109" t="s">
+        <v>73</v>
+      </c>
+      <c r="L109" s="6"/>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B110" s="5"/>
+      <c r="H110" t="s">
+        <v>74</v>
+      </c>
+      <c r="L110" s="6"/>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B111" s="5"/>
+      <c r="H111" t="s">
+        <v>75</v>
+      </c>
+      <c r="L111" s="6"/>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B112" s="5"/>
+      <c r="H112" t="s">
+        <v>76</v>
+      </c>
+      <c r="L112" s="6"/>
+    </row>
+    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B113" s="5"/>
+      <c r="G113" t="s">
+        <v>77</v>
+      </c>
+      <c r="L113" s="6"/>
+    </row>
+    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B114" s="5"/>
+      <c r="H114" t="s">
+        <v>78</v>
+      </c>
+      <c r="L114" s="6"/>
+    </row>
+    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B115" s="5"/>
+      <c r="H115" t="s">
+        <v>79</v>
+      </c>
+      <c r="L115" s="6"/>
+    </row>
+    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B116" s="5"/>
+      <c r="H116" t="s">
+        <v>80</v>
+      </c>
+      <c r="L116" s="6"/>
+    </row>
+    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B117" s="5"/>
+      <c r="G117" t="s">
+        <v>81</v>
+      </c>
+      <c r="L117" s="6"/>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B118" s="5"/>
+      <c r="H118" t="s">
+        <v>82</v>
+      </c>
+      <c r="L118" s="6"/>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B119" s="5"/>
+      <c r="H119" t="s">
+        <v>83</v>
+      </c>
+      <c r="L119" s="6"/>
+    </row>
+    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B120" s="5"/>
+      <c r="H120" t="s">
+        <v>84</v>
+      </c>
+      <c r="L120" s="6"/>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B121" s="5"/>
+      <c r="G121" t="s">
+        <v>85</v>
+      </c>
+      <c r="L121" s="6"/>
+    </row>
+    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B122" s="5"/>
+      <c r="H122" t="s">
+        <v>86</v>
+      </c>
+      <c r="L122" s="6"/>
+    </row>
+    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B123" s="5"/>
+      <c r="H123" t="s">
+        <v>87</v>
+      </c>
+      <c r="L123" s="6"/>
+    </row>
+    <row r="124" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B124" s="5"/>
+      <c r="G124" t="s">
+        <v>88</v>
+      </c>
+      <c r="L124" s="6"/>
+    </row>
+    <row r="125" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B125" s="5"/>
+      <c r="H125" t="s">
+        <v>89</v>
+      </c>
+      <c r="L125" s="6"/>
+    </row>
+    <row r="126" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B126" s="5"/>
+      <c r="H126" t="s">
+        <v>90</v>
+      </c>
+      <c r="L126" s="6"/>
+    </row>
+    <row r="127" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B127" s="5"/>
+      <c r="H127" t="s">
+        <v>91</v>
+      </c>
+      <c r="L127" s="6"/>
+    </row>
+    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B128" s="5"/>
+      <c r="G128" t="s">
+        <v>92</v>
+      </c>
+      <c r="L128" s="6"/>
+    </row>
+    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B129" s="5"/>
+      <c r="H129" t="s">
+        <v>93</v>
+      </c>
+      <c r="L129" s="6"/>
+    </row>
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B130" s="5"/>
+      <c r="H130" t="s">
+        <v>94</v>
+      </c>
+      <c r="L130" s="6"/>
+    </row>
+    <row r="131" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B131" s="5"/>
+      <c r="H131" t="s">
+        <v>95</v>
+      </c>
+      <c r="L131" s="6"/>
+    </row>
+    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B132" s="5"/>
+      <c r="G132" t="s">
+        <v>96</v>
+      </c>
+      <c r="L132" s="6"/>
+    </row>
+    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B133" s="5"/>
+      <c r="H133" t="s">
+        <v>97</v>
+      </c>
+      <c r="L133" s="6"/>
+    </row>
+    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B134" s="5"/>
+      <c r="H134" t="s">
+        <v>98</v>
+      </c>
+      <c r="L134" s="6"/>
+    </row>
+    <row r="135" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B135" s="5"/>
+      <c r="H135" t="s">
+        <v>99</v>
+      </c>
+      <c r="L135" s="6"/>
+    </row>
+    <row r="136" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B136" s="5"/>
+      <c r="H136" t="s">
+        <v>100</v>
+      </c>
+      <c r="L136" s="6"/>
+    </row>
+    <row r="137" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B137" s="5"/>
+      <c r="G137" t="s">
+        <v>101</v>
+      </c>
+      <c r="L137" s="6"/>
+    </row>
+    <row r="138" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B138" s="5"/>
+      <c r="H138" t="s">
+        <v>102</v>
+      </c>
+      <c r="L138" s="6"/>
+    </row>
+    <row r="139" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B139" s="5"/>
+      <c r="H139" t="s">
+        <v>103</v>
+      </c>
+      <c r="L139" s="6"/>
+    </row>
+    <row r="140" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B140" s="5"/>
+      <c r="H140" t="s">
+        <v>104</v>
+      </c>
+      <c r="L140" s="6"/>
+    </row>
+    <row r="141" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B141" s="5"/>
+      <c r="G141" t="s">
+        <v>105</v>
+      </c>
+      <c r="L141" s="6"/>
+    </row>
+    <row r="142" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B142" s="5"/>
+      <c r="H142" t="s">
+        <v>106</v>
+      </c>
+      <c r="L142" s="6"/>
+    </row>
+    <row r="143" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B143" s="5"/>
+      <c r="H143" t="s">
+        <v>107</v>
+      </c>
+      <c r="L143" s="6"/>
+    </row>
+    <row r="144" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B144" s="5"/>
+      <c r="H144" t="s">
+        <v>108</v>
+      </c>
+      <c r="L144" s="6"/>
+    </row>
+    <row r="145" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B145" s="5"/>
+      <c r="G145" t="s">
+        <v>109</v>
+      </c>
+      <c r="L145" s="6"/>
+    </row>
+    <row r="146" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B146" s="5"/>
+      <c r="H146" t="s">
+        <v>110</v>
+      </c>
+      <c r="L146" s="6"/>
+    </row>
+    <row r="147" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B147" s="5"/>
+      <c r="I147" t="s">
+        <v>111</v>
+      </c>
+      <c r="L147" s="6"/>
+    </row>
+    <row r="148" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B148" s="5"/>
+      <c r="H148" t="s">
+        <v>112</v>
+      </c>
+      <c r="L148" s="6"/>
+    </row>
+    <row r="149" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B149" s="5"/>
+      <c r="H149" t="s">
+        <v>113</v>
+      </c>
+      <c r="L149" s="6"/>
+    </row>
+    <row r="150" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B150" s="5"/>
+      <c r="G150" t="s">
+        <v>114</v>
+      </c>
+      <c r="L150" s="6"/>
+    </row>
+    <row r="151" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B151" s="5"/>
+      <c r="H151" t="s">
+        <v>115</v>
+      </c>
+      <c r="L151" s="6"/>
+    </row>
+    <row r="152" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B152" s="5"/>
+      <c r="H152" t="s">
+        <v>116</v>
+      </c>
+      <c r="L152" s="6"/>
+    </row>
+    <row r="153" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B153" s="5"/>
+      <c r="H153" t="s">
+        <v>117</v>
+      </c>
+      <c r="L153" s="6"/>
+    </row>
+    <row r="154" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B154" s="5"/>
+      <c r="H154" t="s">
+        <v>118</v>
+      </c>
+      <c r="L154" s="6"/>
+    </row>
+    <row r="155" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B155" s="5"/>
+      <c r="G155" t="s">
+        <v>119</v>
+      </c>
+      <c r="L155" s="6"/>
+    </row>
+    <row r="156" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B156" s="5"/>
+      <c r="H156" t="s">
+        <v>120</v>
+      </c>
+      <c r="L156" s="6"/>
+    </row>
+    <row r="157" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B157" s="5"/>
+      <c r="H157" t="s">
+        <v>121</v>
+      </c>
+      <c r="L157" s="6"/>
+    </row>
+    <row r="158" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B158" s="5"/>
+      <c r="H158" t="s">
+        <v>122</v>
+      </c>
+      <c r="L158" s="6"/>
+    </row>
+    <row r="159" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B159" s="5"/>
+      <c r="G159" t="s">
+        <v>123</v>
+      </c>
+      <c r="L159" s="6"/>
+    </row>
+    <row r="160" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B160" s="5"/>
+      <c r="H160" t="s">
+        <v>124</v>
+      </c>
+      <c r="L160" s="6"/>
+    </row>
+    <row r="161" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B161" s="5"/>
+      <c r="H161" t="s">
+        <v>125</v>
+      </c>
+      <c r="L161" s="6"/>
+    </row>
+    <row r="162" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B162" s="5"/>
+      <c r="H162" t="s">
+        <v>126</v>
+      </c>
+      <c r="L162" s="6"/>
+    </row>
+    <row r="163" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B163" s="5"/>
+      <c r="H163" t="s">
+        <v>127</v>
+      </c>
+      <c r="L163" s="6"/>
+    </row>
+    <row r="164" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B164" s="5"/>
+      <c r="G164" t="s">
+        <v>128</v>
+      </c>
+      <c r="L164" s="6"/>
+    </row>
+    <row r="165" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B165" s="5"/>
+      <c r="H165" t="s">
+        <v>129</v>
+      </c>
+      <c r="L165" s="6"/>
+    </row>
+    <row r="166" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B166" s="5"/>
+      <c r="H166" t="s">
+        <v>130</v>
+      </c>
+      <c r="L166" s="6"/>
+    </row>
+    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B167" s="5"/>
+      <c r="H167" t="s">
+        <v>131</v>
+      </c>
+      <c r="L167" s="6"/>
+    </row>
+    <row r="168" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B168" s="5"/>
+      <c r="H168" t="s">
+        <v>132</v>
+      </c>
+      <c r="L168" s="6"/>
+    </row>
+    <row r="169" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B169" s="5"/>
+      <c r="G169" t="s">
+        <v>133</v>
+      </c>
+      <c r="L169" s="6"/>
+    </row>
+    <row r="170" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B170" s="5"/>
+      <c r="H170" t="s">
+        <v>134</v>
+      </c>
+      <c r="L170" s="6"/>
+    </row>
+    <row r="171" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B171" s="5"/>
+      <c r="H171" t="s">
+        <v>135</v>
+      </c>
+      <c r="L171" s="6"/>
+    </row>
+    <row r="172" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B172" s="5"/>
+      <c r="G172" t="s">
+        <v>136</v>
+      </c>
+      <c r="L172" s="6"/>
+    </row>
+    <row r="173" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B173" s="5"/>
+      <c r="G173" t="s">
+        <v>137</v>
+      </c>
+      <c r="L173" s="6"/>
+    </row>
+    <row r="174" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B174" s="5"/>
+      <c r="H174" t="s">
+        <v>138</v>
+      </c>
+      <c r="L174" s="6"/>
+    </row>
+    <row r="175" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B175" s="5"/>
+      <c r="H175" t="s">
+        <v>139</v>
+      </c>
+      <c r="L175" s="6"/>
+    </row>
+    <row r="176" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B176" s="5"/>
+      <c r="G176" t="s">
+        <v>140</v>
+      </c>
+      <c r="L176" s="6"/>
+    </row>
+    <row r="177" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B177" s="5"/>
+      <c r="H177" t="s">
+        <v>141</v>
+      </c>
+      <c r="L177" s="6"/>
+    </row>
+    <row r="178" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B178" s="5"/>
+      <c r="H178" t="s">
+        <v>142</v>
+      </c>
+      <c r="L178" s="6"/>
+    </row>
+    <row r="179" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B179" s="5"/>
+      <c r="H179" t="s">
+        <v>143</v>
+      </c>
+      <c r="L179" s="6"/>
+    </row>
+    <row r="180" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B180" s="5"/>
+      <c r="G180" t="s">
+        <v>144</v>
+      </c>
+      <c r="L180" s="6"/>
+    </row>
+    <row r="181" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B181" s="5"/>
+      <c r="H181" t="s">
+        <v>145</v>
+      </c>
+      <c r="L181" s="6"/>
+    </row>
+    <row r="182" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B182" s="5"/>
+      <c r="H182" t="s">
+        <v>146</v>
+      </c>
+      <c r="L182" s="6"/>
+    </row>
+    <row r="183" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B183" s="5"/>
+      <c r="H183" t="s">
+        <v>147</v>
+      </c>
+      <c r="L183" s="6"/>
+    </row>
+    <row r="184" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B184" s="5"/>
+      <c r="G184" t="s">
+        <v>148</v>
+      </c>
+      <c r="L184" s="6"/>
+    </row>
+    <row r="185" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B185" s="5"/>
+      <c r="H185" t="s">
+        <v>149</v>
+      </c>
+      <c r="L185" s="6"/>
+    </row>
+    <row r="186" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B186" s="5"/>
+      <c r="H186" t="s">
+        <v>150</v>
+      </c>
+      <c r="L186" s="6"/>
+    </row>
+    <row r="187" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B187" s="5"/>
+      <c r="H187" t="s">
+        <v>151</v>
+      </c>
+      <c r="L187" s="6"/>
+    </row>
+    <row r="188" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B188" s="5"/>
+      <c r="H188" t="s">
+        <v>152</v>
+      </c>
+      <c r="L188" s="6"/>
+    </row>
+    <row r="189" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B189" s="5"/>
+      <c r="G189" t="s">
+        <v>230</v>
+      </c>
+      <c r="L189" s="6"/>
+    </row>
+    <row r="190" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B190" s="5"/>
+      <c r="H190" t="s">
+        <v>231</v>
+      </c>
+      <c r="L190" s="6"/>
+    </row>
+    <row r="191" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B191" s="5"/>
+      <c r="H191" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="L191" s="6"/>
+    </row>
+    <row r="192" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B192" s="5"/>
+      <c r="H192" t="s">
+        <v>233</v>
+      </c>
+      <c r="L192" s="6"/>
+    </row>
+    <row r="193" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B193" s="5"/>
+      <c r="F193" t="s">
+        <v>153</v>
+      </c>
+      <c r="L193" s="6"/>
+    </row>
+    <row r="194" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B194" s="5"/>
+      <c r="G194" t="s">
+        <v>154</v>
+      </c>
+      <c r="L194" s="6"/>
+    </row>
+    <row r="195" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B195" s="5"/>
+      <c r="F195" t="s">
+        <v>155</v>
+      </c>
+      <c r="L195" s="6"/>
+    </row>
+    <row r="196" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B196" s="5"/>
+      <c r="G196" t="s">
+        <v>156</v>
+      </c>
+      <c r="L196" s="6"/>
+    </row>
+    <row r="197" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B197" s="5"/>
+      <c r="G197" t="s">
+        <v>157</v>
+      </c>
+      <c r="L197" s="6"/>
+    </row>
+    <row r="198" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B198" s="5"/>
+      <c r="G198" t="s">
+        <v>158</v>
+      </c>
+      <c r="L198" s="6"/>
+    </row>
+    <row r="199" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B199" s="5"/>
+      <c r="F199" t="s">
+        <v>159</v>
+      </c>
+      <c r="L199" s="6"/>
+    </row>
+    <row r="200" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B200" s="5"/>
+      <c r="G200" t="s">
+        <v>160</v>
+      </c>
+      <c r="L200" s="6"/>
+    </row>
+    <row r="201" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B201" s="5"/>
+      <c r="H201" t="s">
+        <v>161</v>
+      </c>
+      <c r="L201" s="6"/>
+    </row>
+    <row r="202" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B202" s="5"/>
+      <c r="H202" t="s">
+        <v>162</v>
+      </c>
+      <c r="L202" s="6"/>
+    </row>
+    <row r="203" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B203" s="5"/>
+      <c r="H203" t="s">
+        <v>163</v>
+      </c>
+      <c r="L203" s="6"/>
+    </row>
+    <row r="204" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B204" s="5"/>
+      <c r="H204" t="s">
+        <v>164</v>
+      </c>
+      <c r="L204" s="6"/>
+    </row>
+    <row r="205" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B205" s="5"/>
+      <c r="G205" t="s">
+        <v>165</v>
+      </c>
+      <c r="L205" s="6"/>
+    </row>
+    <row r="206" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B206" s="5"/>
+      <c r="H206" t="s">
+        <v>166</v>
+      </c>
+      <c r="L206" s="6"/>
+    </row>
+    <row r="207" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B207" s="5"/>
+      <c r="H207" t="s">
+        <v>167</v>
+      </c>
+      <c r="L207" s="6"/>
+    </row>
+    <row r="208" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B208" s="5"/>
+      <c r="H208" t="s">
+        <v>168</v>
+      </c>
+      <c r="L208" s="6"/>
+    </row>
+    <row r="209" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B209" s="5"/>
+      <c r="H209" t="s">
+        <v>169</v>
+      </c>
+      <c r="L209" s="6"/>
+    </row>
+    <row r="210" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B210" s="5"/>
+      <c r="H210" t="s">
+        <v>170</v>
+      </c>
+      <c r="L210" s="6"/>
+    </row>
+    <row r="211" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B211" s="5"/>
+      <c r="H211" t="s">
+        <v>171</v>
+      </c>
+      <c r="L211" s="6"/>
+    </row>
+    <row r="212" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B212" s="5"/>
+      <c r="F212" t="s">
+        <v>172</v>
+      </c>
+      <c r="L212" s="6"/>
+    </row>
+    <row r="213" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B213" s="5"/>
+      <c r="G213" t="s">
+        <v>173</v>
+      </c>
+      <c r="L213" s="6"/>
+    </row>
+    <row r="214" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B214" s="5"/>
+      <c r="G214" t="s">
+        <v>174</v>
+      </c>
+      <c r="L214" s="6"/>
+    </row>
+    <row r="215" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B215" s="5"/>
+      <c r="G215" t="s">
+        <v>175</v>
+      </c>
+      <c r="L215" s="6"/>
+    </row>
+    <row r="216" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B216" s="5"/>
+      <c r="D216" t="s">
+        <v>176</v>
+      </c>
+      <c r="L216" s="6"/>
+    </row>
+    <row r="217" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B217" s="5"/>
+      <c r="C217" t="s">
+        <v>177</v>
+      </c>
+      <c r="L217" s="6"/>
+    </row>
+    <row r="218" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B218" s="5"/>
+      <c r="D218" t="s">
+        <v>207</v>
+      </c>
+      <c r="L218" s="6"/>
+    </row>
+    <row r="219" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B219" s="5"/>
+      <c r="E219" t="s">
+        <v>178</v>
+      </c>
+      <c r="L219" s="6"/>
+    </row>
+    <row r="220" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B220" s="5"/>
+      <c r="E220" t="s">
+        <v>179</v>
+      </c>
+      <c r="L220" s="6"/>
+    </row>
+    <row r="221" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B221" s="5"/>
+      <c r="D221" t="s">
+        <v>212</v>
+      </c>
+      <c r="L221" s="6"/>
+    </row>
+    <row r="222" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B222" s="5"/>
+      <c r="E222" t="s">
+        <v>178</v>
+      </c>
+      <c r="L222" s="6"/>
+    </row>
+    <row r="223" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B223" s="5"/>
+      <c r="E223" t="s">
+        <v>179</v>
+      </c>
+      <c r="L223" s="6"/>
+    </row>
+    <row r="224" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B224" s="5"/>
+      <c r="D224" t="s">
+        <v>312</v>
+      </c>
+      <c r="L224" s="6"/>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B225" s="5"/>
+      <c r="E225" t="s">
+        <v>313</v>
+      </c>
+      <c r="L225" s="6"/>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B226" s="5"/>
+      <c r="F226" t="s">
+        <v>314</v>
+      </c>
+      <c r="L226" s="6"/>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B227" s="8"/>
+      <c r="C227" s="9"/>
+      <c r="D227" s="9"/>
+      <c r="E227" s="9"/>
+      <c r="F227" s="9"/>
+      <c r="G227" s="9"/>
+      <c r="H227" s="9"/>
+      <c r="I227" s="9"/>
+      <c r="J227" s="9"/>
+      <c r="K227" s="9"/>
+      <c r="L227" s="10"/>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B231" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C231" s="3"/>
+      <c r="D231" s="3"/>
+      <c r="E231" s="3"/>
+      <c r="F231" s="3"/>
+      <c r="G231" s="3"/>
+      <c r="H231" s="3"/>
+      <c r="I231" s="3"/>
+      <c r="J231" s="4"/>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B232" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C232" s="16"/>
+      <c r="D232" s="16"/>
+      <c r="E232" s="16"/>
+      <c r="F232" s="16"/>
+      <c r="G232" s="16"/>
+      <c r="H232" s="16"/>
+      <c r="I232" s="16"/>
+      <c r="J232" s="6"/>
+    </row>
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B233" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C233" s="16"/>
+      <c r="D233" s="16"/>
+      <c r="E233" s="16"/>
+      <c r="F233" s="16"/>
+      <c r="G233" s="16"/>
+      <c r="H233" s="16"/>
+      <c r="I233" s="16"/>
+      <c r="J233" s="6"/>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B234" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="C234" s="16"/>
+      <c r="D234" s="16"/>
+      <c r="E234" s="16"/>
+      <c r="F234" s="16"/>
+      <c r="G234" s="16"/>
+      <c r="H234" s="16"/>
+      <c r="I234" s="16"/>
+      <c r="J234" s="6"/>
+    </row>
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B235" s="5"/>
+      <c r="C235" s="16"/>
+      <c r="D235" s="16"/>
+      <c r="E235" s="16"/>
+      <c r="F235" s="16"/>
+      <c r="G235" s="16"/>
+      <c r="H235" s="16"/>
+      <c r="I235" s="16"/>
+      <c r="J235" s="6"/>
+    </row>
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B236" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C236" s="16"/>
+      <c r="D236" s="16"/>
+      <c r="E236" s="16"/>
+      <c r="F236" s="16"/>
+      <c r="G236" s="16"/>
+      <c r="H236" s="16"/>
+      <c r="I236" s="16"/>
+      <c r="J236" s="6"/>
+    </row>
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B237" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C237" s="16"/>
+      <c r="D237" s="16"/>
+      <c r="E237" s="16"/>
+      <c r="F237" s="16"/>
+      <c r="G237" s="16"/>
+      <c r="H237" s="16"/>
+      <c r="I237" s="16"/>
+      <c r="J237" s="6"/>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B238" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C238" s="16"/>
+      <c r="D238" s="16"/>
+      <c r="E238" s="16"/>
+      <c r="F238" s="16"/>
+      <c r="G238" s="16"/>
+      <c r="H238" s="16"/>
+      <c r="I238" s="16"/>
+      <c r="J238" s="6"/>
+    </row>
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B239" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C239" s="16"/>
+      <c r="D239" s="16"/>
+      <c r="E239" s="16"/>
+      <c r="F239" s="16"/>
+      <c r="G239" s="16"/>
+      <c r="H239" s="16"/>
+      <c r="I239" s="16"/>
+      <c r="J239" s="6"/>
+    </row>
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B240" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C240" s="16"/>
+      <c r="D240" s="16"/>
+      <c r="E240" s="16"/>
+      <c r="F240" s="16"/>
+      <c r="G240" s="16"/>
+      <c r="H240" s="16"/>
+      <c r="I240" s="16"/>
+      <c r="J240" s="6"/>
+      <c r="K240" t="s">
+        <v>181</v>
+      </c>
+      <c r="L240" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B241" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C241" s="16"/>
+      <c r="D241" s="16"/>
+      <c r="E241" s="16"/>
+      <c r="F241" s="16"/>
+      <c r="G241" s="16"/>
+      <c r="H241" s="16"/>
+      <c r="I241" s="16"/>
+      <c r="J241" s="6"/>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B242" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C242" s="9"/>
+      <c r="D242" s="9"/>
+      <c r="E242" s="9"/>
+      <c r="F242" s="9"/>
+      <c r="G242" s="9"/>
+      <c r="H242" s="9"/>
+      <c r="I242" s="9"/>
+      <c r="J242" s="10"/>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B243" s="16"/>
+      <c r="C243" s="16"/>
+      <c r="D243" s="16"/>
+      <c r="E243" s="16"/>
+      <c r="F243" s="16"/>
+      <c r="G243" s="16"/>
+      <c r="H243" s="16"/>
+      <c r="I243" s="16"/>
+      <c r="J243" s="16"/>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="399" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B399" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>